<commit_message>
Attempt to fix the micron detection issue.
</commit_message>
<xml_diff>
--- a/processed/test_1/kmeans/process_results.xlsx
+++ b/processed/test_1/kmeans/process_results.xlsx
@@ -13,7 +13,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>test_image_1.tif</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>img_id</t>
+  </si>
+  <si>
+    <t>pixsize</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>aspect_ratio</t>
+  </si>
+  <si>
+    <t>num_pixels</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Rg</t>
+  </si>
+  <si>
+    <t>perimeter</t>
+  </si>
+  <si>
+    <t>circularity</t>
+  </si>
+  <si>
+    <t>zbar_opt</t>
+  </si>
+  <si>
+    <t>center_mass_1</t>
+  </si>
+  <si>
+    <t>center_mass_2</t>
+  </si>
+  <si>
+    <t>dp_pcm</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
   <si>
     <t>fname</t>
   </si>
@@ -204,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -215,15 +272,17 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,7 +296,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="true"/>
-    <col min="2" max="2" width="3.140625" customWidth="true"/>
+    <col min="2" max="2" width="2.85546875" customWidth="true"/>
     <col min="3" max="3" width="7.140625" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="11.7109375" customWidth="true"/>
@@ -248,7 +307,7 @@
     <col min="10" max="10" width="11.7109375" customWidth="true"/>
     <col min="11" max="11" width="11.7109375" customWidth="true"/>
     <col min="12" max="12" width="11.7109375" customWidth="true"/>
-    <col min="13" max="13" width="12.7109375" customWidth="true"/>
+    <col min="13" max="13" width="13.7109375" customWidth="true"/>
     <col min="14" max="14" width="13.7109375" customWidth="true"/>
     <col min="15" max="15" width="14.28515625" customWidth="true"/>
     <col min="16" max="16" width="14.28515625" customWidth="true"/>
@@ -258,63 +317,63 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
@@ -335,42 +394,42 @@
         <v>1.1914580265095729</v>
       </c>
       <c r="H2" s="0">
-        <v>162530</v>
+        <v>192210</v>
       </c>
       <c r="I2" s="0">
-        <v>368.34507665762828</v>
+        <v>400.56785152729407</v>
       </c>
       <c r="J2" s="0">
-        <v>106561.3270173253</v>
+        <v>126020.75103673227</v>
       </c>
       <c r="K2" s="0">
-        <v>217.1334195843194</v>
+        <v>213.80144697404555</v>
       </c>
       <c r="L2" s="0">
-        <v>4265.5870445344126</v>
+        <v>5335.2226720647768</v>
       </c>
       <c r="M2" s="0">
-        <v>0.073595602795398105</v>
+        <v>0.0556348379808402</v>
       </c>
       <c r="N2" s="0">
-        <v>0.078187073471100862</v>
+        <v>0.078128335136030333</v>
       </c>
       <c r="O2" s="0">
-        <v>302.80476219774812</v>
+        <v>334.58405389938088</v>
       </c>
       <c r="P2" s="0">
-        <v>558.04083553805447</v>
+        <v>549.73586702044634</v>
       </c>
       <c r="Q2" s="0">
-        <v>5.200751274483479</v>
+        <v>26.565763847707888</v>
       </c>
       <c r="R2" s="0">
-        <v>5.200751274483479</v>
+        <v>26.565763847707888</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B3" s="0">
         <v>2</v>
@@ -382,51 +441,51 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E3" s="0">
-        <v>294.73684210526318</v>
+        <v>295.54655870445345</v>
       </c>
       <c r="F3" s="0">
-        <v>225.10121457489879</v>
+        <v>225.91093117408906</v>
       </c>
       <c r="G3" s="0">
-        <v>1.3093525179856116</v>
+        <v>1.3082437275985663</v>
       </c>
       <c r="H3" s="0">
-        <v>48920</v>
+        <v>49529</v>
       </c>
       <c r="I3" s="0">
-        <v>202.08371908497389</v>
+        <v>203.33768814013857</v>
       </c>
       <c r="J3" s="0">
-        <v>32073.956301529281</v>
+        <v>32473.241652870885</v>
       </c>
       <c r="K3" s="0">
-        <v>82.139749162288041</v>
+        <v>82.321156136135841</v>
       </c>
       <c r="L3" s="0">
-        <v>1465.5870445344128</v>
+        <v>1429.9595141700404</v>
       </c>
       <c r="M3" s="0">
-        <v>0.187645935854965</v>
+        <v>0.19956667663600342</v>
       </c>
       <c r="N3" s="0">
-        <v>0.34815322263556142</v>
+        <v>0.34628551744154062</v>
       </c>
       <c r="O3" s="0">
-        <v>839.67567457072767</v>
+        <v>839.44668779906726</v>
       </c>
       <c r="P3" s="0">
-        <v>468.33977923139821</v>
+        <v>468.32403238506731</v>
       </c>
       <c r="Q3" s="0">
-        <v>32.340473668208794</v>
+        <v>30.050364680042847</v>
       </c>
       <c r="R3" s="0">
-        <v>32.340473668208794</v>
+        <v>30.050364680042847</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B4" s="0">
         <v>3</v>
@@ -438,46 +497,46 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E4" s="0">
-        <v>12.955465587044534</v>
+        <v>9.7165991902834001</v>
       </c>
       <c r="F4" s="0">
-        <v>9.7165991902834001</v>
+        <v>6.4777327935222671</v>
       </c>
       <c r="G4" s="0">
-        <v>1.3333333333333335</v>
+        <v>1.5</v>
       </c>
       <c r="H4" s="0">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="I4" s="0">
-        <v>10.536925809758296</v>
+        <v>9.5826239234059862</v>
       </c>
       <c r="J4" s="0">
-        <v>87.200249143568968</v>
+        <v>72.120506810470573</v>
       </c>
       <c r="K4" s="0">
-        <v>4.5072381968227511</v>
+        <v>3.5330940923602463</v>
       </c>
       <c r="L4" s="0">
-        <v>39.773173615747666</v>
+        <v>31.247639500791408</v>
       </c>
       <c r="M4" s="0">
-        <v>0.69270304680226957</v>
+        <v>0.92818426720588398</v>
       </c>
       <c r="N4" s="0">
-        <v>0.22046572047499041</v>
+        <v>0.18568439238296125</v>
       </c>
       <c r="O4" s="0">
-        <v>611.79699248120301</v>
+        <v>317.92727272727274</v>
       </c>
       <c r="P4" s="0">
-        <v>384.79699248120301</v>
+        <v>616.25454545454545</v>
       </c>
       <c r="Q4" s="0">
-        <v>3.5632085561497329</v>
+        <v>6.851449106449107</v>
       </c>
       <c r="R4" s="0">
-        <v>3.5632085561497329</v>
+        <v>6.851449106449107</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Fix and test scale detection on all 270 files.
</commit_message>
<xml_diff>
--- a/processed/test_1/kmeans/process_results.xlsx
+++ b/processed/test_1/kmeans/process_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="128">
   <si>
     <t>fname</t>
   </si>
@@ -190,6 +190,84 @@
   </si>
   <si>
     <t>test_image_1.tif</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>img_id</t>
+  </si>
+  <si>
+    <t>pixsize</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>aspect_ratio</t>
+  </si>
+  <si>
+    <t>num_pixels</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Rg</t>
+  </si>
+  <si>
+    <t>perimeter</t>
+  </si>
+  <si>
+    <t>circularity</t>
+  </si>
+  <si>
+    <t>zbar_opt</t>
+  </si>
+  <si>
+    <t>center_mass_1</t>
+  </si>
+  <si>
+    <t>center_mass_2</t>
+  </si>
+  <si>
+    <t>dp_pcm</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0014.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0015.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0019.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0021.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0022.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0023.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0024.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0025.tif</t>
   </si>
   <si>
     <t>id</t>
@@ -339,7 +417,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -352,17 +430,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,63 +477,63 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
@@ -474,42 +554,42 @@
         <v>1.0166666666666666</v>
       </c>
       <c r="H2" s="0">
-        <v>28007</v>
+        <v>28013</v>
       </c>
       <c r="I2" s="0">
-        <v>152.90489801230638</v>
+        <v>152.92127570819702</v>
       </c>
       <c r="J2" s="0">
-        <v>18362.536674916813</v>
+        <v>18366.470520742838</v>
       </c>
       <c r="K2" s="0">
-        <v>61.676040873312829</v>
+        <v>61.68864806593723</v>
       </c>
       <c r="L2" s="0">
-        <v>819.28217012908488</v>
+        <v>818.19163370818626</v>
       </c>
       <c r="M2" s="0">
-        <v>0.34377598351362154</v>
+        <v>0.34476685035677906</v>
       </c>
       <c r="N2" s="0">
-        <v>0.2343266050935226</v>
+        <v>0.23429733827134921</v>
       </c>
       <c r="O2" s="0">
-        <v>462.15292605420075</v>
+        <v>462.26448434655339</v>
       </c>
       <c r="P2" s="0">
-        <v>155.40047131074374</v>
+        <v>155.41894834541105</v>
       </c>
       <c r="Q2" s="0">
-        <v>30.829842435778723</v>
+        <v>29.332843439016941</v>
       </c>
       <c r="R2" s="0">
-        <v>30.829842435778723</v>
+        <v>29.332843439016941</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="B3" s="0">
         <v>2</v>
@@ -530,42 +610,42 @@
         <v>1.6968215158924207</v>
       </c>
       <c r="H3" s="0">
-        <v>110995</v>
+        <v>110943</v>
       </c>
       <c r="I3" s="0">
-        <v>304.39660860266963</v>
+        <v>304.32529693111678</v>
       </c>
       <c r="J3" s="0">
-        <v>72772.869576619836</v>
+        <v>72738.776246127614</v>
       </c>
       <c r="K3" s="0">
-        <v>145.99972949762159</v>
+        <v>146.00977607846761</v>
       </c>
       <c r="L3" s="0">
-        <v>2717.4089068825911</v>
+        <v>2722.2672064777325</v>
       </c>
       <c r="M3" s="0">
-        <v>0.12384240439807843</v>
+        <v>0.1233429556736088</v>
       </c>
       <c r="N3" s="0">
-        <v>0.25358622860896274</v>
+        <v>0.25374215872483774</v>
       </c>
       <c r="O3" s="0">
-        <v>435.66587684129917</v>
+        <v>435.71453809613945</v>
       </c>
       <c r="P3" s="0">
-        <v>548.45025451596916</v>
+        <v>548.45382764122121</v>
       </c>
       <c r="Q3" s="0">
-        <v>32.656870523272872</v>
+        <v>24.1943710687502</v>
       </c>
       <c r="R3" s="0">
-        <v>32.656870523272872</v>
+        <v>24.1943710687502</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="B4" s="0">
         <v>3</v>
@@ -586,42 +666,42 @@
         <v>1.3883928571428572</v>
       </c>
       <c r="H4" s="0">
-        <v>43877</v>
+        <v>43902</v>
       </c>
       <c r="I4" s="0">
-        <v>191.38441309983179</v>
+        <v>191.43892832402935</v>
       </c>
       <c r="J4" s="0">
-        <v>28767.558884754704</v>
+        <v>28783.949909029812</v>
       </c>
       <c r="K4" s="0">
-        <v>73.583144609676012</v>
+        <v>73.575232766156148</v>
       </c>
       <c r="L4" s="0">
-        <v>779.64775411139226</v>
+        <v>777.69400289441</v>
       </c>
       <c r="M4" s="0">
-        <v>0.59472474721545188</v>
+        <v>0.59805724286997441</v>
       </c>
       <c r="N4" s="0">
-        <v>0.41050893794841797</v>
+        <v>0.41015744342683302</v>
       </c>
       <c r="O4" s="0">
-        <v>730.37272375048428</v>
+        <v>730.42729260625936</v>
       </c>
       <c r="P4" s="0">
-        <v>895.53123504341681</v>
+        <v>895.49813220354429</v>
       </c>
       <c r="Q4" s="0">
-        <v>46.290390601296721</v>
+        <v>43.256633425945189</v>
       </c>
       <c r="R4" s="0">
-        <v>46.290390601296721</v>
+        <v>43.256633425945189</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B5" s="0">
         <v>4</v>
@@ -633,51 +713,51 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E5" s="0">
-        <v>200.80971659919027</v>
+        <v>199.1902834008097</v>
       </c>
       <c r="F5" s="0">
-        <v>192.71255060728745</v>
+        <v>191.90283400809716</v>
       </c>
       <c r="G5" s="0">
-        <v>1.0420168067226889</v>
+        <v>1.0379746835443038</v>
       </c>
       <c r="H5" s="0">
-        <v>27506</v>
+        <v>27534</v>
       </c>
       <c r="I5" s="0">
-        <v>151.53111575655603</v>
+        <v>151.60822242459957</v>
       </c>
       <c r="J5" s="0">
-        <v>18034.060548443671</v>
+        <v>18052.418495631791</v>
       </c>
       <c r="K5" s="0">
-        <v>62.436018883026186</v>
+        <v>62.357238312590795</v>
       </c>
       <c r="L5" s="0">
-        <v>905.63587998485468</v>
+        <v>903.96888124372549</v>
       </c>
       <c r="M5" s="0">
-        <v>0.27630970989401216</v>
+        <v>0.27761203921462169</v>
       </c>
       <c r="N5" s="0">
-        <v>0.11895778007628496</v>
+        <v>0.11730515159962532</v>
       </c>
       <c r="O5" s="0">
-        <v>411.50992510724933</v>
+        <v>411.66732040386432</v>
       </c>
       <c r="P5" s="0">
-        <v>170.69421217188977</v>
+        <v>170.64680031960486</v>
       </c>
       <c r="Q5" s="0">
-        <v>24.868845876221283</v>
+        <v>26.17763581495549</v>
       </c>
       <c r="R5" s="0">
-        <v>24.868845876221283</v>
+        <v>26.17763581495549</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B6" s="0">
         <v>5</v>
@@ -689,51 +769,51 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E6" s="0">
-        <v>5.668016194331984</v>
+        <v>589.47368421052636</v>
       </c>
       <c r="F6" s="0">
-        <v>4.8582995951417001</v>
+        <v>446.9635627530364</v>
       </c>
       <c r="G6" s="0">
-        <v>1.1666666666666667</v>
+        <v>1.3188405797101452</v>
       </c>
       <c r="H6" s="0">
-        <v>50</v>
+        <v>205707</v>
       </c>
       <c r="I6" s="0">
-        <v>6.4606037311972901</v>
+        <v>414.39321600079228</v>
       </c>
       <c r="J6" s="0">
-        <v>32.782048550213901</v>
+        <v>134869.93722237702</v>
       </c>
       <c r="K6" s="0">
-        <v>2.3257338649951529</v>
+        <v>167.16022959179074</v>
       </c>
       <c r="L6" s="0">
-        <v>20.718533585054026</v>
+        <v>3967.6113360323884</v>
       </c>
       <c r="M6" s="0">
-        <v>0.95968327417437516</v>
+        <v>0.10766307371795013</v>
       </c>
       <c r="N6" s="0">
-        <v>0.15473594881244546</v>
+        <v>0.11752253958138303</v>
       </c>
       <c r="O6" s="0">
-        <v>589.5</v>
+        <v>492.40452196570851</v>
       </c>
       <c r="P6" s="0">
-        <v>97</v>
+        <v>552.11559645515229</v>
       </c>
       <c r="Q6" s="0">
-        <v>6.1244963503649634</v>
+        <v>19.404544921390041</v>
       </c>
       <c r="R6" s="0">
-        <v>6.1244963503649634</v>
+        <v>19.404544921390041</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B7" s="0">
         <v>6</v>
@@ -748,48 +828,48 @@
         <v>9.7165991902834001</v>
       </c>
       <c r="F7" s="0">
-        <v>6.4777327935222671</v>
+        <v>9.7165991902834001</v>
       </c>
       <c r="G7" s="0">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H7" s="0">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="I7" s="0">
-        <v>8.7158309437620378</v>
+        <v>11.338313532461777</v>
       </c>
       <c r="J7" s="0">
-        <v>59.663328361389297</v>
+        <v>100.96870953465881</v>
       </c>
       <c r="K7" s="0">
-        <v>3.4048949346531057</v>
+        <v>4.1016068710001647</v>
       </c>
       <c r="L7" s="0">
-        <v>29.780363948387102</v>
+        <v>35.627530364372468</v>
       </c>
       <c r="M7" s="0">
-        <v>0.845390453241463</v>
+        <v>0.99959766250584337</v>
       </c>
       <c r="N7" s="0">
-        <v>0.15713566000506968</v>
+        <v>0.068597646237994137</v>
       </c>
       <c r="O7" s="0">
-        <v>634.45054945054949</v>
+        <v>277.25974025974028</v>
       </c>
       <c r="P7" s="0">
-        <v>155.71428571428572</v>
+        <v>318.11688311688312</v>
       </c>
       <c r="Q7" s="0">
-        <v>5.0228090464688346</v>
+        <v>7.2763285940585716</v>
       </c>
       <c r="R7" s="0">
-        <v>5.0228090464688346</v>
+        <v>7.2763285940585716</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B8" s="0">
         <v>7</v>
@@ -801,51 +881,51 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E8" s="0">
-        <v>593.52226720647775</v>
+        <v>320.64777327935224</v>
       </c>
       <c r="F8" s="0">
-        <v>448.58299595141699</v>
+        <v>180.56680161943319</v>
       </c>
       <c r="G8" s="0">
-        <v>1.3231046931407944</v>
+        <v>1.7757847533632287</v>
       </c>
       <c r="H8" s="0">
-        <v>210540</v>
+        <v>47377</v>
       </c>
       <c r="I8" s="0">
-        <v>419.23295186176188</v>
+        <v>198.87119353384566</v>
       </c>
       <c r="J8" s="0">
-        <v>138038.65003524069</v>
+        <v>31062.302283269677</v>
       </c>
       <c r="K8" s="0">
-        <v>168.04631274236482</v>
+        <v>88.704127092473342</v>
       </c>
       <c r="L8" s="0">
-        <v>4025.910931174089</v>
+        <v>1340.080971659919</v>
       </c>
       <c r="M8" s="0">
-        <v>0.10702426222190931</v>
+        <v>0.21736090053814569</v>
       </c>
       <c r="N8" s="0">
-        <v>0.117787046427088</v>
+        <v>0.25356125302901139</v>
       </c>
       <c r="O8" s="0">
-        <v>496.12195782274154</v>
+        <v>652.47573717204546</v>
       </c>
       <c r="P8" s="0">
-        <v>551.58658687185334</v>
+        <v>911.01393081030881</v>
       </c>
       <c r="Q8" s="0">
-        <v>23.0254240994594</v>
+        <v>23.489889801609994</v>
       </c>
       <c r="R8" s="0">
-        <v>23.0254240994594</v>
+        <v>23.489889801609994</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B9" s="0">
         <v>8</v>
@@ -857,275 +937,275 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E9" s="0">
-        <v>15.384615384615385</v>
+        <v>8.9068825910931171</v>
       </c>
       <c r="F9" s="0">
-        <v>13.765182186234817</v>
+        <v>7.2874493927125501</v>
       </c>
       <c r="G9" s="0">
-        <v>1.1176470588235294</v>
+        <v>1.2222222222222223</v>
       </c>
       <c r="H9" s="0">
-        <v>288</v>
+        <v>97</v>
       </c>
       <c r="I9" s="0">
-        <v>15.505448954873495</v>
+        <v>8.9985797273140324</v>
       </c>
       <c r="J9" s="0">
-        <v>188.82459964923206</v>
+        <v>63.597174187414964</v>
       </c>
       <c r="K9" s="0">
-        <v>5.7580052974742832</v>
+        <v>3.3095235543022978</v>
       </c>
       <c r="L9" s="0">
-        <v>52.683030837874981</v>
+        <v>30.587757655576251</v>
       </c>
       <c r="M9" s="0">
-        <v>0.85492286586856026</v>
+        <v>0.85418590693116558</v>
       </c>
       <c r="N9" s="0">
-        <v>0.041554143642868337</v>
+        <v>0.30340462727369194</v>
       </c>
       <c r="O9" s="0">
-        <v>275.85763888888891</v>
+        <v>174.32989690721649</v>
       </c>
       <c r="P9" s="0">
-        <v>316.74652777777777</v>
+        <v>948.2268041237113</v>
       </c>
       <c r="Q9" s="0">
-        <v>6.270243764172335</v>
+        <v>5.6733323347712918</v>
       </c>
       <c r="R9" s="0">
-        <v>6.270243764172335</v>
+        <v>5.6733323347712918</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B10" s="0">
         <v>9</v>
       </c>
       <c r="C10" s="0">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D10" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E10" s="0">
-        <v>7.2874493927125501</v>
+        <v>370.1799485861182</v>
       </c>
       <c r="F10" s="0">
-        <v>6.4777327935222671</v>
+        <v>303.34190231362464</v>
       </c>
       <c r="G10" s="0">
-        <v>1.125</v>
+        <v>1.2203389830508475</v>
       </c>
       <c r="H10" s="0">
-        <v>77</v>
+        <v>3106</v>
       </c>
       <c r="I10" s="0">
-        <v>8.0173983860229203</v>
+        <v>323.32268697740017</v>
       </c>
       <c r="J10" s="0">
-        <v>50.484354767329407</v>
+        <v>82103.60756273086</v>
       </c>
       <c r="K10" s="0">
-        <v>2.8876547609568459</v>
+        <v>117.00625334557238</v>
       </c>
       <c r="L10" s="0">
-        <v>25.996930142259334</v>
+        <v>1188.4561326159242</v>
       </c>
       <c r="M10" s="0">
-        <v>0.93869075300985871</v>
+        <v>0.73047573160390833</v>
       </c>
       <c r="N10" s="0">
-        <v>0.20634508499726975</v>
+        <v>0.32867925906731715</v>
       </c>
       <c r="O10" s="0">
-        <v>763.51948051948057</v>
+        <v>527.25273663876374</v>
       </c>
       <c r="P10" s="0">
-        <v>560.80519480519479</v>
+        <v>83.445267224726337</v>
       </c>
       <c r="Q10" s="0">
-        <v>3.1030943396226411</v>
+        <v>92.628</v>
       </c>
       <c r="R10" s="0">
-        <v>3.1030943396226411</v>
+        <v>92.628</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B11" s="0">
         <v>10</v>
       </c>
       <c r="C11" s="0">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D11" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E11" s="0">
-        <v>331.17408906882588</v>
+        <v>185.0899742930591</v>
       </c>
       <c r="F11" s="0">
-        <v>180.56680161943319</v>
+        <v>185.0899742930591</v>
       </c>
       <c r="G11" s="0">
-        <v>1.8340807174887892</v>
+        <v>1</v>
       </c>
       <c r="H11" s="0">
-        <v>50351</v>
+        <v>803</v>
       </c>
       <c r="I11" s="0">
-        <v>205.01807521185225</v>
+        <v>164.39674950056869</v>
       </c>
       <c r="J11" s="0">
-        <v>33012.178531036399</v>
+        <v>21226.399508329967</v>
       </c>
       <c r="K11" s="0">
-        <v>94.771008505833478</v>
+        <v>60.886290468595696</v>
       </c>
       <c r="L11" s="0">
-        <v>1409.7165991902834</v>
+        <v>676.79826428394699</v>
       </c>
       <c r="M11" s="0">
-        <v>0.20874708620574592</v>
+        <v>0.58232807074475335</v>
       </c>
       <c r="N11" s="0">
-        <v>0.24196823421459709</v>
+        <v>0.20055010808409643</v>
       </c>
       <c r="O11" s="0">
-        <v>641.18545808424858</v>
+        <v>331.05603985056041</v>
       </c>
       <c r="P11" s="0">
-        <v>912.85897003038667</v>
+        <v>84.66874221668742</v>
       </c>
       <c r="Q11" s="0">
-        <v>23.63519827586207</v>
+        <v>30.328235294117654</v>
       </c>
       <c r="R11" s="0">
-        <v>23.63519827586207</v>
+        <v>30.328235294117654</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B12" s="0">
         <v>11</v>
       </c>
       <c r="C12" s="0">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D12" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E12" s="0">
-        <v>8.9068825910931171</v>
+        <v>267.35218508997423</v>
       </c>
       <c r="F12" s="0">
-        <v>7.2874493927125501</v>
+        <v>241.64524421593828</v>
       </c>
       <c r="G12" s="0">
-        <v>1.2222222222222223</v>
+        <v>1.1063829787234041</v>
       </c>
       <c r="H12" s="0">
-        <v>98</v>
+        <v>1670</v>
       </c>
       <c r="I12" s="0">
-        <v>9.0448452236762051</v>
+        <v>237.07932890917806</v>
       </c>
       <c r="J12" s="0">
-        <v>64.252815158419239</v>
+        <v>44144.566847958959</v>
       </c>
       <c r="K12" s="0">
-        <v>3.3446759186635813</v>
+        <v>86.066889054668607</v>
       </c>
       <c r="L12" s="0">
-        <v>30.521775622539934</v>
+        <v>934.96654015954982</v>
       </c>
       <c r="M12" s="0">
-        <v>0.86672721559543764</v>
+        <v>0.63459257434447647</v>
       </c>
       <c r="N12" s="0">
-        <v>0.3025608521418327</v>
+        <v>0.48760387044873588</v>
       </c>
       <c r="O12" s="0">
-        <v>174.28571428571428</v>
+        <v>888.33652694610782</v>
       </c>
       <c r="P12" s="0">
-        <v>948.24489795918362</v>
+        <v>114.3497005988024</v>
       </c>
       <c r="Q12" s="0">
-        <v>8.3087110924273162</v>
+        <v>58.558730158730164</v>
       </c>
       <c r="R12" s="0">
-        <v>8.3087110924273162</v>
+        <v>58.558730158730164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B13" s="0">
         <v>12</v>
       </c>
       <c r="C13" s="0">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D13" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E13" s="0">
-        <v>17.813765182186234</v>
+        <v>107.96915167095113</v>
       </c>
       <c r="F13" s="0">
-        <v>9.7165991902834001</v>
+        <v>46.272493573264775</v>
       </c>
       <c r="G13" s="0">
-        <v>1.8333333333333335</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="H13" s="0">
-        <v>220</v>
+        <v>123</v>
       </c>
       <c r="I13" s="0">
-        <v>13.551876715601628</v>
+        <v>64.341030055242328</v>
       </c>
       <c r="J13" s="0">
-        <v>144.24101362094115</v>
+        <v>3251.3663007778159</v>
       </c>
       <c r="K13" s="0">
-        <v>5.4223026407348804</v>
+        <v>33.32786835185837</v>
       </c>
       <c r="L13" s="0">
-        <v>48.473125700104177</v>
+        <v>306.93273191401573</v>
       </c>
       <c r="M13" s="0">
-        <v>0.77143009767292403</v>
+        <v>0.43369993223293818</v>
       </c>
       <c r="N13" s="0">
-        <v>0.09702882547498469</v>
+        <v>0.46280204292068094</v>
       </c>
       <c r="O13" s="0">
-        <v>472.81818181818181</v>
+        <v>841.48780487804879</v>
       </c>
       <c r="P13" s="0">
-        <v>1000.9772727272727</v>
+        <v>113.04878048780488</v>
       </c>
       <c r="Q13" s="0">
-        <v>5.1817567567567568</v>
+        <v>18.758305084745757</v>
       </c>
       <c r="R13" s="0">
-        <v>5.1817567567567568</v>
+        <v>18.758305084745757</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B14" s="0">
         <v>13</v>
@@ -1137,51 +1217,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E14" s="0">
-        <v>370.1799485861182</v>
+        <v>174.80719794344469</v>
       </c>
       <c r="F14" s="0">
-        <v>303.34190231362464</v>
+        <v>143.95886889460152</v>
       </c>
       <c r="G14" s="0">
-        <v>1.2203389830508475</v>
+        <v>1.2142857142857142</v>
       </c>
       <c r="H14" s="0">
-        <v>3107</v>
+        <v>409</v>
       </c>
       <c r="I14" s="0">
-        <v>323.37473087101336</v>
+        <v>117.32676808931656</v>
       </c>
       <c r="J14" s="0">
-        <v>82130.041435094899</v>
+        <v>10811.453796895339</v>
       </c>
       <c r="K14" s="0">
-        <v>117.00674951462612</v>
+        <v>60.080195435199386</v>
       </c>
       <c r="L14" s="0">
-        <v>1166.5205422649358</v>
+        <v>622.10243400785157</v>
       </c>
       <c r="M14" s="0">
-        <v>0.75845029367069461</v>
+        <v>0.35105095563587979</v>
       </c>
       <c r="N14" s="0">
-        <v>0.32861435169468423</v>
+        <v>0.4624967341480769</v>
       </c>
       <c r="O14" s="0">
-        <v>527.29353073704533</v>
+        <v>999.24205378973102</v>
       </c>
       <c r="P14" s="0">
-        <v>83.4766655938204</v>
+        <v>125.44987775061125</v>
       </c>
       <c r="Q14" s="0">
-        <v>106.41230769230782</v>
+        <v>27.00433734939757</v>
       </c>
       <c r="R14" s="0">
-        <v>106.41230769230782</v>
+        <v>27.00433734939757</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B15" s="0">
         <v>14</v>
@@ -1193,51 +1273,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E15" s="0">
-        <v>185.0899742930591</v>
+        <v>61.696658097686367</v>
       </c>
       <c r="F15" s="0">
-        <v>185.0899742930591</v>
+        <v>41.131105398457578</v>
       </c>
       <c r="G15" s="0">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H15" s="0">
-        <v>802</v>
+        <v>67</v>
       </c>
       <c r="I15" s="0">
-        <v>164.29435350838551</v>
+        <v>47.486794566109914</v>
       </c>
       <c r="J15" s="0">
-        <v>21199.96563596592</v>
+        <v>1771.069448391168</v>
       </c>
       <c r="K15" s="0">
-        <v>60.859749596676558</v>
+        <v>18.476925843710998</v>
       </c>
       <c r="L15" s="0">
-        <v>679.47257657039495</v>
+        <v>185.76273157048769</v>
       </c>
       <c r="M15" s="0">
-        <v>0.57703366898987629</v>
+        <v>0.64495331338879647</v>
       </c>
       <c r="N15" s="0">
-        <v>0.20074545544690314</v>
+        <v>0.40499825687613883</v>
       </c>
       <c r="O15" s="0">
-        <v>331.06733167082297</v>
+        <v>848.17910447761199</v>
       </c>
       <c r="P15" s="0">
-        <v>84.644638403990029</v>
+        <v>135.91044776119404</v>
       </c>
       <c r="Q15" s="0">
-        <v>29.634285714285685</v>
+        <v>16.961630901287556</v>
       </c>
       <c r="R15" s="0">
-        <v>29.634285714285685</v>
+        <v>16.961630901287556</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B16" s="0">
         <v>15</v>
@@ -1249,51 +1329,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E16" s="0">
-        <v>262.21079691516707</v>
+        <v>205.65552699228789</v>
       </c>
       <c r="F16" s="0">
-        <v>236.50385604113109</v>
+        <v>195.37275064267351</v>
       </c>
       <c r="G16" s="0">
-        <v>1.1086956521739131</v>
+        <v>1.0526315789473684</v>
       </c>
       <c r="H16" s="0">
-        <v>1658</v>
+        <v>806</v>
       </c>
       <c r="I16" s="0">
-        <v>236.22601121945394</v>
+        <v>164.70355552080804</v>
       </c>
       <c r="J16" s="0">
-        <v>43827.360379590391</v>
+        <v>21305.701125422111</v>
       </c>
       <c r="K16" s="0">
-        <v>86.098346045252129</v>
+        <v>68.696032708034139</v>
       </c>
       <c r="L16" s="0">
-        <v>958.98001840852453</v>
+        <v>756.62203249068079</v>
       </c>
       <c r="M16" s="0">
-        <v>0.5988748327231781</v>
+        <v>0.46767884698454354</v>
       </c>
       <c r="N16" s="0">
-        <v>0.49265870010964197</v>
+        <v>0.39561231876119851</v>
       </c>
       <c r="O16" s="0">
-        <v>888.16284680337753</v>
+        <v>206.32382133995037</v>
       </c>
       <c r="P16" s="0">
-        <v>114.36791314837153</v>
+        <v>151.3697270471464</v>
       </c>
       <c r="Q16" s="0">
-        <v>56.352173913043401</v>
+        <v>44.594838709677418</v>
       </c>
       <c r="R16" s="0">
-        <v>56.352173913043401</v>
+        <v>44.594838709677418</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B17" s="0">
         <v>16</v>
@@ -1305,51 +1385,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E17" s="0">
-        <v>107.96915167095113</v>
+        <v>46.272493573264775</v>
       </c>
       <c r="F17" s="0">
         <v>46.272493573264775</v>
       </c>
       <c r="G17" s="0">
-        <v>2.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="H17" s="0">
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="I17" s="0">
-        <v>63.286187609240997</v>
+        <v>45.680547283192567</v>
       </c>
       <c r="J17" s="0">
-        <v>3145.6308113216264</v>
+        <v>1638.9000865709315</v>
       </c>
       <c r="K17" s="0">
-        <v>33.081390073700817</v>
+        <v>16.690312415012361</v>
       </c>
       <c r="L17" s="0">
-        <v>300.38314708873548</v>
+        <v>164.76616657311655</v>
       </c>
       <c r="M17" s="0">
-        <v>0.4380931755922422</v>
+        <v>0.7586234567547615</v>
       </c>
       <c r="N17" s="0">
-        <v>0.46801777569440101</v>
+        <v>0.47217752737114177</v>
       </c>
       <c r="O17" s="0">
-        <v>841.55462184873954</v>
+        <v>631.30645161290317</v>
       </c>
       <c r="P17" s="0">
-        <v>113.15126050420169</v>
+        <v>141.64516129032259</v>
       </c>
       <c r="Q17" s="0">
-        <v>18.470719999999996</v>
+        <v>35.70894736838035</v>
       </c>
       <c r="R17" s="0">
-        <v>18.470719999999996</v>
+        <v>35.70894736838035</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B18" s="0">
         <v>17</v>
@@ -1361,51 +1441,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E18" s="0">
-        <v>174.80719794344469</v>
+        <v>113.11053984575834</v>
       </c>
       <c r="F18" s="0">
-        <v>143.95886889460152</v>
+        <v>102.82776349614394</v>
       </c>
       <c r="G18" s="0">
-        <v>1.2142857142857142</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H18" s="0">
-        <v>424</v>
+        <v>291</v>
       </c>
       <c r="I18" s="0">
-        <v>119.4588644031914</v>
+        <v>98.96507272662717</v>
       </c>
       <c r="J18" s="0">
-        <v>11207.961882356047</v>
+        <v>7692.2568579377594</v>
       </c>
       <c r="K18" s="0">
-        <v>60.577954935420642</v>
+        <v>37.998476514163521</v>
       </c>
       <c r="L18" s="0">
-        <v>638.69364813809364</v>
+        <v>390.96087691511633</v>
       </c>
       <c r="M18" s="0">
-        <v>0.34526401386971178</v>
+        <v>0.63240754315906322</v>
       </c>
       <c r="N18" s="0">
-        <v>0.45810212488317797</v>
+        <v>0.48282050097675927</v>
       </c>
       <c r="O18" s="0">
-        <v>999.31839622641508</v>
+        <v>794.14776632302403</v>
       </c>
       <c r="P18" s="0">
-        <v>125.48349056603773</v>
+        <v>146.86254295532646</v>
       </c>
       <c r="Q18" s="0">
-        <v>23.350361445783129</v>
+        <v>20.608275862068968</v>
       </c>
       <c r="R18" s="0">
-        <v>23.350361445783129</v>
+        <v>20.608275862068968</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B19" s="0">
         <v>18</v>
@@ -1417,51 +1497,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E19" s="0">
-        <v>61.696658097686367</v>
+        <v>154.24164524421593</v>
       </c>
       <c r="F19" s="0">
-        <v>35.989717223650381</v>
+        <v>87.403598971722346</v>
       </c>
       <c r="G19" s="0">
-        <v>1.7142857142857142</v>
+        <v>1.7647058823529416</v>
       </c>
       <c r="H19" s="0">
-        <v>65</v>
+        <v>257</v>
       </c>
       <c r="I19" s="0">
-        <v>46.772666750305703</v>
+        <v>93.004083054979091</v>
       </c>
       <c r="J19" s="0">
-        <v>1718.2017036630734</v>
+        <v>6793.5051975601518</v>
       </c>
       <c r="K19" s="0">
-        <v>18.083603614821737</v>
+        <v>42.608865814402499</v>
       </c>
       <c r="L19" s="0">
-        <v>178.09605740735205</v>
+        <v>451.28665261330013</v>
       </c>
       <c r="M19" s="0">
-        <v>0.68073079628620536</v>
+        <v>0.4191783060116071</v>
       </c>
       <c r="N19" s="0">
-        <v>0.40557408073011286</v>
+        <v>0.38257958565784184</v>
       </c>
       <c r="O19" s="0">
-        <v>848.21538461538466</v>
+        <v>821.05447470817126</v>
       </c>
       <c r="P19" s="0">
-        <v>135.83076923076922</v>
+        <v>172.63035019455253</v>
       </c>
       <c r="Q19" s="0">
-        <v>16.708611111111111</v>
+        <v>20.161212121212124</v>
       </c>
       <c r="R19" s="0">
-        <v>16.708611111111111</v>
+        <v>20.161212121212124</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B20" s="0">
         <v>19</v>
@@ -1473,51 +1553,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E20" s="0">
-        <v>205.65552699228789</v>
+        <v>1172.2365038560411</v>
       </c>
       <c r="F20" s="0">
-        <v>195.37275064267351</v>
+        <v>1100.2570694087401</v>
       </c>
       <c r="G20" s="0">
-        <v>1.0526315789473684</v>
+        <v>1.0654205607476637</v>
       </c>
       <c r="H20" s="0">
-        <v>807</v>
+        <v>17021</v>
       </c>
       <c r="I20" s="0">
-        <v>164.80569727048356</v>
+        <v>756.88167313555721</v>
       </c>
       <c r="J20" s="0">
-        <v>21332.134997786157</v>
+        <v>449930.9415084488</v>
       </c>
       <c r="K20" s="0">
-        <v>68.75051521776939</v>
+        <v>394.97924802443379</v>
       </c>
       <c r="L20" s="0">
-        <v>757.18897803811581</v>
+        <v>5695.5106696334742</v>
       </c>
       <c r="M20" s="0">
-        <v>0.46755813784770972</v>
+        <v>0.1742971897341353</v>
       </c>
       <c r="N20" s="0">
-        <v>0.3953709782692269</v>
+        <v>0.24726622611214871</v>
       </c>
       <c r="O20" s="0">
-        <v>206.30235439900866</v>
+        <v>491.0935902708419</v>
       </c>
       <c r="P20" s="0">
-        <v>151.35687732342006</v>
+        <v>282.94618412549204</v>
       </c>
       <c r="Q20" s="0">
-        <v>44.629247311827967</v>
+        <v>72.1802714932127</v>
       </c>
       <c r="R20" s="0">
-        <v>44.629247311827967</v>
+        <v>72.1802714932127</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B21" s="0">
         <v>20</v>
@@ -1529,51 +1609,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E21" s="0">
-        <v>46.272493573264775</v>
+        <v>2493.5732647814907</v>
       </c>
       <c r="F21" s="0">
-        <v>46.272493573264775</v>
+        <v>2133.6760925449867</v>
       </c>
       <c r="G21" s="0">
-        <v>1</v>
+        <v>1.1686746987951808</v>
       </c>
       <c r="H21" s="0">
-        <v>62</v>
+        <v>78797</v>
       </c>
       <c r="I21" s="0">
-        <v>45.680547283192567</v>
+        <v>1628.5094955998413</v>
       </c>
       <c r="J21" s="0">
-        <v>1638.9000865709315</v>
+        <v>2082909.8406698336</v>
       </c>
       <c r="K21" s="0">
-        <v>16.690312415012361</v>
+        <v>833.78863109689735</v>
       </c>
       <c r="L21" s="0">
-        <v>164.76616657311655</v>
+        <v>13290.488431876605</v>
       </c>
       <c r="M21" s="0">
-        <v>0.7586234567547615</v>
+        <v>0.1481830236634743</v>
       </c>
       <c r="N21" s="0">
-        <v>0.4722348453884444</v>
+        <v>0.27619611613855805</v>
       </c>
       <c r="O21" s="0">
-        <v>631.30645161290317</v>
+        <v>261.66034239882231</v>
       </c>
       <c r="P21" s="0">
-        <v>141.64516129032259</v>
+        <v>434.07433024099902</v>
       </c>
       <c r="Q21" s="0">
-        <v>35.70894736838035</v>
+        <v>110.81598156682028</v>
       </c>
       <c r="R21" s="0">
-        <v>35.70894736838035</v>
+        <v>110.81598156682028</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B22" s="0">
         <v>21</v>
@@ -1585,51 +1665,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E22" s="0">
-        <v>113.11053984575834</v>
+        <v>221.07969151670949</v>
       </c>
       <c r="F22" s="0">
-        <v>102.82776349614394</v>
+        <v>190.23136246786629</v>
       </c>
       <c r="G22" s="0">
-        <v>1.1000000000000001</v>
+        <v>1.1621621621621623</v>
       </c>
       <c r="H22" s="0">
-        <v>289</v>
+        <v>984</v>
       </c>
       <c r="I22" s="0">
-        <v>98.624400208862269</v>
+        <v>181.98391464235726</v>
       </c>
       <c r="J22" s="0">
-        <v>7639.3891132096642</v>
+        <v>26010.930406222527</v>
       </c>
       <c r="K22" s="0">
-        <v>37.974781540883775</v>
+        <v>69.090573638776803</v>
       </c>
       <c r="L22" s="0">
-        <v>390.65835130532741</v>
+        <v>738.72825736798097</v>
       </c>
       <c r="M22" s="0">
-        <v>0.629034216540031</v>
+        <v>0.59895794177076711</v>
       </c>
       <c r="N22" s="0">
-        <v>0.48436231738011715</v>
+        <v>0.49397796180266323</v>
       </c>
       <c r="O22" s="0">
-        <v>794.25259515570929</v>
+        <v>727.54573170731703</v>
       </c>
       <c r="P22" s="0">
-        <v>146.91003460207614</v>
+        <v>288.70731707317071</v>
       </c>
       <c r="Q22" s="0">
-        <v>19.142680412371124</v>
+        <v>42.836965294592417</v>
       </c>
       <c r="R22" s="0">
-        <v>19.142680412371124</v>
+        <v>42.836965294592417</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B23" s="0">
         <v>22</v>
@@ -1641,51 +1721,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E23" s="0">
-        <v>154.24164524421593</v>
+        <v>221.07969151670949</v>
       </c>
       <c r="F23" s="0">
-        <v>87.403598971722346</v>
+        <v>164.52442159383031</v>
       </c>
       <c r="G23" s="0">
-        <v>1.7647058823529416</v>
+        <v>1.34375</v>
       </c>
       <c r="H23" s="0">
-        <v>256</v>
+        <v>916</v>
       </c>
       <c r="I23" s="0">
-        <v>92.822964902458608</v>
+        <v>175.58329327922533</v>
       </c>
       <c r="J23" s="0">
-        <v>6767.0713251961042</v>
+        <v>24213.427085467309</v>
       </c>
       <c r="K23" s="0">
-        <v>42.82191950537193</v>
+        <v>69.771200456599971</v>
       </c>
       <c r="L23" s="0">
-        <v>450.25019665160795</v>
+        <v>735.7538489603827</v>
       </c>
       <c r="M23" s="0">
-        <v>0.41947182511845454</v>
+        <v>0.56208376430178886</v>
       </c>
       <c r="N23" s="0">
-        <v>0.38259712850820127</v>
+        <v>0.28269714050550732</v>
       </c>
       <c r="O23" s="0">
-        <v>820.94140625</v>
+        <v>462.04366812227073</v>
       </c>
       <c r="P23" s="0">
-        <v>172.57421875</v>
+        <v>418.48799126637556</v>
       </c>
       <c r="Q23" s="0">
-        <v>20.256000000000004</v>
+        <v>44.845405405405423</v>
       </c>
       <c r="R23" s="0">
-        <v>20.256000000000004</v>
+        <v>44.845405405405423</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B24" s="0">
         <v>23</v>
@@ -1697,51 +1777,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E24" s="0">
-        <v>1172.2365038560411</v>
+        <v>143.95886889460152</v>
       </c>
       <c r="F24" s="0">
-        <v>1100.2570694087401</v>
+        <v>123.39331619537273</v>
       </c>
       <c r="G24" s="0">
-        <v>1.0654205607476637</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="H24" s="0">
-        <v>17003</v>
+        <v>379</v>
       </c>
       <c r="I24" s="0">
-        <v>756.48135958490172</v>
+        <v>112.94189197039627</v>
       </c>
       <c r="J24" s="0">
-        <v>449455.13180589594</v>
+        <v>10018.43762597392</v>
       </c>
       <c r="K24" s="0">
-        <v>394.94330685687191</v>
+        <v>45.42388932578163</v>
       </c>
       <c r="L24" s="0">
-        <v>5711.7908736617946</v>
+        <v>528.9398566505763</v>
       </c>
       <c r="M24" s="0">
-        <v>0.17312174107788583</v>
+        <v>0.44998421175297443</v>
       </c>
       <c r="N24" s="0">
-        <v>0.24808767233380813</v>
+        <v>0.31770271631607477</v>
       </c>
       <c r="O24" s="0">
-        <v>491.14085749573604</v>
+        <v>32.195250659630609</v>
       </c>
       <c r="P24" s="0">
-        <v>282.9083102981827</v>
+        <v>472.89445910290237</v>
       </c>
       <c r="Q24" s="0">
-        <v>81.335858585858603</v>
+        <v>30.139534883720927</v>
       </c>
       <c r="R24" s="0">
-        <v>81.335858585858603</v>
+        <v>30.139534883720927</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B25" s="0">
         <v>24</v>
@@ -1753,51 +1833,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E25" s="0">
-        <v>2493.5732647814907</v>
+        <v>190.23136246786629</v>
       </c>
       <c r="F25" s="0">
-        <v>2133.6760925449867</v>
+        <v>143.95886889460152</v>
       </c>
       <c r="G25" s="0">
-        <v>1.1686746987951808</v>
+        <v>1.3214285714285714</v>
       </c>
       <c r="H25" s="0">
-        <v>78750</v>
+        <v>691</v>
       </c>
       <c r="I25" s="0">
-        <v>1628.0237451072308</v>
+        <v>152.50162709145562</v>
       </c>
       <c r="J25" s="0">
-        <v>2081667.4486687235</v>
+        <v>18265.805803556672</v>
       </c>
       <c r="K25" s="0">
-        <v>833.95297834450287</v>
+        <v>60.47182630670904</v>
       </c>
       <c r="L25" s="0">
-        <v>13383.033419023135</v>
+        <v>604.18589607439878</v>
       </c>
       <c r="M25" s="0">
-        <v>0.14605354085231081</v>
+        <v>0.62879276215908919</v>
       </c>
       <c r="N25" s="0">
-        <v>0.27657205966668519</v>
+        <v>0.29778162620906684</v>
       </c>
       <c r="O25" s="0">
-        <v>261.69471746031746</v>
+        <v>518.59623733719252</v>
       </c>
       <c r="P25" s="0">
-        <v>434.05380317460316</v>
+        <v>498.73661360347324</v>
       </c>
       <c r="Q25" s="0">
-        <v>92.546571428571411</v>
+        <v>53.301333333333353</v>
       </c>
       <c r="R25" s="0">
-        <v>92.546571428571411</v>
+        <v>53.301333333333353</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B26" s="0">
         <v>25</v>
@@ -1809,51 +1889,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E26" s="0">
-        <v>221.07969151670949</v>
+        <v>339.331619537275</v>
       </c>
       <c r="F26" s="0">
-        <v>190.23136246786629</v>
+        <v>318.76606683804624</v>
       </c>
       <c r="G26" s="0">
-        <v>1.1621621621621623</v>
+        <v>1.064516129032258</v>
       </c>
       <c r="H26" s="0">
-        <v>987</v>
+        <v>2085</v>
       </c>
       <c r="I26" s="0">
-        <v>182.26111802411378</v>
+        <v>264.90397999274535</v>
       </c>
       <c r="J26" s="0">
-        <v>26090.232023314667</v>
+        <v>55114.623879038583</v>
       </c>
       <c r="K26" s="0">
-        <v>69.109680630991974</v>
+        <v>108.85500685511379</v>
       </c>
       <c r="L26" s="0">
-        <v>745.67009733623252</v>
+        <v>1126.9253308014218</v>
       </c>
       <c r="M26" s="0">
-        <v>0.58965006454088453</v>
+        <v>0.54536395439602126</v>
       </c>
       <c r="N26" s="0">
-        <v>0.49202025303622027</v>
+        <v>0.3640973521467798</v>
       </c>
       <c r="O26" s="0">
-        <v>727.57750759878422</v>
+        <v>649.15107913669067</v>
       </c>
       <c r="P26" s="0">
-        <v>288.75379939209728</v>
+        <v>565.96019184652278</v>
       </c>
       <c r="Q26" s="0">
-        <v>43.551275720164611</v>
+        <v>60.023418803418778</v>
       </c>
       <c r="R26" s="0">
-        <v>43.551275720164611</v>
+        <v>60.023418803418778</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B27" s="0">
         <v>26</v>
@@ -1865,51 +1945,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E27" s="0">
-        <v>221.07969151670949</v>
+        <v>51.413881748071972</v>
       </c>
       <c r="F27" s="0">
-        <v>164.52442159383031</v>
+        <v>41.131105398457578</v>
       </c>
       <c r="G27" s="0">
-        <v>1.34375</v>
+        <v>1.25</v>
       </c>
       <c r="H27" s="0">
-        <v>918</v>
+        <v>66</v>
       </c>
       <c r="I27" s="0">
-        <v>175.77487357983571</v>
+        <v>47.131083231234342</v>
       </c>
       <c r="J27" s="0">
-        <v>24266.294830195406</v>
+        <v>1744.6355760271206</v>
       </c>
       <c r="K27" s="0">
-        <v>69.878190483206666</v>
+        <v>17.821190892362768</v>
       </c>
       <c r="L27" s="0">
-        <v>724.23491417057323</v>
+        <v>168.77478086234254</v>
       </c>
       <c r="M27" s="0">
-        <v>0.58137241125146888</v>
+        <v>0.76966100354704947</v>
       </c>
       <c r="N27" s="0">
-        <v>0.28203219120288725</v>
+        <v>0.61776484792717157</v>
       </c>
       <c r="O27" s="0">
-        <v>462.06427015250546</v>
+        <v>751.87878787878788</v>
       </c>
       <c r="P27" s="0">
-        <v>418.520697167756</v>
+        <v>604.969696969697</v>
       </c>
       <c r="Q27" s="0">
-        <v>58.636720142602492</v>
+        <v>13.131999999999998</v>
       </c>
       <c r="R27" s="0">
-        <v>58.636720142602492</v>
+        <v>13.131999999999998</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B28" s="0">
         <v>27</v>
@@ -1921,51 +2001,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E28" s="0">
-        <v>143.95886889460152</v>
+        <v>113.11053984575834</v>
       </c>
       <c r="F28" s="0">
-        <v>123.39331619537273</v>
+        <v>56.55526992287917</v>
       </c>
       <c r="G28" s="0">
-        <v>1.1666666666666667</v>
+        <v>2</v>
       </c>
       <c r="H28" s="0">
-        <v>379</v>
+        <v>179</v>
       </c>
       <c r="I28" s="0">
-        <v>112.94189197039627</v>
+        <v>77.617914420417577</v>
       </c>
       <c r="J28" s="0">
-        <v>10018.43762597392</v>
+        <v>4731.6631531644634</v>
       </c>
       <c r="K28" s="0">
-        <v>45.42388932578163</v>
+        <v>33.086117352460398</v>
       </c>
       <c r="L28" s="0">
-        <v>528.9398566505763</v>
+        <v>307.47814161793224</v>
       </c>
       <c r="M28" s="0">
-        <v>0.44998421175297443</v>
+        <v>0.6289196854998812</v>
       </c>
       <c r="N28" s="0">
-        <v>0.317776809272589</v>
+        <v>0.49875819445396746</v>
       </c>
       <c r="O28" s="0">
-        <v>32.195250659630609</v>
+        <v>559.90502793296093</v>
       </c>
       <c r="P28" s="0">
-        <v>472.89445910290237</v>
+        <v>625.9441340782123</v>
       </c>
       <c r="Q28" s="0">
-        <v>30.139534883720927</v>
+        <v>24.150697674418598</v>
       </c>
       <c r="R28" s="0">
-        <v>30.139534883720927</v>
+        <v>24.150697674418598</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B29" s="0">
         <v>28</v>
@@ -1977,51 +2057,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E29" s="0">
-        <v>190.23136246786629</v>
+        <v>71.979434447300761</v>
       </c>
       <c r="F29" s="0">
-        <v>143.95886889460152</v>
+        <v>56.55526992287917</v>
       </c>
       <c r="G29" s="0">
-        <v>1.3214285714285714</v>
+        <v>1.2727272727272727</v>
       </c>
       <c r="H29" s="0">
-        <v>696</v>
+        <v>90</v>
       </c>
       <c r="I29" s="0">
-        <v>153.05237509954992</v>
+        <v>55.037247799057205</v>
       </c>
       <c r="J29" s="0">
-        <v>18397.975165376909</v>
+        <v>2379.0485127642555</v>
       </c>
       <c r="K29" s="0">
-        <v>60.674442565038284</v>
+        <v>24.798509867003716</v>
       </c>
       <c r="L29" s="0">
-        <v>606.6296229970086</v>
+        <v>223.06878045002381</v>
       </c>
       <c r="M29" s="0">
-        <v>0.62825024163783505</v>
+        <v>0.60080781937109651</v>
       </c>
       <c r="N29" s="0">
-        <v>0.29647491126699699</v>
+        <v>0.47825405002724058</v>
       </c>
       <c r="O29" s="0">
-        <v>518.75</v>
+        <v>601.11111111111109</v>
       </c>
       <c r="P29" s="0">
-        <v>498.82183908045977</v>
+        <v>628.70000000000005</v>
       </c>
       <c r="Q29" s="0">
-        <v>57.028571428571425</v>
+        <v>18.420909090909088</v>
       </c>
       <c r="R29" s="0">
-        <v>57.028571428571425</v>
+        <v>18.420909090909088</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B30" s="0">
         <v>29</v>
@@ -2033,51 +2113,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E30" s="0">
-        <v>339.331619537275</v>
+        <v>298.20051413881743</v>
       </c>
       <c r="F30" s="0">
-        <v>318.76606683804624</v>
+        <v>267.35218508997423</v>
       </c>
       <c r="G30" s="0">
-        <v>1.064516129032258</v>
+        <v>1.1153846153846154</v>
       </c>
       <c r="H30" s="0">
-        <v>2074</v>
+        <v>1856</v>
       </c>
       <c r="I30" s="0">
-        <v>264.2042684141166</v>
+        <v>249.93348194330068</v>
       </c>
       <c r="J30" s="0">
-        <v>54823.851283034062</v>
+        <v>49061.267107671752</v>
       </c>
       <c r="K30" s="0">
-        <v>108.64143281575119</v>
+        <v>91.776119947506174</v>
       </c>
       <c r="L30" s="0">
-        <v>1136.2547623948351</v>
+        <v>949.64675447237153</v>
       </c>
       <c r="M30" s="0">
-        <v>0.53361492946589384</v>
+        <v>0.6836352499269791</v>
       </c>
       <c r="N30" s="0">
-        <v>0.36785430909842454</v>
+        <v>0.34380595119321328</v>
       </c>
       <c r="O30" s="0">
-        <v>649.24349083895856</v>
+        <v>92.602370689655174</v>
       </c>
       <c r="P30" s="0">
-        <v>565.91369334619094</v>
+        <v>699.1842672413793</v>
       </c>
       <c r="Q30" s="0">
-        <v>59.136833731105838</v>
+        <v>65.291897435897454</v>
       </c>
       <c r="R30" s="0">
-        <v>59.136833731105838</v>
+        <v>65.291897435897454</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B31" s="0">
         <v>30</v>
@@ -2089,51 +2169,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E31" s="0">
-        <v>51.413881748071972</v>
+        <v>200.5141388174807</v>
       </c>
       <c r="F31" s="0">
-        <v>41.131105398457578</v>
+        <v>174.80719794344469</v>
       </c>
       <c r="G31" s="0">
-        <v>1.25</v>
+        <v>1.1470588235294119</v>
       </c>
       <c r="H31" s="0">
-        <v>64</v>
+        <v>641</v>
       </c>
       <c r="I31" s="0">
-        <v>46.411482451229304</v>
+        <v>146.8806103092646</v>
       </c>
       <c r="J31" s="0">
-        <v>1691.7678312990261</v>
+        <v>16944.112185354308</v>
       </c>
       <c r="K31" s="0">
-        <v>17.581261878081609</v>
+        <v>61.571669691973796</v>
       </c>
       <c r="L31" s="0">
-        <v>168.29864799538856</v>
+        <v>687.34048686538665</v>
       </c>
       <c r="M31" s="0">
-        <v>0.75056683827212967</v>
+        <v>0.45069716870801912</v>
       </c>
       <c r="N31" s="0">
-        <v>0.62250439158939841</v>
+        <v>0.38664531812322217</v>
       </c>
       <c r="O31" s="0">
-        <v>751.84375</v>
+        <v>386.03120124804991</v>
       </c>
       <c r="P31" s="0">
-        <v>605.03125</v>
+        <v>739.27925117004679</v>
       </c>
       <c r="Q31" s="0">
-        <v>13.131999999999998</v>
+        <v>32.664615384615367</v>
       </c>
       <c r="R31" s="0">
-        <v>13.131999999999998</v>
+        <v>32.664615384615367</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B32" s="0">
         <v>31</v>
@@ -2145,51 +2225,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E32" s="0">
-        <v>113.11053984575834</v>
+        <v>56.55526992287917</v>
       </c>
       <c r="F32" s="0">
-        <v>56.55526992287917</v>
+        <v>41.131105398457578</v>
       </c>
       <c r="G32" s="0">
-        <v>2</v>
+        <v>1.375</v>
       </c>
       <c r="H32" s="0">
-        <v>178</v>
+        <v>61</v>
       </c>
       <c r="I32" s="0">
-        <v>77.400800947799496</v>
+        <v>45.310658221632629</v>
       </c>
       <c r="J32" s="0">
-        <v>4705.2292808004158</v>
+        <v>1612.4662142068842</v>
       </c>
       <c r="K32" s="0">
-        <v>33.083346525141209</v>
+        <v>19.126950801882025</v>
       </c>
       <c r="L32" s="0">
-        <v>306.61376168373607</v>
+        <v>181.98478497050439</v>
       </c>
       <c r="M32" s="0">
-        <v>0.62893732384087808</v>
+        <v>0.61182938008607146</v>
       </c>
       <c r="N32" s="0">
-        <v>0.50043633153695133</v>
+        <v>0.41812370332778193</v>
       </c>
       <c r="O32" s="0">
-        <v>559.87640449438197</v>
+        <v>601.24590163934431</v>
       </c>
       <c r="P32" s="0">
-        <v>625.92134831460669</v>
+        <v>751.57377049180332</v>
       </c>
       <c r="Q32" s="0">
-        <v>24.150697674418598</v>
+        <v>14.803187250996011</v>
       </c>
       <c r="R32" s="0">
-        <v>24.150697674418598</v>
+        <v>14.803187250996011</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B33" s="0">
         <v>32</v>
@@ -2201,51 +2281,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E33" s="0">
-        <v>71.979434447300761</v>
+        <v>66.838046272493557</v>
       </c>
       <c r="F33" s="0">
-        <v>56.55526992287917</v>
+        <v>66.838046272493557</v>
       </c>
       <c r="G33" s="0">
-        <v>1.2727272727272727</v>
+        <v>1</v>
       </c>
       <c r="H33" s="0">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="I33" s="0">
-        <v>55.645412645820144</v>
+        <v>60.845966814428756</v>
       </c>
       <c r="J33" s="0">
-        <v>2431.9162574923498</v>
+        <v>2907.7259600452012</v>
       </c>
       <c r="K33" s="0">
-        <v>25.092022981464918</v>
+        <v>24.560112401453939</v>
       </c>
       <c r="L33" s="0">
-        <v>223.06878045002381</v>
+        <v>251.59372652112131</v>
       </c>
       <c r="M33" s="0">
-        <v>0.61415910424600972</v>
+        <v>0.57724970848720925</v>
       </c>
       <c r="N33" s="0">
-        <v>0.47493809623059224</v>
+        <v>0.53850649931430405</v>
       </c>
       <c r="O33" s="0">
-        <v>601.054347826087</v>
+        <v>583.92727272727268</v>
       </c>
       <c r="P33" s="0">
-        <v>628.83695652173913</v>
+        <v>760.70909090909095</v>
       </c>
       <c r="Q33" s="0">
-        <v>21.591111111111111</v>
+        <v>20.780799999999999</v>
       </c>
       <c r="R33" s="0">
-        <v>21.591111111111111</v>
+        <v>20.780799999999999</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B34" s="0">
         <v>33</v>
@@ -2257,51 +2337,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E34" s="0">
-        <v>298.20051413881743</v>
+        <v>71.979434447300761</v>
       </c>
       <c r="F34" s="0">
-        <v>267.35218508997423</v>
+        <v>25.706940874035986</v>
       </c>
       <c r="G34" s="0">
-        <v>1.1153846153846154</v>
+        <v>2.7999999999999998</v>
       </c>
       <c r="H34" s="0">
-        <v>1847</v>
+        <v>76</v>
       </c>
       <c r="I34" s="0">
-        <v>249.3267645716615</v>
+        <v>50.575740456204976</v>
       </c>
       <c r="J34" s="0">
-        <v>48823.362256395332</v>
+        <v>2008.9742996675934</v>
       </c>
       <c r="K34" s="0">
-        <v>91.468540865273653</v>
+        <v>21.603827141930985</v>
       </c>
       <c r="L34" s="0">
-        <v>945.81950002723772</v>
+        <v>197.40368277133101</v>
       </c>
       <c r="M34" s="0">
-        <v>0.68583717341363792</v>
+        <v>0.64784892688923201</v>
       </c>
       <c r="N34" s="0">
-        <v>0.34554992825614517</v>
+        <v>0.69979724970179447</v>
       </c>
       <c r="O34" s="0">
-        <v>92.690308608554417</v>
+        <v>956.17105263157896</v>
       </c>
       <c r="P34" s="0">
-        <v>699.14943151055763</v>
+        <v>853.65789473684208</v>
       </c>
       <c r="Q34" s="0">
-        <v>57.647123287671278</v>
+        <v>16.292244897959183</v>
       </c>
       <c r="R34" s="0">
-        <v>57.647123287671278</v>
+        <v>16.292244897959183</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B35" s="0">
         <v>34</v>
@@ -2313,51 +2393,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E35" s="0">
-        <v>200.5141388174807</v>
+        <v>128.53470437017992</v>
       </c>
       <c r="F35" s="0">
-        <v>174.80719794344469</v>
+        <v>56.55526992287917</v>
       </c>
       <c r="G35" s="0">
-        <v>1.1470588235294119</v>
+        <v>2.2727272727272725</v>
       </c>
       <c r="H35" s="0">
-        <v>640</v>
+        <v>186</v>
       </c>
       <c r="I35" s="0">
-        <v>146.76599413081919</v>
+        <v>79.12102881204197</v>
       </c>
       <c r="J35" s="0">
-        <v>16917.678312990261</v>
+        <v>4916.7002597127948</v>
       </c>
       <c r="K35" s="0">
-        <v>61.532418622510455</v>
+        <v>36.346066023042539</v>
       </c>
       <c r="L35" s="0">
-        <v>681.82752712906495</v>
+        <v>341.40027469336081</v>
       </c>
       <c r="M35" s="0">
-        <v>0.45730038290306896</v>
+        <v>0.53009763235657381</v>
       </c>
       <c r="N35" s="0">
-        <v>0.38670921093201416</v>
+        <v>0.73712327504169639</v>
       </c>
       <c r="O35" s="0">
-        <v>386.05781250000001</v>
+        <v>906.11827956989248</v>
       </c>
       <c r="P35" s="0">
-        <v>739.31093750000002</v>
+        <v>904.98924731182797</v>
       </c>
       <c r="Q35" s="0">
-        <v>32.347999999999971</v>
+        <v>18.276107382550332</v>
       </c>
       <c r="R35" s="0">
-        <v>32.347999999999971</v>
+        <v>18.276107382550332</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B36" s="0">
         <v>35</v>
@@ -2369,51 +2449,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E36" s="0">
-        <v>56.55526992287917</v>
+        <v>102.82776349614394</v>
       </c>
       <c r="F36" s="0">
-        <v>41.131105398457578</v>
+        <v>102.82776349614394</v>
       </c>
       <c r="G36" s="0">
-        <v>1.375</v>
+        <v>1</v>
       </c>
       <c r="H36" s="0">
-        <v>59</v>
+        <v>243</v>
       </c>
       <c r="I36" s="0">
-        <v>44.561670135317314</v>
+        <v>90.435426367635557</v>
       </c>
       <c r="J36" s="0">
-        <v>1559.5984694787896</v>
+        <v>6423.4309844634899</v>
       </c>
       <c r="K36" s="0">
-        <v>18.800507176966239</v>
+        <v>36.574424236092121</v>
       </c>
       <c r="L36" s="0">
-        <v>175.35453556426069</v>
+        <v>356.20042724512268</v>
       </c>
       <c r="M36" s="0">
-        <v>0.63736565504754739</v>
+        <v>0.63619178111807817</v>
       </c>
       <c r="N36" s="0">
-        <v>0.42129132004634567</v>
+        <v>0.50263449045368502</v>
       </c>
       <c r="O36" s="0">
-        <v>601.23728813559319</v>
+        <v>313.04938271604937</v>
       </c>
       <c r="P36" s="0">
-        <v>751.40677966101691</v>
+        <v>946.90123456790127</v>
       </c>
       <c r="Q36" s="0">
-        <v>15.176578645235354</v>
+        <v>21.51576923076923</v>
       </c>
       <c r="R36" s="0">
-        <v>15.176578645235354</v>
+        <v>21.51576923076923</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B37" s="0">
         <v>36</v>
@@ -2425,51 +2505,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E37" s="0">
-        <v>66.838046272493557</v>
+        <v>149.10025706940871</v>
       </c>
       <c r="F37" s="0">
-        <v>66.838046272493557</v>
+        <v>143.95886889460152</v>
       </c>
       <c r="G37" s="0">
-        <v>1</v>
+        <v>1.0357142857142856</v>
       </c>
       <c r="H37" s="0">
-        <v>110</v>
+        <v>230</v>
       </c>
       <c r="I37" s="0">
-        <v>60.845966814428756</v>
+        <v>87.983122650364038</v>
       </c>
       <c r="J37" s="0">
-        <v>2907.7259600452012</v>
+        <v>6079.7906437308748</v>
       </c>
       <c r="K37" s="0">
-        <v>24.560112401453939</v>
+        <v>58.619446494517391</v>
       </c>
       <c r="L37" s="0">
-        <v>251.59372652112131</v>
+        <v>572.02165190084213</v>
       </c>
       <c r="M37" s="0">
-        <v>0.57724970848720925</v>
+        <v>0.23349283220621125</v>
       </c>
       <c r="N37" s="0">
-        <v>0.53855661444548741</v>
+        <v>0.54685896642520104</v>
       </c>
       <c r="O37" s="0">
-        <v>583.92727272727268</v>
+        <v>365.99130434782609</v>
       </c>
       <c r="P37" s="0">
-        <v>760.70909090909095</v>
+        <v>980.87826086956522</v>
       </c>
       <c r="Q37" s="0">
-        <v>20.780799999999999</v>
+        <v>15.129651567944249</v>
       </c>
       <c r="R37" s="0">
-        <v>20.780799999999999</v>
+        <v>15.129651567944249</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B38" s="0">
         <v>37</v>
@@ -2481,1110 +2561,1110 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E38" s="0">
-        <v>71.979434447300761</v>
+        <v>87.403598971722346</v>
       </c>
       <c r="F38" s="0">
-        <v>25.706940874035986</v>
+        <v>61.696658097686367</v>
       </c>
       <c r="G38" s="0">
-        <v>2.7999999999999998</v>
+        <v>1.4166666666666665</v>
       </c>
       <c r="H38" s="0">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="I38" s="0">
-        <v>50.575740456204976</v>
+        <v>68.888227424056737</v>
       </c>
       <c r="J38" s="0">
-        <v>2008.9742996675934</v>
+        <v>3727.1760033306668</v>
       </c>
       <c r="K38" s="0">
-        <v>21.603827141930985</v>
+        <v>27.749892897314066</v>
       </c>
       <c r="L38" s="0">
-        <v>197.40368277133101</v>
+        <v>287.6297286907166</v>
       </c>
       <c r="M38" s="0">
-        <v>0.64784892688923201</v>
+        <v>0.56613789019932426</v>
       </c>
       <c r="N38" s="0">
-        <v>0.69982984972799311</v>
+        <v>0.60824092599297153</v>
       </c>
       <c r="O38" s="0">
-        <v>956.17105263157896</v>
+        <v>74.872340425531917</v>
       </c>
       <c r="P38" s="0">
-        <v>853.65789473684208</v>
+        <v>988.80851063829789</v>
       </c>
       <c r="Q38" s="0">
-        <v>16.292244897959183</v>
+        <v>22.093333333333337</v>
       </c>
       <c r="R38" s="0">
-        <v>16.292244897959183</v>
+        <v>22.093333333333337</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B39" s="0">
         <v>38</v>
       </c>
       <c r="C39" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D39" s="0">
-        <v>5.1413881748071972</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E39" s="0">
-        <v>128.53470437017992</v>
+        <v>655.0607287449393</v>
       </c>
       <c r="F39" s="0">
-        <v>56.55526992287917</v>
+        <v>549.79757085020242</v>
       </c>
       <c r="G39" s="0">
-        <v>2.2727272727272725</v>
+        <v>1.1914580265095729</v>
       </c>
       <c r="H39" s="0">
-        <v>184</v>
+        <v>192069</v>
       </c>
       <c r="I39" s="0">
-        <v>78.694497247566176</v>
+        <v>400.42090176160946</v>
       </c>
       <c r="J39" s="0">
-        <v>4863.8325149846996</v>
+        <v>125928.30565982067</v>
       </c>
       <c r="K39" s="0">
-        <v>36.027738188715752</v>
+        <v>213.97986317527509</v>
       </c>
       <c r="L39" s="0">
-        <v>340.77401726381083</v>
+        <v>5262.3481781376513</v>
       </c>
       <c r="M39" s="0">
-        <v>0.52632685240400412</v>
+        <v>0.057144451082816038</v>
       </c>
       <c r="N39" s="0">
-        <v>0.73877610121856274</v>
+        <v>0.078056031183731472</v>
       </c>
       <c r="O39" s="0">
-        <v>906.13586956521738</v>
+        <v>334.60025303406587</v>
       </c>
       <c r="P39" s="0">
-        <v>904.945652173913</v>
+        <v>549.71435265451476</v>
       </c>
       <c r="Q39" s="0">
-        <v>17.822119205298016</v>
+        <v>18.67084543494737</v>
       </c>
       <c r="R39" s="0">
-        <v>17.822119205298016</v>
+        <v>18.67084543494737</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B40" s="0">
         <v>39</v>
       </c>
       <c r="C40" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D40" s="0">
-        <v>5.1413881748071972</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E40" s="0">
-        <v>102.82776349614394</v>
+        <v>296.35627530364371</v>
       </c>
       <c r="F40" s="0">
-        <v>102.82776349614394</v>
+        <v>225.91093117408906</v>
       </c>
       <c r="G40" s="0">
-        <v>1</v>
+        <v>1.3118279569892473</v>
       </c>
       <c r="H40" s="0">
-        <v>241</v>
+        <v>49515</v>
       </c>
       <c r="I40" s="0">
-        <v>90.062495185661248</v>
+        <v>203.30894812087394</v>
       </c>
       <c r="J40" s="0">
-        <v>6370.5632397353947</v>
+        <v>32464.062679276823</v>
       </c>
       <c r="K40" s="0">
-        <v>36.647878549316559</v>
+        <v>82.37664240394102</v>
       </c>
       <c r="L40" s="0">
-        <v>364.29138591207442</v>
+        <v>1425.910931174089</v>
       </c>
       <c r="M40" s="0">
-        <v>0.60323966671249507</v>
+        <v>0.20064481230174325</v>
       </c>
       <c r="N40" s="0">
-        <v>0.50520470445139332</v>
+        <v>0.34676113050223306</v>
       </c>
       <c r="O40" s="0">
-        <v>313.02904564315355</v>
+        <v>839.21890336261743</v>
       </c>
       <c r="P40" s="0">
-        <v>946.93775933609959</v>
+        <v>468.30015146925172</v>
       </c>
       <c r="Q40" s="0">
-        <v>21.298928571428572</v>
+        <v>27.443156284639421</v>
       </c>
       <c r="R40" s="0">
-        <v>21.298928571428572</v>
+        <v>27.443156284639421</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B41" s="0">
         <v>40</v>
       </c>
       <c r="C41" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D41" s="0">
-        <v>5.1413881748071972</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E41" s="0">
-        <v>149.10025706940871</v>
+        <v>9.7165991902834001</v>
       </c>
       <c r="F41" s="0">
-        <v>143.95886889460152</v>
+        <v>6.4777327935222671</v>
       </c>
       <c r="G41" s="0">
-        <v>1.0357142857142856</v>
+        <v>1.5</v>
       </c>
       <c r="H41" s="0">
-        <v>233</v>
+        <v>110</v>
       </c>
       <c r="I41" s="0">
-        <v>88.555066631741425</v>
+        <v>9.5826239234059862</v>
       </c>
       <c r="J41" s="0">
-        <v>6159.0922608230167</v>
+        <v>72.120506810470573</v>
       </c>
       <c r="K41" s="0">
-        <v>58.744607538856201</v>
+        <v>3.5330940923602463</v>
       </c>
       <c r="L41" s="0">
-        <v>563.01959153749544</v>
+        <v>31.247639500791408</v>
       </c>
       <c r="M41" s="0">
-        <v>0.24416283502262645</v>
+        <v>0.92818426720588398</v>
       </c>
       <c r="N41" s="0">
-        <v>0.54410115979086737</v>
+        <v>0.18559147582963123</v>
       </c>
       <c r="O41" s="0">
-        <v>366</v>
+        <v>317.92727272727274</v>
       </c>
       <c r="P41" s="0">
-        <v>980.93562231759654</v>
+        <v>616.25454545454545</v>
       </c>
       <c r="Q41" s="0">
-        <v>16.173392857142858</v>
+        <v>6.851449106449107</v>
       </c>
       <c r="R41" s="0">
-        <v>16.173392857142858</v>
+        <v>6.851449106449107</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B42" s="0">
         <v>41</v>
       </c>
       <c r="C42" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D42" s="0">
-        <v>5.1413881748071972</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E42" s="0">
-        <v>87.403598971722346</v>
+        <v>10.526315789473683</v>
       </c>
       <c r="F42" s="0">
-        <v>66.838046272493557</v>
+        <v>8.9068825910931171</v>
       </c>
       <c r="G42" s="0">
-        <v>1.3076923076923077</v>
+        <v>1.1818181818181817</v>
       </c>
       <c r="H42" s="0">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="I42" s="0">
-        <v>69.85853193480456</v>
+        <v>9.4510484721611245</v>
       </c>
       <c r="J42" s="0">
-        <v>3832.9114927868559</v>
+        <v>70.15358389745775</v>
       </c>
       <c r="K42" s="0">
-        <v>28.272827179718881</v>
+        <v>3.7963541089374435</v>
       </c>
       <c r="L42" s="0">
-        <v>290.0898696682039</v>
+        <v>34.355278485492676</v>
       </c>
       <c r="M42" s="0">
-        <v>0.5723656065339523</v>
+        <v>0.74691774936711841</v>
       </c>
       <c r="N42" s="0">
-        <v>0.60520454577145244</v>
+        <v>0.20959681048385345</v>
       </c>
       <c r="O42" s="0">
-        <v>74.903448275862075</v>
+        <v>550.8878504672897</v>
       </c>
       <c r="P42" s="0">
-        <v>988.66896551724142</v>
+        <v>629.12149532710282</v>
       </c>
       <c r="Q42" s="0">
-        <v>21.763870967741941</v>
+        <v>3.3691803278688521</v>
       </c>
       <c r="R42" s="0">
-        <v>21.763870967741941</v>
+        <v>3.3691803278688521</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B43" s="0">
         <v>42</v>
       </c>
       <c r="C43" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D43" s="0">
         <v>0.80971659919028338</v>
       </c>
       <c r="E43" s="0">
-        <v>655.0607287449393</v>
+        <v>654.25101214574897</v>
       </c>
       <c r="F43" s="0">
-        <v>549.79757085020242</v>
+        <v>543.31983805668017</v>
       </c>
       <c r="G43" s="0">
-        <v>1.1914580265095729</v>
+        <v>1.2041728763040238</v>
       </c>
       <c r="H43" s="0">
-        <v>163513</v>
+        <v>145161</v>
       </c>
       <c r="I43" s="0">
-        <v>369.45729403159839</v>
+        <v>348.10725721732007</v>
       </c>
       <c r="J43" s="0">
-        <v>107205.82209182251</v>
+        <v>95173.498991952001</v>
       </c>
       <c r="K43" s="0">
-        <v>217.17205287513357</v>
+        <v>220.91077859704089</v>
       </c>
       <c r="L43" s="0">
-        <v>4319.0283400809712</v>
+        <v>3282.5910931174089</v>
       </c>
       <c r="M43" s="0">
-        <v>0.07221977449197195</v>
+        <v>0.1109921659928771</v>
       </c>
       <c r="N43" s="0">
-        <v>0.079064649180896091</v>
+        <v>0.29440532818941728</v>
       </c>
       <c r="O43" s="0">
-        <v>304.67187930011681</v>
+        <v>278.51236213583536</v>
       </c>
       <c r="P43" s="0">
-        <v>557.92740026786862</v>
+        <v>559.59487052307441</v>
       </c>
       <c r="Q43" s="0">
-        <v>24.730954227935221</v>
+        <v>7.9368686868686984</v>
       </c>
       <c r="R43" s="0">
-        <v>24.730954227935221</v>
+        <v>7.9368686868686984</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B44" s="0">
         <v>43</v>
       </c>
       <c r="C44" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D44" s="0">
         <v>0.80971659919028338</v>
       </c>
       <c r="E44" s="0">
-        <v>294.73684210526318</v>
+        <v>297.9757085020243</v>
       </c>
       <c r="F44" s="0">
-        <v>225.91093117408906</v>
+        <v>229.14979757085021</v>
       </c>
       <c r="G44" s="0">
-        <v>1.3046594982078854</v>
+        <v>1.3003533568904593</v>
       </c>
       <c r="H44" s="0">
-        <v>48982</v>
+        <v>53245</v>
       </c>
       <c r="I44" s="0">
-        <v>202.21173649401109</v>
+        <v>210.82762548739817</v>
       </c>
       <c r="J44" s="0">
-        <v>32114.606041731546</v>
+        <v>34909.60350112278</v>
       </c>
       <c r="K44" s="0">
-        <v>82.148678213641091</v>
+        <v>81.88225902940566</v>
       </c>
       <c r="L44" s="0">
-        <v>1443.7246963562752</v>
+        <v>1067.2064777327935</v>
       </c>
       <c r="M44" s="0">
-        <v>0.1936170913845259</v>
+        <v>0.385174808109009</v>
       </c>
       <c r="N44" s="0">
-        <v>0.34808276751752587</v>
+        <v>0.42393699746583402</v>
       </c>
       <c r="O44" s="0">
-        <v>839.79890572046872</v>
+        <v>840.35060569067514</v>
       </c>
       <c r="P44" s="0">
-        <v>468.26013637662817</v>
+        <v>467.51995492534508</v>
       </c>
       <c r="Q44" s="0">
-        <v>24.146762377434236</v>
+        <v>34.458660632949524</v>
       </c>
       <c r="R44" s="0">
-        <v>24.146762377434236</v>
+        <v>34.458660632949524</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B45" s="0">
         <v>44</v>
       </c>
       <c r="C45" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D45" s="0">
-        <v>0.80971659919028338</v>
+        <v>1.7421602787456445</v>
       </c>
       <c r="E45" s="0">
-        <v>13.765182186234817</v>
+        <v>670.73170731707319</v>
       </c>
       <c r="F45" s="0">
-        <v>9.7165991902834001</v>
+        <v>555.7491289198606</v>
       </c>
       <c r="G45" s="0">
-        <v>1.4166666666666667</v>
+        <v>1.2068965517241381</v>
       </c>
       <c r="H45" s="0">
-        <v>143</v>
+        <v>37579</v>
       </c>
       <c r="I45" s="0">
-        <v>10.925872305434591</v>
+        <v>381.0796664852175</v>
       </c>
       <c r="J45" s="0">
-        <v>93.756658853611754</v>
+        <v>114056.8660539766</v>
       </c>
       <c r="K45" s="0">
-        <v>4.6078411151648977</v>
+        <v>225.0478601637725</v>
       </c>
       <c r="L45" s="0">
-        <v>41.483073737632559</v>
+        <v>2653.3101045296166</v>
       </c>
       <c r="M45" s="0">
-        <v>0.68465239127023658</v>
+        <v>0.20358945342653759</v>
       </c>
       <c r="N45" s="0">
-        <v>0.21449099038796299</v>
+        <v>0.34481529184477416</v>
       </c>
       <c r="O45" s="0">
-        <v>611.91608391608395</v>
+        <v>463.32813539476837</v>
       </c>
       <c r="P45" s="0">
-        <v>385.26573426573424</v>
+        <v>614.99507703770723</v>
       </c>
       <c r="Q45" s="0">
-        <v>3.606153846153846</v>
+        <v>41.271183399933406</v>
       </c>
       <c r="R45" s="0">
-        <v>3.606153846153846</v>
+        <v>41.271183399933406</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B46" s="0">
         <v>45</v>
       </c>
       <c r="C46" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D46" s="0">
-        <v>0.80971659919028338</v>
+        <v>1.7421602787456445</v>
       </c>
       <c r="E46" s="0">
-        <v>7.2874493927125501</v>
+        <v>297.90940766550523</v>
       </c>
       <c r="F46" s="0">
-        <v>4.8582995951417001</v>
+        <v>238.67595818815329</v>
       </c>
       <c r="G46" s="0">
-        <v>1.5</v>
+        <v>1.248175182481752</v>
       </c>
       <c r="H46" s="0">
-        <v>64</v>
+        <v>13411</v>
       </c>
       <c r="I46" s="0">
-        <v>7.3093387342219431</v>
+        <v>227.65319415053173</v>
       </c>
       <c r="J46" s="0">
-        <v>41.961022144273791</v>
+        <v>40704.02700044919</v>
       </c>
       <c r="K46" s="0">
-        <v>2.6903795015324925</v>
+        <v>84.864612343631165</v>
       </c>
       <c r="L46" s="0">
-        <v>24.240962098350753</v>
+        <v>929.1036715137991</v>
       </c>
       <c r="M46" s="0">
-        <v>0.89733832716492301</v>
+        <v>0.59254165914542334</v>
       </c>
       <c r="N46" s="0">
-        <v>0.16234140673282249</v>
+        <v>0.43748629323283383</v>
       </c>
       <c r="O46" s="0">
-        <v>590.40625</v>
+        <v>728.28588472149727</v>
       </c>
       <c r="P46" s="0">
-        <v>413.828125</v>
+        <v>570.30542092312282</v>
       </c>
       <c r="Q46" s="0">
-        <v>3.4211518324607337</v>
+        <v>46.943796924862184</v>
       </c>
       <c r="R46" s="0">
-        <v>3.4211518324607337</v>
+        <v>46.943796924862184</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B47" s="0">
         <v>46</v>
       </c>
       <c r="C47" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D47" s="0">
-        <v>0.80971659919028338</v>
+        <v>2.9761904761904758</v>
       </c>
       <c r="E47" s="0">
-        <v>43.724696356275302</v>
+        <v>392.85714285714283</v>
       </c>
       <c r="F47" s="0">
-        <v>41.295546558704451</v>
+        <v>193.45238095238093</v>
       </c>
       <c r="G47" s="0">
-        <v>1.0588235294117647</v>
+        <v>2.0307692307692307</v>
       </c>
       <c r="H47" s="0">
-        <v>2001</v>
+        <v>4823</v>
       </c>
       <c r="I47" s="0">
-        <v>40.870659535586711</v>
+        <v>233.22463006850967</v>
       </c>
       <c r="J47" s="0">
-        <v>1311.9375829795601</v>
+        <v>42720.73412698412</v>
       </c>
       <c r="K47" s="0">
-        <v>14.752567359074037</v>
+        <v>112.81257441123842</v>
       </c>
       <c r="L47" s="0">
-        <v>142.0662584976717</v>
+        <v>1181.9188243279252</v>
       </c>
       <c r="M47" s="0">
-        <v>0.8168478149941597</v>
+        <v>0.38430255497135807</v>
       </c>
       <c r="N47" s="0">
-        <v>0.13794918832196859</v>
+        <v>0.2940384535503765</v>
       </c>
       <c r="O47" s="0">
-        <v>615.7256371814093</v>
+        <v>501.99274310595064</v>
       </c>
       <c r="P47" s="0">
-        <v>441.1934032983508</v>
+        <v>160.17934895293385</v>
       </c>
       <c r="Q47" s="0">
-        <v>20.357806947503811</v>
+        <v>54.549081601927142</v>
       </c>
       <c r="R47" s="0">
-        <v>20.357806947503811</v>
+        <v>54.549081601927142</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B48" s="0">
         <v>47</v>
       </c>
       <c r="C48" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D48" s="0">
-        <v>0.80971659919028338</v>
+        <v>2.9761904761904758</v>
       </c>
       <c r="E48" s="0">
-        <v>64.777327935222672</v>
+        <v>684.5238095238094</v>
       </c>
       <c r="F48" s="0">
-        <v>54.251012145748987</v>
+        <v>598.21428571428567</v>
       </c>
       <c r="G48" s="0">
-        <v>1.1940298507462688</v>
+        <v>1.144278606965174</v>
       </c>
       <c r="H48" s="0">
-        <v>2531</v>
+        <v>17089</v>
       </c>
       <c r="I48" s="0">
-        <v>45.965731332508845</v>
+        <v>439.00969055013411</v>
       </c>
       <c r="J48" s="0">
-        <v>1659.4272976118275</v>
+        <v>151369.4019274376</v>
       </c>
       <c r="K48" s="0">
-        <v>19.896059229984175</v>
+        <v>198.45004257694367</v>
       </c>
       <c r="L48" s="0">
-        <v>226.13977577639238</v>
+        <v>2594.7804094117705</v>
       </c>
       <c r="M48" s="0">
-        <v>0.40776897503621029</v>
+        <v>0.28251840019482732</v>
       </c>
       <c r="N48" s="0">
-        <v>0.03927862186894248</v>
+        <v>0.34923220730026111</v>
       </c>
       <c r="O48" s="0">
-        <v>387.29474516001579</v>
+        <v>596.41008836093397</v>
       </c>
       <c r="P48" s="0">
-        <v>478.47767680758591</v>
+        <v>291.65720639007549</v>
       </c>
       <c r="Q48" s="0">
-        <v>8.7264931100645349</v>
+        <v>53.893411552346606</v>
       </c>
       <c r="R48" s="0">
-        <v>8.7264931100645349</v>
+        <v>53.893411552346606</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B49" s="0">
         <v>48</v>
       </c>
       <c r="C49" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D49" s="0">
-        <v>0.80971659919028338</v>
+        <v>2.9761904761904758</v>
       </c>
       <c r="E49" s="0">
-        <v>19.4331983805668</v>
+        <v>68.452380952380949</v>
       </c>
       <c r="F49" s="0">
-        <v>13.765182186234817</v>
+        <v>65.476190476190467</v>
       </c>
       <c r="G49" s="0">
-        <v>1.4117647058823528</v>
+        <v>1.0454545454545456</v>
       </c>
       <c r="H49" s="0">
-        <v>235</v>
+        <v>310</v>
       </c>
       <c r="I49" s="0">
-        <v>14.006255127132793</v>
+        <v>59.128468290363145</v>
       </c>
       <c r="J49" s="0">
-        <v>154.07562818600533</v>
+        <v>2745.8900226757364</v>
       </c>
       <c r="K49" s="0">
-        <v>6.2606133730227294</v>
+        <v>23.69240440529801</v>
       </c>
       <c r="L49" s="0">
-        <v>56.126087085160393</v>
+        <v>223.71829968530756</v>
       </c>
       <c r="M49" s="0">
-        <v>0.61463074336104895</v>
+        <v>0.68942969166229773</v>
       </c>
       <c r="N49" s="0">
-        <v>0.18137388593670764</v>
+        <v>0.22096917280189901</v>
       </c>
       <c r="O49" s="0">
-        <v>637.77872340425529</v>
+        <v>509.54838709677421</v>
       </c>
       <c r="P49" s="0">
-        <v>510.54893617021276</v>
+        <v>240.81612903225806</v>
       </c>
       <c r="Q49" s="0">
-        <v>4.27871709952937</v>
+        <v>18.32516129032259</v>
       </c>
       <c r="R49" s="0">
-        <v>4.27871709952937</v>
+        <v>18.32516129032259</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B50" s="0">
         <v>49</v>
       </c>
       <c r="C50" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D50" s="0">
-        <v>0.80971659919028338</v>
+        <v>2.9761904761904758</v>
       </c>
       <c r="E50" s="0">
-        <v>21.862348178137651</v>
+        <v>675.59523809523796</v>
       </c>
       <c r="F50" s="0">
-        <v>17.004048582995949</v>
+        <v>547.61904761904759</v>
       </c>
       <c r="G50" s="0">
-        <v>1.2857142857142858</v>
+        <v>1.2336956521739129</v>
       </c>
       <c r="H50" s="0">
-        <v>323</v>
+        <v>12785</v>
       </c>
       <c r="I50" s="0">
-        <v>16.420612890275436</v>
+        <v>379.72233965321198</v>
       </c>
       <c r="J50" s="0">
-        <v>211.77203363438178</v>
+        <v>113245.81916099771</v>
       </c>
       <c r="K50" s="0">
-        <v>7.6219150844718291</v>
+        <v>223.68946868753591</v>
       </c>
       <c r="L50" s="0">
-        <v>65.754331676784005</v>
+        <v>2497.0238095238092</v>
       </c>
       <c r="M50" s="0">
-        <v>0.61550237803969166</v>
+        <v>0.22823732820100839</v>
       </c>
       <c r="N50" s="0">
-        <v>0.21895539815260376</v>
+        <v>0.19563852339345231</v>
       </c>
       <c r="O50" s="0">
-        <v>647.49226006191952</v>
+        <v>197.91615174032069</v>
       </c>
       <c r="P50" s="0">
-        <v>526.82352941176475</v>
+        <v>877.12139225655062</v>
       </c>
       <c r="Q50" s="0">
-        <v>5.509568480300187</v>
+        <v>48.470947562097535</v>
       </c>
       <c r="R50" s="0">
-        <v>5.509568480300187</v>
+        <v>48.470947562097535</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B51" s="0">
         <v>50</v>
       </c>
       <c r="C51" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D51" s="0">
-        <v>0.80971659919028338</v>
+        <v>2.9761904761904758</v>
       </c>
       <c r="E51" s="0">
-        <v>42.914979757085021</v>
+        <v>297.61904761904759</v>
       </c>
       <c r="F51" s="0">
-        <v>34.817813765182187</v>
+        <v>232.14285714285711</v>
       </c>
       <c r="G51" s="0">
-        <v>1.2325581395348837</v>
+        <v>1.2820512820512822</v>
       </c>
       <c r="H51" s="0">
-        <v>1189</v>
+        <v>4635</v>
       </c>
       <c r="I51" s="0">
-        <v>31.504966998740137</v>
+        <v>228.63391402089519</v>
       </c>
       <c r="J51" s="0">
-        <v>779.5571145240865</v>
+        <v>41055.484693877544</v>
       </c>
       <c r="K51" s="0">
-        <v>13.634917247023283</v>
+        <v>83.229709992887962</v>
       </c>
       <c r="L51" s="0">
-        <v>148.64416659434926</v>
+        <v>911.67841514443876</v>
       </c>
       <c r="M51" s="0">
-        <v>0.44336567022380335</v>
+        <v>0.62072280663394364</v>
       </c>
       <c r="N51" s="0">
-        <v>0.057270622432740725</v>
+        <v>0.26267497345821511</v>
       </c>
       <c r="O51" s="0">
-        <v>413.51303616484438</v>
+        <v>355.0314994606257</v>
       </c>
       <c r="P51" s="0">
-        <v>573.20689655172418</v>
+        <v>847.85911542610575</v>
       </c>
       <c r="Q51" s="0">
-        <v>8.5897260123481161</v>
+        <v>52.946815286624208</v>
       </c>
       <c r="R51" s="0">
-        <v>8.5897260123481161</v>
+        <v>52.946815286624208</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="B52" s="0">
         <v>51</v>
       </c>
       <c r="C52" s="0">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D52" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E52" s="0">
-        <v>27.530364372469634</v>
+        <v>1871.4652956298198</v>
       </c>
       <c r="F52" s="0">
-        <v>27.530364372469634</v>
+        <v>1048.8431876606683</v>
       </c>
       <c r="G52" s="0">
-        <v>1</v>
+        <v>1.784313725490196</v>
       </c>
       <c r="H52" s="0">
-        <v>835</v>
+        <v>26363</v>
       </c>
       <c r="I52" s="0">
-        <v>26.401666416062792</v>
+        <v>941.96088374734722</v>
       </c>
       <c r="J52" s="0">
-        <v>547.46021078857211</v>
+        <v>696876.17713337846</v>
       </c>
       <c r="K52" s="0">
-        <v>9.488709675040262</v>
+        <v>505.22297357936441</v>
       </c>
       <c r="L52" s="0">
-        <v>90.33104487605425</v>
+        <v>7017.9948586118244</v>
       </c>
       <c r="M52" s="0">
-        <v>0.843117991004391</v>
+        <v>0.17780312549818236</v>
       </c>
       <c r="N52" s="0">
-        <v>0.20268882042338901</v>
+        <v>0.23317125491670873</v>
       </c>
       <c r="O52" s="0">
-        <v>640.5880239520958</v>
+        <v>590.53347494594698</v>
       </c>
       <c r="P52" s="0">
-        <v>593.11616766467068</v>
+        <v>186.15756932063877</v>
       </c>
       <c r="Q52" s="0">
-        <v>13.278102546215557</v>
+        <v>45.02266666666678</v>
       </c>
       <c r="R52" s="0">
-        <v>13.278102546215557</v>
+        <v>45.02266666666678</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="B53" s="0">
         <v>52</v>
       </c>
       <c r="C53" s="0">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D53" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E53" s="0">
-        <v>8.9068825910931171</v>
+        <v>503.85604113110531</v>
       </c>
       <c r="F53" s="0">
-        <v>6.4777327935222671</v>
+        <v>395.88688946015418</v>
       </c>
       <c r="G53" s="0">
-        <v>1.375</v>
+        <v>1.2727272727272727</v>
       </c>
       <c r="H53" s="0">
-        <v>98</v>
+        <v>4177</v>
       </c>
       <c r="I53" s="0">
-        <v>9.0448452236762051</v>
+        <v>374.94510770684064</v>
       </c>
       <c r="J53" s="0">
-        <v>64.252815158419239</v>
+        <v>110414.2848646255</v>
       </c>
       <c r="K53" s="0">
-        <v>3.3492448158159767</v>
+        <v>147.40189220926868</v>
       </c>
       <c r="L53" s="0">
-        <v>29.209894652755953</v>
+        <v>1501.2853470437017</v>
       </c>
       <c r="M53" s="0">
-        <v>0.94632876914591868</v>
+        <v>0.61561421064198563</v>
       </c>
       <c r="N53" s="0">
-        <v>0.20293071568774917</v>
+        <v>0.2562505337488174</v>
       </c>
       <c r="O53" s="0">
-        <v>318.18367346938777</v>
+        <v>491.09265022743597</v>
       </c>
       <c r="P53" s="0">
-        <v>616.42857142857144</v>
+        <v>270.70457265980366</v>
       </c>
       <c r="Q53" s="0">
-        <v>6.1413027963027957</v>
+        <v>42.573202614379085</v>
       </c>
       <c r="R53" s="0">
-        <v>6.1413027963027957</v>
+        <v>42.573202614379085</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B54" s="0">
         <v>53</v>
       </c>
       <c r="C54" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D54" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E54" s="0">
-        <v>654.25101214574897</v>
+        <v>215.93830334190227</v>
       </c>
       <c r="F54" s="0">
-        <v>544.12955465587038</v>
+        <v>205.65552699228789</v>
       </c>
       <c r="G54" s="0">
-        <v>1.2023809523809526</v>
+        <v>1.0499999999999998</v>
       </c>
       <c r="H54" s="0">
-        <v>146219</v>
+        <v>1264</v>
       </c>
       <c r="I54" s="0">
-        <v>349.37353683909669</v>
+        <v>206.25713961117836</v>
       </c>
       <c r="J54" s="0">
-        <v>95867.167139274519</v>
+        <v>33412.414668155761</v>
       </c>
       <c r="K54" s="0">
-        <v>220.78859353475929</v>
+        <v>74.319259946128739</v>
       </c>
       <c r="L54" s="0">
-        <v>3279.3522267206476</v>
+        <v>791.77377892030836</v>
       </c>
       <c r="M54" s="0">
-        <v>0.11202207863807245</v>
+        <v>0.66975427797900122</v>
       </c>
       <c r="N54" s="0">
-        <v>0.2926145515627096</v>
+        <v>0.2861826415416957</v>
       </c>
       <c r="O54" s="0">
-        <v>279.2530040555605</v>
+        <v>702.76265822784808</v>
       </c>
       <c r="P54" s="0">
-        <v>558.94948672881094</v>
+        <v>347.16218354430379</v>
       </c>
       <c r="Q54" s="0">
-        <v>29.707277124625673</v>
+        <v>31.585030674846632</v>
       </c>
       <c r="R54" s="0">
-        <v>29.707277124625673</v>
+        <v>31.585030674846632</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B55" s="0">
         <v>54</v>
       </c>
       <c r="C55" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D55" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E55" s="0">
-        <v>298.78542510121457</v>
+        <v>169.6658097686375</v>
       </c>
       <c r="F55" s="0">
-        <v>229.95951417004048</v>
+        <v>169.6658097686375</v>
       </c>
       <c r="G55" s="0">
-        <v>1.2992957746478873</v>
+        <v>1</v>
       </c>
       <c r="H55" s="0">
-        <v>53508</v>
+        <v>793</v>
       </c>
       <c r="I55" s="0">
-        <v>211.34766834687582</v>
+        <v>163.36990154312042</v>
       </c>
       <c r="J55" s="0">
-        <v>35082.037076496905</v>
+        <v>20962.060784689496</v>
       </c>
       <c r="K55" s="0">
-        <v>82.073015717623676</v>
+        <v>59.355532509816683</v>
       </c>
       <c r="L55" s="0">
-        <v>1071.2550607287449</v>
+        <v>586.11825192802053</v>
       </c>
       <c r="M55" s="0">
-        <v>0.38415712636488947</v>
+        <v>0.76678454118088823</v>
       </c>
       <c r="N55" s="0">
-        <v>0.42258142935927046</v>
+        <v>0.27808454190577137</v>
       </c>
       <c r="O55" s="0">
-        <v>840.30230993496298</v>
+        <v>740.79823455233293</v>
       </c>
       <c r="P55" s="0">
-        <v>467.42530088958659</v>
+        <v>410.58511979823453</v>
       </c>
       <c r="Q55" s="0">
-        <v>39.232092288918146</v>
+        <v>32.477377049180333</v>
       </c>
       <c r="R55" s="0">
-        <v>39.232092288918146</v>
+        <v>32.477377049180333</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B56" s="0">
         <v>55</v>
       </c>
       <c r="C56" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D56" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E56" s="0">
-        <v>24.291497975708502</v>
+        <v>1280.2056555269921</v>
       </c>
       <c r="F56" s="0">
-        <v>22.672064777327936</v>
+        <v>791.77377892030836</v>
       </c>
       <c r="G56" s="0">
-        <v>1.0714285714285714</v>
+        <v>1.616883116883117</v>
       </c>
       <c r="H56" s="0">
-        <v>413</v>
+        <v>16357</v>
       </c>
       <c r="I56" s="0">
-        <v>18.567914495739377</v>
+        <v>741.97159679904701</v>
       </c>
       <c r="J56" s="0">
-        <v>270.77972102476679</v>
+        <v>432378.85025872139</v>
       </c>
       <c r="K56" s="0">
-        <v>8.7813741916498138</v>
+        <v>373.34943259033338</v>
       </c>
       <c r="L56" s="0">
-        <v>80.817594310480246</v>
+        <v>4812.339331619537</v>
       </c>
       <c r="M56" s="0">
-        <v>0.52097173683925491</v>
+        <v>0.23461826573694317</v>
       </c>
       <c r="N56" s="0">
-        <v>0.12515201032526607</v>
+        <v>0.32558002009820936</v>
       </c>
       <c r="O56" s="0">
-        <v>498.87167070217919</v>
+        <v>782.87155346334907</v>
       </c>
       <c r="P56" s="0">
-        <v>385.58353510895881</v>
+        <v>512.71675735159261</v>
       </c>
       <c r="Q56" s="0">
-        <v>5.6164446775039325</v>
+        <v>54.96145454527057</v>
       </c>
       <c r="R56" s="0">
-        <v>5.6164446775039325</v>
+        <v>54.96145454527057</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B57" s="0">
         <v>56</v>
       </c>
       <c r="C57" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D57" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E57" s="0">
-        <v>8.9068825910931171</v>
+        <v>478.14910025706934</v>
       </c>
       <c r="F57" s="0">
-        <v>4.048582995951417</v>
+        <v>370.1799485861182</v>
       </c>
       <c r="G57" s="0">
-        <v>2.1999999999999997</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="H57" s="0">
-        <v>66</v>
+        <v>3462</v>
       </c>
       <c r="I57" s="0">
-        <v>7.4226685736640334</v>
+        <v>341.349275506786</v>
       </c>
       <c r="J57" s="0">
-        <v>43.272304086282347</v>
+        <v>91514.066124331686</v>
       </c>
       <c r="K57" s="0">
-        <v>3.0318175798172762</v>
+        <v>139.03513006514936</v>
       </c>
       <c r="L57" s="0">
-        <v>25.360378764421885</v>
+        <v>2123.3933161953723</v>
       </c>
       <c r="M57" s="0">
-        <v>0.84548987904777673</v>
+        <v>0.25505675161906005</v>
       </c>
       <c r="N57" s="0">
-        <v>0.12830467489446123</v>
+        <v>0.25011937640526977</v>
       </c>
       <c r="O57" s="0">
-        <v>479.68181818181819</v>
+        <v>418.72848064702487</v>
       </c>
       <c r="P57" s="0">
-        <v>380.34848484848487</v>
+        <v>778.8021374927788</v>
       </c>
       <c r="Q57" s="0">
-        <v>3.5440672268907574</v>
+        <v>21.963066954643633</v>
       </c>
       <c r="R57" s="0">
-        <v>3.5440672268907574</v>
+        <v>21.963066954643633</v>
       </c>
     </row>
     <row r="58">

</xml_diff>

<commit_message>
Add some debugging tools for identifying aggregates.
</commit_message>
<xml_diff>
--- a/processed/test_1/kmeans/process_results.xlsx
+++ b/processed/test_1/kmeans/process_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="154">
   <si>
     <t>fname</t>
   </si>
@@ -190,6 +190,84 @@
   </si>
   <si>
     <t>test_image_1.tif</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>img_id</t>
+  </si>
+  <si>
+    <t>pixsize</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>aspect_ratio</t>
+  </si>
+  <si>
+    <t>num_pixels</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Rg</t>
+  </si>
+  <si>
+    <t>perimeter</t>
+  </si>
+  <si>
+    <t>circularity</t>
+  </si>
+  <si>
+    <t>zbar_opt</t>
+  </si>
+  <si>
+    <t>center_mass_1</t>
+  </si>
+  <si>
+    <t>center_mass_2</t>
+  </si>
+  <si>
+    <t>dp_pcm</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0014.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0015.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0019.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0021.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0022.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0023.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0024.tif</t>
+  </si>
+  <si>
+    <t>c3_343a_2322K_4.6atm_0025.tif</t>
   </si>
   <si>
     <t>id</t>
@@ -417,7 +495,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -431,11 +509,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -443,6 +522,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,63 +557,63 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
@@ -554,42 +634,42 @@
         <v>1.0166666666666666</v>
       </c>
       <c r="H2" s="0">
-        <v>28013</v>
+        <v>27967</v>
       </c>
       <c r="I2" s="0">
-        <v>152.92127570819702</v>
+        <v>152.79566851091221</v>
       </c>
       <c r="J2" s="0">
-        <v>18366.470520742838</v>
+        <v>18336.311036076644</v>
       </c>
       <c r="K2" s="0">
-        <v>61.68864806593723</v>
+        <v>61.644948794860397</v>
       </c>
       <c r="L2" s="0">
-        <v>818.19163370818626</v>
+        <v>821.40532226598953</v>
       </c>
       <c r="M2" s="0">
-        <v>0.34476685035677906</v>
+        <v>0.34151265876320092</v>
       </c>
       <c r="N2" s="0">
-        <v>0.23429733827134921</v>
+        <v>0.23481210026116844</v>
       </c>
       <c r="O2" s="0">
-        <v>462.26448434655339</v>
+        <v>462.30131941216433</v>
       </c>
       <c r="P2" s="0">
-        <v>155.41894834541105</v>
+        <v>155.39618121357313</v>
       </c>
       <c r="Q2" s="0">
-        <v>29.332843439016941</v>
+        <v>26.554859298682857</v>
       </c>
       <c r="R2" s="0">
-        <v>29.332843439016941</v>
+        <v>26.554859298682857</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="B3" s="0">
         <v>2</v>
@@ -610,42 +690,42 @@
         <v>1.6968215158924207</v>
       </c>
       <c r="H3" s="0">
-        <v>110943</v>
+        <v>111070</v>
       </c>
       <c r="I3" s="0">
-        <v>304.32529693111678</v>
+        <v>304.49943256049619</v>
       </c>
       <c r="J3" s="0">
-        <v>72738.776246127614</v>
+        <v>72822.042649445153</v>
       </c>
       <c r="K3" s="0">
-        <v>146.00977607846761</v>
+        <v>146.02530383864928</v>
       </c>
       <c r="L3" s="0">
-        <v>2722.2672064777325</v>
+        <v>2709.3117408906883</v>
       </c>
       <c r="M3" s="0">
-        <v>0.1233429556736088</v>
+        <v>0.12466793406843056</v>
       </c>
       <c r="N3" s="0">
-        <v>0.25374215872483774</v>
+        <v>0.25330900624069869</v>
       </c>
       <c r="O3" s="0">
-        <v>435.71453809613945</v>
+        <v>435.61033582425495</v>
       </c>
       <c r="P3" s="0">
-        <v>548.45382764122121</v>
+        <v>548.53974070406048</v>
       </c>
       <c r="Q3" s="0">
-        <v>24.1943710687502</v>
+        <v>37.523467975474439</v>
       </c>
       <c r="R3" s="0">
-        <v>24.1943710687502</v>
+        <v>37.523467975474439</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="B4" s="0">
         <v>3</v>
@@ -666,42 +746,42 @@
         <v>1.3883928571428572</v>
       </c>
       <c r="H4" s="0">
-        <v>43902</v>
+        <v>43917</v>
       </c>
       <c r="I4" s="0">
-        <v>191.43892832402935</v>
+        <v>191.47163000827126</v>
       </c>
       <c r="J4" s="0">
-        <v>28783.949909029812</v>
+        <v>28793.784523594877</v>
       </c>
       <c r="K4" s="0">
-        <v>73.575232766156148</v>
+        <v>73.609072169929476</v>
       </c>
       <c r="L4" s="0">
-        <v>777.69400289441</v>
+        <v>776.46008676153849</v>
       </c>
       <c r="M4" s="0">
-        <v>0.59805724286997441</v>
+        <v>0.60016455384800682</v>
       </c>
       <c r="N4" s="0">
-        <v>0.41015744342683302</v>
+        <v>0.41002063633257901</v>
       </c>
       <c r="O4" s="0">
-        <v>730.42729260625936</v>
+        <v>730.35596693763239</v>
       </c>
       <c r="P4" s="0">
-        <v>895.49813220354429</v>
+        <v>895.52123323542139</v>
       </c>
       <c r="Q4" s="0">
-        <v>43.256633425945189</v>
+        <v>55.355852855521604</v>
       </c>
       <c r="R4" s="0">
-        <v>43.256633425945189</v>
+        <v>55.355852855521604</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="B5" s="0">
         <v>4</v>
@@ -722,42 +802,42 @@
         <v>1.0379746835443038</v>
       </c>
       <c r="H5" s="0">
-        <v>27534</v>
+        <v>27517</v>
       </c>
       <c r="I5" s="0">
-        <v>151.60822242459957</v>
+        <v>151.5614123401881</v>
       </c>
       <c r="J5" s="0">
-        <v>18052.418495631791</v>
+        <v>18041.272599124717</v>
       </c>
       <c r="K5" s="0">
-        <v>62.357238312590795</v>
+        <v>62.330545737801749</v>
       </c>
       <c r="L5" s="0">
-        <v>903.96888124372549</v>
+        <v>902.73878144783043</v>
       </c>
       <c r="M5" s="0">
-        <v>0.27761203921462169</v>
+        <v>0.27819724994853329</v>
       </c>
       <c r="N5" s="0">
-        <v>0.11730515159962532</v>
+        <v>0.11749969436458078</v>
       </c>
       <c r="O5" s="0">
-        <v>411.66732040386432</v>
+        <v>411.71592106697676</v>
       </c>
       <c r="P5" s="0">
-        <v>170.64680031960486</v>
+        <v>170.74383108623761</v>
       </c>
       <c r="Q5" s="0">
-        <v>26.17763581495549</v>
+        <v>30.895619715696931</v>
       </c>
       <c r="R5" s="0">
-        <v>26.17763581495549</v>
+        <v>30.895619715696931</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="B6" s="0">
         <v>5</v>
@@ -769,51 +849,51 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E6" s="0">
-        <v>589.47368421052636</v>
+        <v>9.7165991902834001</v>
       </c>
       <c r="F6" s="0">
-        <v>446.9635627530364</v>
+        <v>5.668016194331984</v>
       </c>
       <c r="G6" s="0">
-        <v>1.3188405797101452</v>
+        <v>1.7142857142857142</v>
       </c>
       <c r="H6" s="0">
-        <v>205707</v>
+        <v>82</v>
       </c>
       <c r="I6" s="0">
-        <v>414.39321600079228</v>
+        <v>8.2736096679356947</v>
       </c>
       <c r="J6" s="0">
-        <v>134869.93722237702</v>
+        <v>53.762559622350793</v>
       </c>
       <c r="K6" s="0">
-        <v>167.16022959179074</v>
+        <v>3.2951857526882415</v>
       </c>
       <c r="L6" s="0">
-        <v>3967.6113360323884</v>
+        <v>28.471193657085877</v>
       </c>
       <c r="M6" s="0">
-        <v>0.10766307371795013</v>
+        <v>0.83344788818044324</v>
       </c>
       <c r="N6" s="0">
-        <v>0.11752253958138303</v>
+        <v>0.15468091183897834</v>
       </c>
       <c r="O6" s="0">
-        <v>492.40452196570851</v>
+        <v>634.20731707317077</v>
       </c>
       <c r="P6" s="0">
-        <v>552.11559645515229</v>
+        <v>155.28048780487805</v>
       </c>
       <c r="Q6" s="0">
-        <v>19.404544921390041</v>
+        <v>4.5733063861966023</v>
       </c>
       <c r="R6" s="0">
-        <v>19.404544921390041</v>
+        <v>4.5733063861966023</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="B7" s="0">
         <v>6</v>
@@ -825,51 +905,51 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E7" s="0">
-        <v>9.7165991902834001</v>
+        <v>589.47368421052636</v>
       </c>
       <c r="F7" s="0">
-        <v>9.7165991902834001</v>
+        <v>446.9635627530364</v>
       </c>
       <c r="G7" s="0">
-        <v>1</v>
+        <v>1.3188405797101452</v>
       </c>
       <c r="H7" s="0">
-        <v>154</v>
+        <v>205725</v>
       </c>
       <c r="I7" s="0">
-        <v>11.338313532461777</v>
+        <v>414.41134594951075</v>
       </c>
       <c r="J7" s="0">
-        <v>100.96870953465881</v>
+        <v>134881.7387598551</v>
       </c>
       <c r="K7" s="0">
-        <v>4.1016068710001647</v>
+        <v>167.23172825899346</v>
       </c>
       <c r="L7" s="0">
-        <v>35.627530364372468</v>
+        <v>3968.4210526315787</v>
       </c>
       <c r="M7" s="0">
-        <v>0.99959766250584337</v>
+        <v>0.10762856006338441</v>
       </c>
       <c r="N7" s="0">
-        <v>0.068597646237994137</v>
+        <v>0.11753416730411036</v>
       </c>
       <c r="O7" s="0">
-        <v>277.25974025974028</v>
+        <v>492.47779317049458</v>
       </c>
       <c r="P7" s="0">
-        <v>318.11688311688312</v>
+        <v>551.78092113257992</v>
       </c>
       <c r="Q7" s="0">
-        <v>7.2763285940585716</v>
+        <v>47.964818747623553</v>
       </c>
       <c r="R7" s="0">
-        <v>7.2763285940585716</v>
+        <v>47.964818747623553</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="B8" s="0">
         <v>7</v>
@@ -881,51 +961,51 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E8" s="0">
-        <v>320.64777327935224</v>
+        <v>9.7165991902834001</v>
       </c>
       <c r="F8" s="0">
-        <v>180.56680161943319</v>
+        <v>9.7165991902834001</v>
       </c>
       <c r="G8" s="0">
-        <v>1.7757847533632287</v>
+        <v>1</v>
       </c>
       <c r="H8" s="0">
-        <v>47377</v>
+        <v>154</v>
       </c>
       <c r="I8" s="0">
-        <v>198.87119353384566</v>
+        <v>11.338313532461777</v>
       </c>
       <c r="J8" s="0">
-        <v>31062.302283269677</v>
+        <v>100.96870953465881</v>
       </c>
       <c r="K8" s="0">
-        <v>88.704127092473342</v>
+        <v>4.1016068710001647</v>
       </c>
       <c r="L8" s="0">
-        <v>1340.080971659919</v>
+        <v>35.627530364372468</v>
       </c>
       <c r="M8" s="0">
-        <v>0.21736090053814569</v>
+        <v>0.99959766250584337</v>
       </c>
       <c r="N8" s="0">
-        <v>0.25356125302901139</v>
+        <v>0.068580865385264603</v>
       </c>
       <c r="O8" s="0">
-        <v>652.47573717204546</v>
+        <v>277.25974025974028</v>
       </c>
       <c r="P8" s="0">
-        <v>911.01393081030881</v>
+        <v>318.11688311688312</v>
       </c>
       <c r="Q8" s="0">
-        <v>23.489889801609994</v>
+        <v>7.2763285940585716</v>
       </c>
       <c r="R8" s="0">
-        <v>23.489889801609994</v>
+        <v>7.2763285940585716</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="B9" s="0">
         <v>8</v>
@@ -937,107 +1017,107 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E9" s="0">
-        <v>8.9068825910931171</v>
+        <v>320.64777327935224</v>
       </c>
       <c r="F9" s="0">
-        <v>7.2874493927125501</v>
+        <v>180.56680161943319</v>
       </c>
       <c r="G9" s="0">
-        <v>1.2222222222222223</v>
+        <v>1.7757847533632287</v>
       </c>
       <c r="H9" s="0">
-        <v>97</v>
+        <v>47248</v>
       </c>
       <c r="I9" s="0">
-        <v>8.9985797273140324</v>
+        <v>198.60026174227886</v>
       </c>
       <c r="J9" s="0">
-        <v>63.597174187414964</v>
+        <v>30977.724598010125</v>
       </c>
       <c r="K9" s="0">
-        <v>3.3095235543022978</v>
+        <v>88.473630108936746</v>
       </c>
       <c r="L9" s="0">
-        <v>30.587757655576251</v>
+        <v>1319.8380566801618</v>
       </c>
       <c r="M9" s="0">
-        <v>0.85418590693116558</v>
+        <v>0.22346941126397013</v>
       </c>
       <c r="N9" s="0">
-        <v>0.30340462727369194</v>
+        <v>0.25387887986623947</v>
       </c>
       <c r="O9" s="0">
-        <v>174.32989690721649</v>
+        <v>653.01693193362678</v>
       </c>
       <c r="P9" s="0">
-        <v>948.2268041237113</v>
+        <v>911.0500550287843</v>
       </c>
       <c r="Q9" s="0">
-        <v>5.6733323347712918</v>
+        <v>28.661386386048282</v>
       </c>
       <c r="R9" s="0">
-        <v>5.6733323347712918</v>
+        <v>28.661386386048282</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B10" s="0">
         <v>9</v>
       </c>
       <c r="C10" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D10" s="0">
-        <v>5.1413881748071972</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E10" s="0">
-        <v>370.1799485861182</v>
+        <v>8.9068825910931171</v>
       </c>
       <c r="F10" s="0">
-        <v>303.34190231362464</v>
+        <v>7.2874493927125501</v>
       </c>
       <c r="G10" s="0">
-        <v>1.2203389830508475</v>
+        <v>1.2222222222222223</v>
       </c>
       <c r="H10" s="0">
-        <v>3106</v>
+        <v>97</v>
       </c>
       <c r="I10" s="0">
-        <v>323.32268697740017</v>
+        <v>8.9985797273140324</v>
       </c>
       <c r="J10" s="0">
-        <v>82103.60756273086</v>
+        <v>63.597174187414964</v>
       </c>
       <c r="K10" s="0">
-        <v>117.00625334557238</v>
+        <v>3.316632540151419</v>
       </c>
       <c r="L10" s="0">
-        <v>1188.4561326159242</v>
+        <v>30.756701122425039</v>
       </c>
       <c r="M10" s="0">
-        <v>0.73047573160390833</v>
+        <v>0.84482776477470045</v>
       </c>
       <c r="N10" s="0">
-        <v>0.32867925906731715</v>
+        <v>0.30296370263390121</v>
       </c>
       <c r="O10" s="0">
-        <v>527.25273663876374</v>
+        <v>174.24742268041237</v>
       </c>
       <c r="P10" s="0">
-        <v>83.445267224726337</v>
+        <v>948.1649484536083</v>
       </c>
       <c r="Q10" s="0">
-        <v>92.628</v>
+        <v>5.628993175850848</v>
       </c>
       <c r="R10" s="0">
-        <v>92.628</v>
+        <v>5.628993175850848</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B11" s="0">
         <v>10</v>
@@ -1049,51 +1129,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E11" s="0">
-        <v>185.0899742930591</v>
+        <v>370.1799485861182</v>
       </c>
       <c r="F11" s="0">
-        <v>185.0899742930591</v>
+        <v>303.34190231362464</v>
       </c>
       <c r="G11" s="0">
-        <v>1</v>
+        <v>1.2203389830508475</v>
       </c>
       <c r="H11" s="0">
-        <v>803</v>
+        <v>3122</v>
       </c>
       <c r="I11" s="0">
-        <v>164.39674950056869</v>
+        <v>324.15438658163504</v>
       </c>
       <c r="J11" s="0">
-        <v>21226.399508329967</v>
+        <v>82526.549520555622</v>
       </c>
       <c r="K11" s="0">
-        <v>60.886290468595696</v>
+        <v>117.27417272934851</v>
       </c>
       <c r="L11" s="0">
-        <v>676.79826428394699</v>
+        <v>1186.9836573465645</v>
       </c>
       <c r="M11" s="0">
-        <v>0.58232807074475335</v>
+        <v>0.73606144912844829</v>
       </c>
       <c r="N11" s="0">
-        <v>0.20055010808409643</v>
+        <v>0.32616119829612855</v>
       </c>
       <c r="O11" s="0">
-        <v>331.05603985056041</v>
+        <v>527.36386931454194</v>
       </c>
       <c r="P11" s="0">
-        <v>84.66874221668742</v>
+        <v>83.396540679051895</v>
       </c>
       <c r="Q11" s="0">
-        <v>30.328235294117654</v>
+        <v>96.246495726495681</v>
       </c>
       <c r="R11" s="0">
-        <v>30.328235294117654</v>
+        <v>96.246495726495681</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B12" s="0">
         <v>11</v>
@@ -1105,51 +1185,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E12" s="0">
-        <v>267.35218508997423</v>
+        <v>185.0899742930591</v>
       </c>
       <c r="F12" s="0">
-        <v>241.64524421593828</v>
+        <v>179.94858611825191</v>
       </c>
       <c r="G12" s="0">
-        <v>1.1063829787234041</v>
+        <v>1.0285714285714285</v>
       </c>
       <c r="H12" s="0">
-        <v>1670</v>
+        <v>790</v>
       </c>
       <c r="I12" s="0">
-        <v>237.07932890917806</v>
+        <v>163.06058621066498</v>
       </c>
       <c r="J12" s="0">
-        <v>44144.566847958959</v>
+        <v>20882.759167597353</v>
       </c>
       <c r="K12" s="0">
-        <v>86.066889054668607</v>
+        <v>60.417515151913165</v>
       </c>
       <c r="L12" s="0">
-        <v>934.96654015954982</v>
+        <v>669.33868289180589</v>
       </c>
       <c r="M12" s="0">
-        <v>0.63459257434447647</v>
+        <v>0.58574136430000745</v>
       </c>
       <c r="N12" s="0">
-        <v>0.48760387044873588</v>
+        <v>0.20187916677220974</v>
       </c>
       <c r="O12" s="0">
-        <v>888.33652694610782</v>
+        <v>330.97341772151901</v>
       </c>
       <c r="P12" s="0">
-        <v>114.3497005988024</v>
+        <v>84.756962025316454</v>
       </c>
       <c r="Q12" s="0">
-        <v>58.558730158730164</v>
+        <v>31.403999999999996</v>
       </c>
       <c r="R12" s="0">
-        <v>58.558730158730164</v>
+        <v>31.403999999999996</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B13" s="0">
         <v>12</v>
@@ -1161,51 +1241,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E13" s="0">
-        <v>107.96915167095113</v>
+        <v>267.35218508997423</v>
       </c>
       <c r="F13" s="0">
-        <v>46.272493573264775</v>
+        <v>236.50385604113109</v>
       </c>
       <c r="G13" s="0">
-        <v>2.333333333333333</v>
+        <v>1.1304347826086956</v>
       </c>
       <c r="H13" s="0">
-        <v>123</v>
+        <v>1611</v>
       </c>
       <c r="I13" s="0">
-        <v>64.341030055242328</v>
+        <v>232.85374326125273</v>
       </c>
       <c r="J13" s="0">
-        <v>3251.3663007778159</v>
+        <v>42584.968378480175</v>
       </c>
       <c r="K13" s="0">
-        <v>33.32786835185837</v>
+        <v>84.984592744685813</v>
       </c>
       <c r="L13" s="0">
-        <v>306.93273191401573</v>
+        <v>960.05687728314376</v>
       </c>
       <c r="M13" s="0">
-        <v>0.43369993223293818</v>
+        <v>0.58059363063903624</v>
       </c>
       <c r="N13" s="0">
-        <v>0.46280204292068094</v>
+        <v>0.50410944703458993</v>
       </c>
       <c r="O13" s="0">
-        <v>841.48780487804879</v>
+        <v>887.665425201738</v>
       </c>
       <c r="P13" s="0">
-        <v>113.04878048780488</v>
+        <v>114.56486654252018</v>
       </c>
       <c r="Q13" s="0">
-        <v>18.758305084745757</v>
+        <v>42.774110032362486</v>
       </c>
       <c r="R13" s="0">
-        <v>18.758305084745757</v>
+        <v>42.774110032362486</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B14" s="0">
         <v>13</v>
@@ -1217,51 +1297,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E14" s="0">
-        <v>174.80719794344469</v>
+        <v>107.96915167095113</v>
       </c>
       <c r="F14" s="0">
-        <v>143.95886889460152</v>
+        <v>46.272493573264775</v>
       </c>
       <c r="G14" s="0">
-        <v>1.2142857142857142</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="H14" s="0">
-        <v>409</v>
+        <v>124</v>
       </c>
       <c r="I14" s="0">
-        <v>117.32676808931656</v>
+        <v>64.602049504516373</v>
       </c>
       <c r="J14" s="0">
-        <v>10811.453796895339</v>
+        <v>3277.8001731418631</v>
       </c>
       <c r="K14" s="0">
-        <v>60.080195435199386</v>
+        <v>33.573585372692953</v>
       </c>
       <c r="L14" s="0">
-        <v>622.10243400785157</v>
+        <v>301.27857000841669</v>
       </c>
       <c r="M14" s="0">
-        <v>0.35105095563587979</v>
+        <v>0.45379097583997008</v>
       </c>
       <c r="N14" s="0">
-        <v>0.4624967341480769</v>
+        <v>0.46239807090737722</v>
       </c>
       <c r="O14" s="0">
-        <v>999.24205378973102</v>
+        <v>841.48387096774195</v>
       </c>
       <c r="P14" s="0">
-        <v>125.44987775061125</v>
+        <v>112.94354838709677</v>
       </c>
       <c r="Q14" s="0">
-        <v>27.00433734939757</v>
+        <v>20.28142857142857</v>
       </c>
       <c r="R14" s="0">
-        <v>27.00433734939757</v>
+        <v>20.28142857142857</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B15" s="0">
         <v>14</v>
@@ -1273,51 +1353,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E15" s="0">
-        <v>61.696658097686367</v>
+        <v>174.80719794344469</v>
       </c>
       <c r="F15" s="0">
-        <v>41.131105398457578</v>
+        <v>143.95886889460152</v>
       </c>
       <c r="G15" s="0">
-        <v>1.5</v>
+        <v>1.2142857142857142</v>
       </c>
       <c r="H15" s="0">
-        <v>67</v>
+        <v>458</v>
       </c>
       <c r="I15" s="0">
-        <v>47.486794566109914</v>
+        <v>124.15613734080659</v>
       </c>
       <c r="J15" s="0">
-        <v>1771.069448391168</v>
+        <v>12106.713542733654</v>
       </c>
       <c r="K15" s="0">
-        <v>18.476925843710998</v>
+        <v>60.159730078298168</v>
       </c>
       <c r="L15" s="0">
-        <v>185.76273157048769</v>
+        <v>666.91145534683733</v>
       </c>
       <c r="M15" s="0">
-        <v>0.64495331338879647</v>
+        <v>0.34205801901424909</v>
       </c>
       <c r="N15" s="0">
-        <v>0.40499825687613883</v>
+        <v>0.44604565095041254</v>
       </c>
       <c r="O15" s="0">
-        <v>848.17910447761199</v>
+        <v>999.77947598253274</v>
       </c>
       <c r="P15" s="0">
-        <v>135.91044776119404</v>
+        <v>125.13755458515284</v>
       </c>
       <c r="Q15" s="0">
-        <v>16.961630901287556</v>
+        <v>29.310967741935485</v>
       </c>
       <c r="R15" s="0">
-        <v>16.961630901287556</v>
+        <v>29.310967741935485</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B16" s="0">
         <v>15</v>
@@ -1329,51 +1409,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E16" s="0">
-        <v>205.65552699228789</v>
+        <v>66.838046272493557</v>
       </c>
       <c r="F16" s="0">
-        <v>195.37275064267351</v>
+        <v>35.989717223650381</v>
       </c>
       <c r="G16" s="0">
-        <v>1.0526315789473684</v>
+        <v>1.857142857142857</v>
       </c>
       <c r="H16" s="0">
-        <v>806</v>
+        <v>68</v>
       </c>
       <c r="I16" s="0">
-        <v>164.70355552080804</v>
+        <v>47.839861096979718</v>
       </c>
       <c r="J16" s="0">
-        <v>21305.701125422111</v>
+        <v>1797.5033207552151</v>
       </c>
       <c r="K16" s="0">
-        <v>68.696032708034139</v>
+        <v>18.945964672341148</v>
       </c>
       <c r="L16" s="0">
-        <v>756.62203249068079</v>
+        <v>194.66247052605303</v>
       </c>
       <c r="M16" s="0">
-        <v>0.46767884698454354</v>
+        <v>0.59609448486482153</v>
       </c>
       <c r="N16" s="0">
-        <v>0.39561231876119851</v>
+        <v>0.4032712144287729</v>
       </c>
       <c r="O16" s="0">
-        <v>206.32382133995037</v>
+        <v>848.25</v>
       </c>
       <c r="P16" s="0">
-        <v>151.3697270471464</v>
+        <v>135.9264705882353</v>
       </c>
       <c r="Q16" s="0">
-        <v>44.594838709677418</v>
+        <v>16.049310344827582</v>
       </c>
       <c r="R16" s="0">
-        <v>44.594838709677418</v>
+        <v>16.049310344827582</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B17" s="0">
         <v>16</v>
@@ -1385,51 +1465,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E17" s="0">
-        <v>46.272493573264775</v>
+        <v>205.65552699228789</v>
       </c>
       <c r="F17" s="0">
-        <v>46.272493573264775</v>
+        <v>195.37275064267351</v>
       </c>
       <c r="G17" s="0">
-        <v>1</v>
+        <v>1.0526315789473684</v>
       </c>
       <c r="H17" s="0">
-        <v>62</v>
+        <v>805</v>
       </c>
       <c r="I17" s="0">
-        <v>45.680547283192567</v>
+        <v>164.60135038808613</v>
       </c>
       <c r="J17" s="0">
-        <v>1638.9000865709315</v>
+        <v>21279.26725305806</v>
       </c>
       <c r="K17" s="0">
-        <v>16.690312415012361</v>
+        <v>68.667397179892021</v>
       </c>
       <c r="L17" s="0">
-        <v>164.76616657311655</v>
+        <v>756.32347243006359</v>
       </c>
       <c r="M17" s="0">
-        <v>0.7586234567547615</v>
+        <v>0.46746744910059373</v>
       </c>
       <c r="N17" s="0">
-        <v>0.47217752737114177</v>
+        <v>0.3962951671074737</v>
       </c>
       <c r="O17" s="0">
-        <v>631.30645161290317</v>
+        <v>206.33291925465838</v>
       </c>
       <c r="P17" s="0">
-        <v>141.64516129032259</v>
+        <v>151.3503105590062</v>
       </c>
       <c r="Q17" s="0">
-        <v>35.70894736838035</v>
+        <v>44.572698412698415</v>
       </c>
       <c r="R17" s="0">
-        <v>35.70894736838035</v>
+        <v>44.572698412698415</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B18" s="0">
         <v>17</v>
@@ -1441,51 +1521,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E18" s="0">
-        <v>113.11053984575834</v>
+        <v>46.272493573264775</v>
       </c>
       <c r="F18" s="0">
-        <v>102.82776349614394</v>
+        <v>46.272493573264775</v>
       </c>
       <c r="G18" s="0">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="H18" s="0">
-        <v>291</v>
+        <v>63</v>
       </c>
       <c r="I18" s="0">
-        <v>98.96507272662717</v>
+        <v>46.047465203921689</v>
       </c>
       <c r="J18" s="0">
-        <v>7692.2568579377594</v>
+        <v>1665.3339589349787</v>
       </c>
       <c r="K18" s="0">
-        <v>37.998476514163521</v>
+        <v>16.834880560070026</v>
       </c>
       <c r="L18" s="0">
-        <v>390.96087691511633</v>
+        <v>165.35612870134352</v>
       </c>
       <c r="M18" s="0">
-        <v>0.63240754315906322</v>
+        <v>0.765368545517913</v>
       </c>
       <c r="N18" s="0">
-        <v>0.48282050097675927</v>
+        <v>0.47087689733260879</v>
       </c>
       <c r="O18" s="0">
-        <v>794.14776632302403</v>
+        <v>631.38095238095241</v>
       </c>
       <c r="P18" s="0">
-        <v>146.86254295532646</v>
+        <v>141.63492063492063</v>
       </c>
       <c r="Q18" s="0">
-        <v>20.608275862068968</v>
+        <v>15.545903257649883</v>
       </c>
       <c r="R18" s="0">
-        <v>20.608275862068968</v>
+        <v>15.545903257649883</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B19" s="0">
         <v>18</v>
@@ -1497,51 +1577,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E19" s="0">
-        <v>154.24164524421593</v>
+        <v>113.11053984575834</v>
       </c>
       <c r="F19" s="0">
-        <v>87.403598971722346</v>
+        <v>102.82776349614394</v>
       </c>
       <c r="G19" s="0">
-        <v>1.7647058823529416</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H19" s="0">
-        <v>257</v>
+        <v>295</v>
       </c>
       <c r="I19" s="0">
-        <v>93.004083054979091</v>
+        <v>99.64292361349176</v>
       </c>
       <c r="J19" s="0">
-        <v>6793.5051975601518</v>
+        <v>7797.992347393948</v>
       </c>
       <c r="K19" s="0">
-        <v>42.608865814402499</v>
+        <v>38.087083279880481</v>
       </c>
       <c r="L19" s="0">
-        <v>451.28665261330013</v>
+        <v>391.2784896489826</v>
       </c>
       <c r="M19" s="0">
-        <v>0.4191783060116071</v>
+        <v>0.64006005106653652</v>
       </c>
       <c r="N19" s="0">
-        <v>0.38257958565784184</v>
+        <v>0.47851732778274764</v>
       </c>
       <c r="O19" s="0">
-        <v>821.05447470817126</v>
+        <v>794.0542372881356</v>
       </c>
       <c r="P19" s="0">
-        <v>172.63035019455253</v>
+        <v>146.89491525423728</v>
       </c>
       <c r="Q19" s="0">
-        <v>20.161212121212124</v>
+        <v>20.581249999999994</v>
       </c>
       <c r="R19" s="0">
-        <v>20.161212121212124</v>
+        <v>20.581249999999994</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B20" s="0">
         <v>19</v>
@@ -1553,51 +1633,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E20" s="0">
-        <v>1172.2365038560411</v>
+        <v>154.24164524421593</v>
       </c>
       <c r="F20" s="0">
-        <v>1100.2570694087401</v>
+        <v>87.403598971722346</v>
       </c>
       <c r="G20" s="0">
-        <v>1.0654205607476637</v>
+        <v>1.7647058823529416</v>
       </c>
       <c r="H20" s="0">
-        <v>17021</v>
+        <v>261</v>
       </c>
       <c r="I20" s="0">
-        <v>756.88167313555721</v>
+        <v>93.725055728737757</v>
       </c>
       <c r="J20" s="0">
-        <v>449930.9415084488</v>
+        <v>6899.2406870163404</v>
       </c>
       <c r="K20" s="0">
-        <v>394.97924802443379</v>
+        <v>43.106954574040714</v>
       </c>
       <c r="L20" s="0">
-        <v>5695.5106696334742</v>
+        <v>451.93093457114173</v>
       </c>
       <c r="M20" s="0">
-        <v>0.1742971897341353</v>
+        <v>0.4244895668938683</v>
       </c>
       <c r="N20" s="0">
-        <v>0.24726622611214871</v>
+        <v>0.38136012621905302</v>
       </c>
       <c r="O20" s="0">
-        <v>491.0935902708419</v>
+        <v>821.0306513409962</v>
       </c>
       <c r="P20" s="0">
-        <v>282.94618412549204</v>
+        <v>172.57854406130269</v>
       </c>
       <c r="Q20" s="0">
-        <v>72.1802714932127</v>
+        <v>21.101428571428571</v>
       </c>
       <c r="R20" s="0">
-        <v>72.1802714932127</v>
+        <v>21.101428571428571</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B21" s="0">
         <v>20</v>
@@ -1609,51 +1689,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E21" s="0">
-        <v>2493.5732647814907</v>
+        <v>1167.0951156812337</v>
       </c>
       <c r="F21" s="0">
-        <v>2133.6760925449867</v>
+        <v>1100.2570694087401</v>
       </c>
       <c r="G21" s="0">
-        <v>1.1686746987951808</v>
+        <v>1.0607476635514019</v>
       </c>
       <c r="H21" s="0">
-        <v>78797</v>
+        <v>17015</v>
       </c>
       <c r="I21" s="0">
-        <v>1628.5094955998413</v>
+        <v>756.74825881451102</v>
       </c>
       <c r="J21" s="0">
-        <v>2082909.8406698336</v>
+        <v>449772.33827426453</v>
       </c>
       <c r="K21" s="0">
-        <v>833.78863109689735</v>
+        <v>395.06610161450959</v>
       </c>
       <c r="L21" s="0">
-        <v>13290.488431876605</v>
+        <v>5670.8641390799639</v>
       </c>
       <c r="M21" s="0">
-        <v>0.1481830236634743</v>
+        <v>0.17575355596137454</v>
       </c>
       <c r="N21" s="0">
-        <v>0.27619611613855805</v>
+        <v>0.24755965090814602</v>
       </c>
       <c r="O21" s="0">
-        <v>261.66034239882231</v>
+        <v>491.15427563914193</v>
       </c>
       <c r="P21" s="0">
-        <v>434.07433024099902</v>
+        <v>282.90420217455187</v>
       </c>
       <c r="Q21" s="0">
-        <v>110.81598156682028</v>
+        <v>85.257241379310329</v>
       </c>
       <c r="R21" s="0">
-        <v>110.81598156682028</v>
+        <v>85.257241379310329</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B22" s="0">
         <v>21</v>
@@ -1665,51 +1745,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E22" s="0">
-        <v>221.07969151670949</v>
+        <v>2493.5732647814907</v>
       </c>
       <c r="F22" s="0">
-        <v>190.23136246786629</v>
+        <v>2133.6760925449867</v>
       </c>
       <c r="G22" s="0">
-        <v>1.1621621621621623</v>
+        <v>1.1686746987951808</v>
       </c>
       <c r="H22" s="0">
-        <v>984</v>
+        <v>78747</v>
       </c>
       <c r="I22" s="0">
-        <v>181.98391464235726</v>
+        <v>1627.9927348357949</v>
       </c>
       <c r="J22" s="0">
-        <v>26010.930406222527</v>
+        <v>2081588.1470516312</v>
       </c>
       <c r="K22" s="0">
-        <v>69.090573638776803</v>
+        <v>833.78366077408543</v>
       </c>
       <c r="L22" s="0">
-        <v>738.72825736798097</v>
+        <v>13285.347043701797</v>
       </c>
       <c r="M22" s="0">
-        <v>0.59895794177076711</v>
+        <v>0.14820363746671314</v>
       </c>
       <c r="N22" s="0">
-        <v>0.49397796180266323</v>
+        <v>0.27651405866228956</v>
       </c>
       <c r="O22" s="0">
-        <v>727.54573170731703</v>
+        <v>261.62467141605396</v>
       </c>
       <c r="P22" s="0">
-        <v>288.70731707317071</v>
+        <v>434.04436994425186</v>
       </c>
       <c r="Q22" s="0">
-        <v>42.836965294592417</v>
+        <v>123.12824896887889</v>
       </c>
       <c r="R22" s="0">
-        <v>42.836965294592417</v>
+        <v>123.12824896887889</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B23" s="0">
         <v>22</v>
@@ -1724,48 +1804,48 @@
         <v>221.07969151670949</v>
       </c>
       <c r="F23" s="0">
-        <v>164.52442159383031</v>
+        <v>190.23136246786629</v>
       </c>
       <c r="G23" s="0">
-        <v>1.34375</v>
+        <v>1.1621621621621623</v>
       </c>
       <c r="H23" s="0">
-        <v>916</v>
+        <v>988</v>
       </c>
       <c r="I23" s="0">
-        <v>175.58329327922533</v>
+        <v>182.35342550940555</v>
       </c>
       <c r="J23" s="0">
-        <v>24213.427085467309</v>
+        <v>26116.665895678714</v>
       </c>
       <c r="K23" s="0">
-        <v>69.771200456599971</v>
+        <v>69.135625188575546</v>
       </c>
       <c r="L23" s="0">
-        <v>735.7538489603827</v>
+        <v>735.21850899742924</v>
       </c>
       <c r="M23" s="0">
-        <v>0.56208376430178886</v>
+        <v>0.60714823057297951</v>
       </c>
       <c r="N23" s="0">
-        <v>0.28269714050550732</v>
+        <v>0.491485127959922</v>
       </c>
       <c r="O23" s="0">
-        <v>462.04366812227073</v>
+        <v>727.61032388663966</v>
       </c>
       <c r="P23" s="0">
-        <v>418.48799126637556</v>
+        <v>288.77226720647775</v>
       </c>
       <c r="Q23" s="0">
-        <v>44.845405405405423</v>
+        <v>44.319999999999993</v>
       </c>
       <c r="R23" s="0">
-        <v>44.845405405405423</v>
+        <v>44.319999999999993</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B24" s="0">
         <v>23</v>
@@ -1777,51 +1857,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E24" s="0">
-        <v>143.95886889460152</v>
+        <v>221.07969151670949</v>
       </c>
       <c r="F24" s="0">
-        <v>123.39331619537273</v>
+        <v>164.52442159383031</v>
       </c>
       <c r="G24" s="0">
-        <v>1.1666666666666667</v>
+        <v>1.34375</v>
       </c>
       <c r="H24" s="0">
-        <v>379</v>
+        <v>912</v>
       </c>
       <c r="I24" s="0">
-        <v>112.94189197039627</v>
+        <v>175.19950420112758</v>
       </c>
       <c r="J24" s="0">
-        <v>10018.43762597392</v>
+        <v>24107.691596011122</v>
       </c>
       <c r="K24" s="0">
-        <v>45.42388932578163</v>
+        <v>69.700487823134736</v>
       </c>
       <c r="L24" s="0">
-        <v>528.9398566505763</v>
+        <v>729.98366964658737</v>
       </c>
       <c r="M24" s="0">
-        <v>0.44998421175297443</v>
+        <v>0.56851143128114301</v>
       </c>
       <c r="N24" s="0">
-        <v>0.31770271631607477</v>
+        <v>0.28459428074503318</v>
       </c>
       <c r="O24" s="0">
-        <v>32.195250659630609</v>
+        <v>462.06359649122805</v>
       </c>
       <c r="P24" s="0">
-        <v>472.89445910290237</v>
+        <v>418.50986842105266</v>
       </c>
       <c r="Q24" s="0">
-        <v>30.139534883720927</v>
+        <v>50.930140845070426</v>
       </c>
       <c r="R24" s="0">
-        <v>30.139534883720927</v>
+        <v>50.930140845070426</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B25" s="0">
         <v>24</v>
@@ -1833,51 +1913,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E25" s="0">
-        <v>190.23136246786629</v>
+        <v>143.95886889460152</v>
       </c>
       <c r="F25" s="0">
-        <v>143.95886889460152</v>
+        <v>123.39331619537273</v>
       </c>
       <c r="G25" s="0">
-        <v>1.3214285714285714</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="H25" s="0">
-        <v>691</v>
+        <v>379</v>
       </c>
       <c r="I25" s="0">
-        <v>152.50162709145562</v>
+        <v>112.94189197039627</v>
       </c>
       <c r="J25" s="0">
-        <v>18265.805803556672</v>
+        <v>10018.43762597392</v>
       </c>
       <c r="K25" s="0">
-        <v>60.47182630670904</v>
+        <v>45.42388932578163</v>
       </c>
       <c r="L25" s="0">
-        <v>604.18589607439878</v>
+        <v>528.9398566505763</v>
       </c>
       <c r="M25" s="0">
-        <v>0.62879276215908919</v>
+        <v>0.44998421175297443</v>
       </c>
       <c r="N25" s="0">
-        <v>0.29778162620906684</v>
+        <v>0.31774069731448912</v>
       </c>
       <c r="O25" s="0">
-        <v>518.59623733719252</v>
+        <v>32.195250659630609</v>
       </c>
       <c r="P25" s="0">
-        <v>498.73661360347324</v>
+        <v>472.89445910290237</v>
       </c>
       <c r="Q25" s="0">
-        <v>53.301333333333353</v>
+        <v>30.139534883720927</v>
       </c>
       <c r="R25" s="0">
-        <v>53.301333333333353</v>
+        <v>30.139534883720927</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B26" s="0">
         <v>25</v>
@@ -1889,51 +1969,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E26" s="0">
-        <v>339.331619537275</v>
+        <v>190.23136246786629</v>
       </c>
       <c r="F26" s="0">
-        <v>318.76606683804624</v>
+        <v>143.95886889460152</v>
       </c>
       <c r="G26" s="0">
-        <v>1.064516129032258</v>
+        <v>1.3214285714285714</v>
       </c>
       <c r="H26" s="0">
-        <v>2085</v>
+        <v>691</v>
       </c>
       <c r="I26" s="0">
-        <v>264.90397999274535</v>
+        <v>152.50162709145562</v>
       </c>
       <c r="J26" s="0">
-        <v>55114.623879038583</v>
+        <v>18265.805803556672</v>
       </c>
       <c r="K26" s="0">
-        <v>108.85500685511379</v>
+        <v>60.545556696854177</v>
       </c>
       <c r="L26" s="0">
-        <v>1126.9253308014218</v>
+        <v>604.07628712278267</v>
       </c>
       <c r="M26" s="0">
-        <v>0.54536395439602126</v>
+        <v>0.6290209703167684</v>
       </c>
       <c r="N26" s="0">
-        <v>0.3640973521467798</v>
+        <v>0.29784060537078783</v>
       </c>
       <c r="O26" s="0">
-        <v>649.15107913669067</v>
+        <v>518.56439942112877</v>
       </c>
       <c r="P26" s="0">
-        <v>565.96019184652278</v>
+        <v>498.70477568740955</v>
       </c>
       <c r="Q26" s="0">
-        <v>60.023418803418778</v>
+        <v>53.42000000000003</v>
       </c>
       <c r="R26" s="0">
-        <v>60.023418803418778</v>
+        <v>53.42000000000003</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B27" s="0">
         <v>26</v>
@@ -1945,51 +2025,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E27" s="0">
-        <v>51.413881748071972</v>
+        <v>339.331619537275</v>
       </c>
       <c r="F27" s="0">
-        <v>41.131105398457578</v>
+        <v>318.76606683804624</v>
       </c>
       <c r="G27" s="0">
-        <v>1.25</v>
+        <v>1.064516129032258</v>
       </c>
       <c r="H27" s="0">
-        <v>66</v>
+        <v>2083</v>
       </c>
       <c r="I27" s="0">
-        <v>47.131083231234342</v>
+        <v>264.77689724137196</v>
       </c>
       <c r="J27" s="0">
-        <v>1744.6355760271206</v>
+        <v>55061.75613431049</v>
       </c>
       <c r="K27" s="0">
-        <v>17.821190892362768</v>
+        <v>108.74929311873673</v>
       </c>
       <c r="L27" s="0">
-        <v>168.77478086234254</v>
+        <v>1127.2853172771609</v>
       </c>
       <c r="M27" s="0">
-        <v>0.76966100354704947</v>
+        <v>0.54449290091911395</v>
       </c>
       <c r="N27" s="0">
-        <v>0.61776484792717157</v>
+        <v>0.36506943137846404</v>
       </c>
       <c r="O27" s="0">
-        <v>751.87878787878788</v>
+        <v>649.19155064810366</v>
       </c>
       <c r="P27" s="0">
-        <v>604.969696969697</v>
+        <v>565.94767162746041</v>
       </c>
       <c r="Q27" s="0">
-        <v>13.131999999999998</v>
+        <v>59.105007824726137</v>
       </c>
       <c r="R27" s="0">
-        <v>13.131999999999998</v>
+        <v>59.105007824726137</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B28" s="0">
         <v>27</v>
@@ -2001,51 +2081,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E28" s="0">
-        <v>113.11053984575834</v>
+        <v>51.413881748071972</v>
       </c>
       <c r="F28" s="0">
-        <v>56.55526992287917</v>
+        <v>41.131105398457578</v>
       </c>
       <c r="G28" s="0">
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="H28" s="0">
-        <v>179</v>
+        <v>68</v>
       </c>
       <c r="I28" s="0">
-        <v>77.617914420417577</v>
+        <v>47.839861096979718</v>
       </c>
       <c r="J28" s="0">
-        <v>4731.6631531644634</v>
+        <v>1797.5033207552151</v>
       </c>
       <c r="K28" s="0">
-        <v>33.086117352460398</v>
+        <v>17.887638719621084</v>
       </c>
       <c r="L28" s="0">
-        <v>307.47814161793224</v>
+        <v>169.74261966501007</v>
       </c>
       <c r="M28" s="0">
-        <v>0.6289196854998812</v>
+        <v>0.78396696841063818</v>
       </c>
       <c r="N28" s="0">
-        <v>0.49875819445396746</v>
+        <v>0.60992834677308438</v>
       </c>
       <c r="O28" s="0">
-        <v>559.90502793296093</v>
+        <v>751.76470588235293</v>
       </c>
       <c r="P28" s="0">
-        <v>625.9441340782123</v>
+        <v>604.95588235294122</v>
       </c>
       <c r="Q28" s="0">
-        <v>24.150697674418598</v>
+        <v>13.131999999999998</v>
       </c>
       <c r="R28" s="0">
-        <v>24.150697674418598</v>
+        <v>13.131999999999998</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B29" s="0">
         <v>28</v>
@@ -2057,51 +2137,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E29" s="0">
-        <v>71.979434447300761</v>
+        <v>113.11053984575834</v>
       </c>
       <c r="F29" s="0">
         <v>56.55526992287917</v>
       </c>
       <c r="G29" s="0">
-        <v>1.2727272727272727</v>
+        <v>2</v>
       </c>
       <c r="H29" s="0">
-        <v>90</v>
+        <v>178</v>
       </c>
       <c r="I29" s="0">
-        <v>55.037247799057205</v>
+        <v>77.400800947799496</v>
       </c>
       <c r="J29" s="0">
-        <v>2379.0485127642555</v>
+        <v>4705.2292808004158</v>
       </c>
       <c r="K29" s="0">
-        <v>24.798509867003716</v>
+        <v>32.940214525126308</v>
       </c>
       <c r="L29" s="0">
-        <v>223.06878045002381</v>
+        <v>307.2481659654444</v>
       </c>
       <c r="M29" s="0">
-        <v>0.60080781937109651</v>
+        <v>0.62634275275275342</v>
       </c>
       <c r="N29" s="0">
-        <v>0.47825405002724058</v>
+        <v>0.50064151955328284</v>
       </c>
       <c r="O29" s="0">
-        <v>601.11111111111109</v>
+        <v>559.84831460674161</v>
       </c>
       <c r="P29" s="0">
-        <v>628.70000000000005</v>
+        <v>625.95505617977528</v>
       </c>
       <c r="Q29" s="0">
-        <v>18.420909090909088</v>
+        <v>22.673333333333332</v>
       </c>
       <c r="R29" s="0">
-        <v>18.420909090909088</v>
+        <v>22.673333333333332</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B30" s="0">
         <v>29</v>
@@ -2113,51 +2193,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E30" s="0">
-        <v>298.20051413881743</v>
+        <v>66.838046272493557</v>
       </c>
       <c r="F30" s="0">
-        <v>267.35218508997423</v>
+        <v>56.55526992287917</v>
       </c>
       <c r="G30" s="0">
-        <v>1.1153846153846154</v>
+        <v>1.1818181818181817</v>
       </c>
       <c r="H30" s="0">
-        <v>1856</v>
+        <v>89</v>
       </c>
       <c r="I30" s="0">
-        <v>249.93348194330068</v>
+        <v>54.730631219459177</v>
       </c>
       <c r="J30" s="0">
-        <v>49061.267107671752</v>
+        <v>2352.6146404002079</v>
       </c>
       <c r="K30" s="0">
-        <v>91.776119947506174</v>
+        <v>24.555310416070903</v>
       </c>
       <c r="L30" s="0">
-        <v>949.64675447237153</v>
+        <v>216.82465641619768</v>
       </c>
       <c r="M30" s="0">
-        <v>0.6836352499269791</v>
+        <v>0.62884458507517615</v>
       </c>
       <c r="N30" s="0">
-        <v>0.34380595119321328</v>
+        <v>0.47921562418042413</v>
       </c>
       <c r="O30" s="0">
-        <v>92.602370689655174</v>
+        <v>601.14606741573039</v>
       </c>
       <c r="P30" s="0">
-        <v>699.1842672413793</v>
+        <v>628.61797752808991</v>
       </c>
       <c r="Q30" s="0">
-        <v>65.291897435897454</v>
+        <v>21.029090909090908</v>
       </c>
       <c r="R30" s="0">
-        <v>65.291897435897454</v>
+        <v>21.029090909090908</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B31" s="0">
         <v>30</v>
@@ -2169,51 +2249,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E31" s="0">
-        <v>200.5141388174807</v>
+        <v>298.20051413881743</v>
       </c>
       <c r="F31" s="0">
-        <v>174.80719794344469</v>
+        <v>267.35218508997423</v>
       </c>
       <c r="G31" s="0">
-        <v>1.1470588235294119</v>
+        <v>1.1153846153846154</v>
       </c>
       <c r="H31" s="0">
-        <v>641</v>
+        <v>1855</v>
       </c>
       <c r="I31" s="0">
-        <v>146.8806103092646</v>
+        <v>249.86614165326165</v>
       </c>
       <c r="J31" s="0">
-        <v>16944.112185354308</v>
+        <v>49034.833235307706</v>
       </c>
       <c r="K31" s="0">
-        <v>61.571669691973796</v>
+        <v>91.725381492263338</v>
       </c>
       <c r="L31" s="0">
-        <v>687.34048686538665</v>
+        <v>939.54613653352885</v>
       </c>
       <c r="M31" s="0">
-        <v>0.45069716870801912</v>
+        <v>0.69803684120487419</v>
       </c>
       <c r="N31" s="0">
-        <v>0.38664531812322217</v>
+        <v>0.34391476551814104</v>
       </c>
       <c r="O31" s="0">
-        <v>386.03120124804991</v>
+        <v>92.598921832884102</v>
       </c>
       <c r="P31" s="0">
-        <v>739.27925117004679</v>
+        <v>699.20646900269537</v>
       </c>
       <c r="Q31" s="0">
-        <v>32.664615384615367</v>
+        <v>80.147169811320779</v>
       </c>
       <c r="R31" s="0">
-        <v>32.664615384615367</v>
+        <v>80.147169811320779</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B32" s="0">
         <v>31</v>
@@ -2225,51 +2305,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E32" s="0">
-        <v>56.55526992287917</v>
+        <v>200.5141388174807</v>
       </c>
       <c r="F32" s="0">
-        <v>41.131105398457578</v>
+        <v>174.80719794344469</v>
       </c>
       <c r="G32" s="0">
-        <v>1.375</v>
+        <v>1.1470588235294119</v>
       </c>
       <c r="H32" s="0">
-        <v>61</v>
+        <v>636</v>
       </c>
       <c r="I32" s="0">
-        <v>45.310658221632629</v>
+        <v>146.30663152007196</v>
       </c>
       <c r="J32" s="0">
-        <v>1612.4662142068842</v>
+        <v>16811.942823534071</v>
       </c>
       <c r="K32" s="0">
-        <v>19.126950801882025</v>
+        <v>61.44629088507935</v>
       </c>
       <c r="L32" s="0">
-        <v>181.98478497050439</v>
+        <v>682.4908711285932</v>
       </c>
       <c r="M32" s="0">
-        <v>0.61182938008607146</v>
+        <v>0.45355929850985327</v>
       </c>
       <c r="N32" s="0">
-        <v>0.41812370332778193</v>
+        <v>0.38984236188366994</v>
       </c>
       <c r="O32" s="0">
-        <v>601.24590163934431</v>
+        <v>386.02358490566036</v>
       </c>
       <c r="P32" s="0">
-        <v>751.57377049180332</v>
+        <v>739.23270440251576</v>
       </c>
       <c r="Q32" s="0">
-        <v>14.803187250996011</v>
+        <v>31.476404494382031</v>
       </c>
       <c r="R32" s="0">
-        <v>14.803187250996011</v>
+        <v>31.476404494382031</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B33" s="0">
         <v>32</v>
@@ -2281,51 +2361,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E33" s="0">
-        <v>66.838046272493557</v>
+        <v>56.55526992287917</v>
       </c>
       <c r="F33" s="0">
-        <v>66.838046272493557</v>
+        <v>41.131105398457578</v>
       </c>
       <c r="G33" s="0">
-        <v>1</v>
+        <v>1.375</v>
       </c>
       <c r="H33" s="0">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="I33" s="0">
-        <v>60.845966814428756</v>
+        <v>44.182414981918356</v>
       </c>
       <c r="J33" s="0">
-        <v>2907.7259600452012</v>
+        <v>1533.1645971147423</v>
       </c>
       <c r="K33" s="0">
-        <v>24.560112401453939</v>
+        <v>18.252399436832906</v>
       </c>
       <c r="L33" s="0">
-        <v>251.59372652112131</v>
+        <v>176.16761738722585</v>
       </c>
       <c r="M33" s="0">
-        <v>0.57724970848720925</v>
+        <v>0.62079253355864017</v>
       </c>
       <c r="N33" s="0">
-        <v>0.53850649931430405</v>
+        <v>0.42194545053421367</v>
       </c>
       <c r="O33" s="0">
-        <v>583.92727272727268</v>
+        <v>601.34482758620686</v>
       </c>
       <c r="P33" s="0">
-        <v>760.70909090909095</v>
+        <v>751.39655172413791</v>
       </c>
       <c r="Q33" s="0">
-        <v>20.780799999999999</v>
+        <v>14.274183976261131</v>
       </c>
       <c r="R33" s="0">
-        <v>20.780799999999999</v>
+        <v>14.274183976261131</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B34" s="0">
         <v>33</v>
@@ -2337,51 +2417,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E34" s="0">
-        <v>71.979434447300761</v>
+        <v>66.838046272493557</v>
       </c>
       <c r="F34" s="0">
-        <v>25.706940874035986</v>
+        <v>66.838046272493557</v>
       </c>
       <c r="G34" s="0">
-        <v>2.7999999999999998</v>
+        <v>1</v>
       </c>
       <c r="H34" s="0">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="I34" s="0">
-        <v>50.575740456204976</v>
+        <v>60.290284245090362</v>
       </c>
       <c r="J34" s="0">
-        <v>2008.9742996675934</v>
+        <v>2854.8582153171064</v>
       </c>
       <c r="K34" s="0">
-        <v>21.603827141930985</v>
+        <v>24.127978644742441</v>
       </c>
       <c r="L34" s="0">
-        <v>197.40368277133101</v>
+        <v>243.87049778339227</v>
       </c>
       <c r="M34" s="0">
-        <v>0.64784892688923201</v>
+        <v>0.60322020332400816</v>
       </c>
       <c r="N34" s="0">
-        <v>0.69979724970179447</v>
+        <v>0.54182113247860941</v>
       </c>
       <c r="O34" s="0">
-        <v>956.17105263157896</v>
+        <v>583.87962962962968</v>
       </c>
       <c r="P34" s="0">
-        <v>853.65789473684208</v>
+        <v>760.90740740740739</v>
       </c>
       <c r="Q34" s="0">
-        <v>16.292244897959183</v>
+        <v>20.877241379310341</v>
       </c>
       <c r="R34" s="0">
-        <v>16.292244897959183</v>
+        <v>20.877241379310341</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B35" s="0">
         <v>34</v>
@@ -2393,51 +2473,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E35" s="0">
-        <v>128.53470437017992</v>
+        <v>71.979434447300761</v>
       </c>
       <c r="F35" s="0">
-        <v>56.55526992287917</v>
+        <v>25.706940874035986</v>
       </c>
       <c r="G35" s="0">
-        <v>2.2727272727272725</v>
+        <v>2.7999999999999998</v>
       </c>
       <c r="H35" s="0">
-        <v>186</v>
+        <v>78</v>
       </c>
       <c r="I35" s="0">
-        <v>79.12102881204197</v>
+        <v>51.236889307628573</v>
       </c>
       <c r="J35" s="0">
-        <v>4916.7002597127948</v>
+        <v>2061.8420443956879</v>
       </c>
       <c r="K35" s="0">
-        <v>36.346066023042539</v>
+        <v>21.907371699511931</v>
       </c>
       <c r="L35" s="0">
-        <v>341.40027469336081</v>
+        <v>196.65894701490868</v>
       </c>
       <c r="M35" s="0">
-        <v>0.53009763235657381</v>
+        <v>0.66994297344333553</v>
       </c>
       <c r="N35" s="0">
-        <v>0.73712327504169639</v>
+        <v>0.69693914865537365</v>
       </c>
       <c r="O35" s="0">
-        <v>906.11827956989248</v>
+        <v>956.02564102564099</v>
       </c>
       <c r="P35" s="0">
-        <v>904.98924731182797</v>
+        <v>853.62820512820508</v>
       </c>
       <c r="Q35" s="0">
-        <v>18.276107382550332</v>
+        <v>18.049763779527559</v>
       </c>
       <c r="R35" s="0">
-        <v>18.276107382550332</v>
+        <v>18.049763779527559</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B36" s="0">
         <v>35</v>
@@ -2449,51 +2529,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E36" s="0">
-        <v>102.82776349614394</v>
+        <v>128.53470437017992</v>
       </c>
       <c r="F36" s="0">
-        <v>102.82776349614394</v>
+        <v>56.55526992287917</v>
       </c>
       <c r="G36" s="0">
-        <v>1</v>
+        <v>2.2727272727272725</v>
       </c>
       <c r="H36" s="0">
-        <v>243</v>
+        <v>190</v>
       </c>
       <c r="I36" s="0">
-        <v>90.435426367635557</v>
+        <v>79.96726709556556</v>
       </c>
       <c r="J36" s="0">
-        <v>6423.4309844634899</v>
+        <v>5022.4357491689834</v>
       </c>
       <c r="K36" s="0">
-        <v>36.574424236092121</v>
+        <v>36.549231967313474</v>
       </c>
       <c r="L36" s="0">
-        <v>356.20042724512268</v>
+        <v>344.17431449410458</v>
       </c>
       <c r="M36" s="0">
-        <v>0.63619178111807817</v>
+        <v>0.53280383420876332</v>
       </c>
       <c r="N36" s="0">
-        <v>0.50263449045368502</v>
+        <v>0.7332684291064927</v>
       </c>
       <c r="O36" s="0">
-        <v>313.04938271604937</v>
+        <v>906.17894736842106</v>
       </c>
       <c r="P36" s="0">
-        <v>946.90123456790127</v>
+        <v>905.03157894736842</v>
       </c>
       <c r="Q36" s="0">
-        <v>21.51576923076923</v>
+        <v>18.174647887323939</v>
       </c>
       <c r="R36" s="0">
-        <v>21.51576923076923</v>
+        <v>18.174647887323939</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B37" s="0">
         <v>36</v>
@@ -2505,51 +2585,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E37" s="0">
-        <v>149.10025706940871</v>
+        <v>102.82776349614394</v>
       </c>
       <c r="F37" s="0">
-        <v>143.95886889460152</v>
+        <v>102.82776349614394</v>
       </c>
       <c r="G37" s="0">
-        <v>1.0357142857142856</v>
+        <v>1</v>
       </c>
       <c r="H37" s="0">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="I37" s="0">
-        <v>87.983122650364038</v>
+        <v>90.991957321178631</v>
       </c>
       <c r="J37" s="0">
-        <v>6079.7906437308748</v>
+        <v>6502.7326015556318</v>
       </c>
       <c r="K37" s="0">
-        <v>58.619446494517391</v>
+        <v>36.469338167629019</v>
       </c>
       <c r="L37" s="0">
-        <v>572.02165190084213</v>
+        <v>355.77469107506772</v>
       </c>
       <c r="M37" s="0">
-        <v>0.23349283220621125</v>
+        <v>0.64558831233612413</v>
       </c>
       <c r="N37" s="0">
-        <v>0.54685896642520104</v>
+        <v>0.50045885096605658</v>
       </c>
       <c r="O37" s="0">
-        <v>365.99130434782609</v>
+        <v>313.01626016260161</v>
       </c>
       <c r="P37" s="0">
-        <v>980.87826086956522</v>
+        <v>946.82520325203257</v>
       </c>
       <c r="Q37" s="0">
-        <v>15.129651567944249</v>
+        <v>21.000714285714281</v>
       </c>
       <c r="R37" s="0">
-        <v>15.129651567944249</v>
+        <v>21.000714285714281</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B38" s="0">
         <v>37</v>
@@ -2561,107 +2641,107 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E38" s="0">
-        <v>87.403598971722346</v>
+        <v>149.10025706940871</v>
       </c>
       <c r="F38" s="0">
-        <v>61.696658097686367</v>
+        <v>143.95886889460152</v>
       </c>
       <c r="G38" s="0">
-        <v>1.4166666666666665</v>
+        <v>1.0357142857142856</v>
       </c>
       <c r="H38" s="0">
-        <v>141</v>
+        <v>229</v>
       </c>
       <c r="I38" s="0">
-        <v>68.888227424056737</v>
+        <v>87.791646639612665</v>
       </c>
       <c r="J38" s="0">
-        <v>3727.1760033306668</v>
+        <v>6053.3567713668272</v>
       </c>
       <c r="K38" s="0">
-        <v>27.749892897314066</v>
+        <v>58.597055375504134</v>
       </c>
       <c r="L38" s="0">
-        <v>287.6297286907166</v>
+        <v>568.19992247941161</v>
       </c>
       <c r="M38" s="0">
-        <v>0.56613789019932426</v>
+        <v>0.23561546613956671</v>
       </c>
       <c r="N38" s="0">
-        <v>0.60824092599297153</v>
+        <v>0.54832638000626255</v>
       </c>
       <c r="O38" s="0">
-        <v>74.872340425531917</v>
+        <v>365.65938864628822</v>
       </c>
       <c r="P38" s="0">
-        <v>988.80851063829789</v>
+        <v>980.61135371179034</v>
       </c>
       <c r="Q38" s="0">
-        <v>22.093333333333337</v>
+        <v>15.09434782608696</v>
       </c>
       <c r="R38" s="0">
-        <v>22.093333333333337</v>
+        <v>15.09434782608696</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="B39" s="0">
         <v>38</v>
       </c>
       <c r="C39" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D39" s="0">
-        <v>0.80971659919028338</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E39" s="0">
-        <v>655.0607287449393</v>
+        <v>87.403598971722346</v>
       </c>
       <c r="F39" s="0">
-        <v>549.79757085020242</v>
+        <v>66.838046272493557</v>
       </c>
       <c r="G39" s="0">
-        <v>1.1914580265095729</v>
+        <v>1.3076923076923077</v>
       </c>
       <c r="H39" s="0">
-        <v>192069</v>
+        <v>144</v>
       </c>
       <c r="I39" s="0">
-        <v>400.42090176160946</v>
+        <v>69.617223676843963</v>
       </c>
       <c r="J39" s="0">
-        <v>125928.30565982067</v>
+        <v>3806.4776204228087</v>
       </c>
       <c r="K39" s="0">
-        <v>213.97986317527509</v>
+        <v>28.306246867294082</v>
       </c>
       <c r="L39" s="0">
-        <v>5262.3481781376513</v>
+        <v>267.200584756468</v>
       </c>
       <c r="M39" s="0">
-        <v>0.057144451082816038</v>
+        <v>0.66997459726396191</v>
       </c>
       <c r="N39" s="0">
-        <v>0.078056031183731472</v>
+        <v>0.60578229156427499</v>
       </c>
       <c r="O39" s="0">
-        <v>334.60025303406587</v>
+        <v>75.034722222222229</v>
       </c>
       <c r="P39" s="0">
-        <v>549.71435265451476</v>
+        <v>988.61805555555554</v>
       </c>
       <c r="Q39" s="0">
-        <v>18.67084543494737</v>
+        <v>21.033142857142856</v>
       </c>
       <c r="R39" s="0">
-        <v>18.67084543494737</v>
+        <v>21.033142857142856</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="B40" s="0">
         <v>39</v>
@@ -2673,51 +2753,51 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E40" s="0">
-        <v>296.35627530364371</v>
+        <v>655.0607287449393</v>
       </c>
       <c r="F40" s="0">
-        <v>225.91093117408906</v>
+        <v>549.79757085020242</v>
       </c>
       <c r="G40" s="0">
-        <v>1.3118279569892473</v>
+        <v>1.1914580265095729</v>
       </c>
       <c r="H40" s="0">
-        <v>49515</v>
+        <v>191409</v>
       </c>
       <c r="I40" s="0">
-        <v>203.30894812087394</v>
+        <v>399.73233354337987</v>
       </c>
       <c r="J40" s="0">
-        <v>32464.062679276823</v>
+        <v>125495.58261895785</v>
       </c>
       <c r="K40" s="0">
-        <v>82.37664240394102</v>
+        <v>214.00092471334267</v>
       </c>
       <c r="L40" s="0">
-        <v>1425.910931174089</v>
+        <v>5251.0121457489877</v>
       </c>
       <c r="M40" s="0">
-        <v>0.20064481230174325</v>
+        <v>0.057194235268599201</v>
       </c>
       <c r="N40" s="0">
-        <v>0.34676113050223306</v>
+        <v>0.07810940864456499</v>
       </c>
       <c r="O40" s="0">
-        <v>839.21890336261743</v>
+        <v>333.86112460751582</v>
       </c>
       <c r="P40" s="0">
-        <v>468.30015146925172</v>
+        <v>549.8282734876625</v>
       </c>
       <c r="Q40" s="0">
-        <v>27.443156284639421</v>
+        <v>31.371863466367437</v>
       </c>
       <c r="R40" s="0">
-        <v>27.443156284639421</v>
+        <v>31.371863466367437</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="B41" s="0">
         <v>40</v>
@@ -2729,51 +2809,51 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E41" s="0">
-        <v>9.7165991902834001</v>
+        <v>296.35627530364371</v>
       </c>
       <c r="F41" s="0">
-        <v>6.4777327935222671</v>
+        <v>225.91093117408906</v>
       </c>
       <c r="G41" s="0">
-        <v>1.5</v>
+        <v>1.3118279569892473</v>
       </c>
       <c r="H41" s="0">
-        <v>110</v>
+        <v>49544</v>
       </c>
       <c r="I41" s="0">
-        <v>9.5826239234059862</v>
+        <v>203.36847651085878</v>
       </c>
       <c r="J41" s="0">
-        <v>72.120506810470573</v>
+        <v>32483.076267435947</v>
       </c>
       <c r="K41" s="0">
-        <v>3.5330940923602463</v>
+        <v>82.312064044505661</v>
       </c>
       <c r="L41" s="0">
-        <v>31.247639500791408</v>
+        <v>1420.242914979757</v>
       </c>
       <c r="M41" s="0">
-        <v>0.92818426720588398</v>
+        <v>0.20236795963934881</v>
       </c>
       <c r="N41" s="0">
-        <v>0.18559147582963123</v>
+        <v>0.34607596182401446</v>
       </c>
       <c r="O41" s="0">
-        <v>317.92727272727274</v>
+        <v>839.28251655094459</v>
       </c>
       <c r="P41" s="0">
-        <v>616.25454545454545</v>
+        <v>468.26039480058131</v>
       </c>
       <c r="Q41" s="0">
-        <v>6.851449106449107</v>
+        <v>30.654738136599967</v>
       </c>
       <c r="R41" s="0">
-        <v>6.851449106449107</v>
+        <v>30.654738136599967</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="B42" s="0">
         <v>41</v>
@@ -2785,107 +2865,107 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E42" s="0">
-        <v>10.526315789473683</v>
+        <v>9.7165991902834001</v>
       </c>
       <c r="F42" s="0">
-        <v>8.9068825910931171</v>
+        <v>6.4777327935222671</v>
       </c>
       <c r="G42" s="0">
-        <v>1.1818181818181817</v>
+        <v>1.5</v>
       </c>
       <c r="H42" s="0">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I42" s="0">
-        <v>9.4510484721611245</v>
+        <v>9.5826239234059862</v>
       </c>
       <c r="J42" s="0">
-        <v>70.15358389745775</v>
+        <v>72.120506810470573</v>
       </c>
       <c r="K42" s="0">
-        <v>3.7963541089374435</v>
+        <v>3.5330940923602463</v>
       </c>
       <c r="L42" s="0">
-        <v>34.355278485492676</v>
+        <v>31.247639500791408</v>
       </c>
       <c r="M42" s="0">
-        <v>0.74691774936711841</v>
+        <v>0.92818426720588398</v>
       </c>
       <c r="N42" s="0">
-        <v>0.20959681048385345</v>
+        <v>0.18553348053730714</v>
       </c>
       <c r="O42" s="0">
-        <v>550.8878504672897</v>
+        <v>317.92727272727274</v>
       </c>
       <c r="P42" s="0">
-        <v>629.12149532710282</v>
+        <v>616.25454545454545</v>
       </c>
       <c r="Q42" s="0">
-        <v>3.3691803278688521</v>
+        <v>6.851449106449107</v>
       </c>
       <c r="R42" s="0">
-        <v>3.3691803278688521</v>
+        <v>6.851449106449107</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="B43" s="0">
         <v>42</v>
       </c>
       <c r="C43" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D43" s="0">
         <v>0.80971659919028338</v>
       </c>
       <c r="E43" s="0">
-        <v>654.25101214574897</v>
+        <v>10.526315789473683</v>
       </c>
       <c r="F43" s="0">
-        <v>543.31983805668017</v>
+        <v>8.9068825910931171</v>
       </c>
       <c r="G43" s="0">
-        <v>1.2041728763040238</v>
+        <v>1.1818181818181817</v>
       </c>
       <c r="H43" s="0">
-        <v>145161</v>
+        <v>107</v>
       </c>
       <c r="I43" s="0">
-        <v>348.10725721732007</v>
+        <v>9.4510484721611245</v>
       </c>
       <c r="J43" s="0">
-        <v>95173.498991952001</v>
+        <v>70.15358389745775</v>
       </c>
       <c r="K43" s="0">
-        <v>220.91077859704089</v>
+        <v>3.7963541089374435</v>
       </c>
       <c r="L43" s="0">
-        <v>3282.5910931174089</v>
+        <v>34.355278485492676</v>
       </c>
       <c r="M43" s="0">
-        <v>0.1109921659928771</v>
+        <v>0.74691774936711841</v>
       </c>
       <c r="N43" s="0">
-        <v>0.29440532818941728</v>
+        <v>0.20954052464858844</v>
       </c>
       <c r="O43" s="0">
-        <v>278.51236213583536</v>
+        <v>550.8878504672897</v>
       </c>
       <c r="P43" s="0">
-        <v>559.59487052307441</v>
+        <v>629.12149532710282</v>
       </c>
       <c r="Q43" s="0">
-        <v>7.9368686868686984</v>
+        <v>3.3691803278688521</v>
       </c>
       <c r="R43" s="0">
-        <v>7.9368686868686984</v>
+        <v>3.3691803278688521</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="B44" s="0">
         <v>43</v>
@@ -2897,331 +2977,331 @@
         <v>0.80971659919028338</v>
       </c>
       <c r="E44" s="0">
-        <v>297.9757085020243</v>
+        <v>654.25101214574897</v>
       </c>
       <c r="F44" s="0">
-        <v>229.14979757085021</v>
+        <v>544.12955465587038</v>
       </c>
       <c r="G44" s="0">
-        <v>1.3003533568904593</v>
+        <v>1.2023809523809526</v>
       </c>
       <c r="H44" s="0">
-        <v>53245</v>
+        <v>146192</v>
       </c>
       <c r="I44" s="0">
-        <v>210.82762548739817</v>
+        <v>349.34127864761558</v>
       </c>
       <c r="J44" s="0">
-        <v>34909.60350112278</v>
+        <v>95849.464833057413</v>
       </c>
       <c r="K44" s="0">
-        <v>81.88225902940566</v>
+        <v>220.79945696299345</v>
       </c>
       <c r="L44" s="0">
-        <v>1067.2064777327935</v>
+        <v>3298.7854251012145</v>
       </c>
       <c r="M44" s="0">
-        <v>0.385174808109009</v>
+        <v>0.1106856761145126</v>
       </c>
       <c r="N44" s="0">
-        <v>0.42393699746583402</v>
+        <v>0.29285231056097821</v>
       </c>
       <c r="O44" s="0">
-        <v>840.35060569067514</v>
+        <v>279.38119732953925</v>
       </c>
       <c r="P44" s="0">
-        <v>467.51995492534508</v>
+        <v>558.84220750793475</v>
       </c>
       <c r="Q44" s="0">
-        <v>34.458660632949524</v>
+        <v>31.05916119054941</v>
       </c>
       <c r="R44" s="0">
-        <v>34.458660632949524</v>
+        <v>31.05916119054941</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="B45" s="0">
         <v>44</v>
       </c>
       <c r="C45" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D45" s="0">
-        <v>1.7421602787456445</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E45" s="0">
-        <v>670.73170731707319</v>
+        <v>7.2874493927125501</v>
       </c>
       <c r="F45" s="0">
-        <v>555.7491289198606</v>
+        <v>6.4777327935222671</v>
       </c>
       <c r="G45" s="0">
-        <v>1.2068965517241381</v>
+        <v>1.125</v>
       </c>
       <c r="H45" s="0">
-        <v>37579</v>
+        <v>58</v>
       </c>
       <c r="I45" s="0">
-        <v>381.0796664852175</v>
+        <v>6.9582831692171023</v>
       </c>
       <c r="J45" s="0">
-        <v>114056.8660539766</v>
+        <v>38.027176318248124</v>
       </c>
       <c r="K45" s="0">
-        <v>225.0478601637725</v>
+        <v>2.9172708606907243</v>
       </c>
       <c r="L45" s="0">
-        <v>2653.3101045296166</v>
+        <v>25.101214574898783</v>
       </c>
       <c r="M45" s="0">
-        <v>0.20358945342653759</v>
+        <v>0.75842819524748395</v>
       </c>
       <c r="N45" s="0">
-        <v>0.34481529184477416</v>
+        <v>0.25303592598641944</v>
       </c>
       <c r="O45" s="0">
-        <v>463.32813539476837</v>
+        <v>967.60344827586209</v>
       </c>
       <c r="P45" s="0">
-        <v>614.99507703770723</v>
+        <v>315.98275862068965</v>
       </c>
       <c r="Q45" s="0">
-        <v>41.271183399933406</v>
+        <v>2.9754481927710845</v>
       </c>
       <c r="R45" s="0">
-        <v>41.271183399933406</v>
+        <v>2.9754481927710845</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="B46" s="0">
         <v>45</v>
       </c>
       <c r="C46" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D46" s="0">
-        <v>1.7421602787456445</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E46" s="0">
-        <v>297.90940766550523</v>
+        <v>299.59514170040484</v>
       </c>
       <c r="F46" s="0">
-        <v>238.67595818815329</v>
+        <v>229.95951417004048</v>
       </c>
       <c r="G46" s="0">
-        <v>1.248175182481752</v>
+        <v>1.3028169014084507</v>
       </c>
       <c r="H46" s="0">
-        <v>13411</v>
+        <v>53595</v>
       </c>
       <c r="I46" s="0">
-        <v>227.65319415053173</v>
+        <v>211.5194163018032</v>
       </c>
       <c r="J46" s="0">
-        <v>40704.02700044919</v>
+        <v>35139.077840974278</v>
       </c>
       <c r="K46" s="0">
-        <v>84.864612343631165</v>
+        <v>82.155777191995838</v>
       </c>
       <c r="L46" s="0">
-        <v>929.1036715137991</v>
+        <v>1072.8744939271255</v>
       </c>
       <c r="M46" s="0">
-        <v>0.59254165914542334</v>
+        <v>0.38362100851638581</v>
       </c>
       <c r="N46" s="0">
-        <v>0.43748629323283383</v>
+        <v>0.42211286476470528</v>
       </c>
       <c r="O46" s="0">
-        <v>728.28588472149727</v>
+        <v>840.39638025935255</v>
       </c>
       <c r="P46" s="0">
-        <v>570.30542092312282</v>
+        <v>467.28661255714155</v>
       </c>
       <c r="Q46" s="0">
-        <v>46.943796924862184</v>
+        <v>30.038983052356635</v>
       </c>
       <c r="R46" s="0">
-        <v>46.943796924862184</v>
+        <v>30.038983052356635</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="B47" s="0">
         <v>46</v>
       </c>
       <c r="C47" s="0">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D47" s="0">
-        <v>2.9761904761904758</v>
+        <v>0.80971659919028338</v>
       </c>
       <c r="E47" s="0">
-        <v>392.85714285714283</v>
+        <v>21.862348178137651</v>
       </c>
       <c r="F47" s="0">
-        <v>193.45238095238093</v>
+        <v>21.052631578947366</v>
       </c>
       <c r="G47" s="0">
-        <v>2.0307692307692307</v>
+        <v>1.0384615384615385</v>
       </c>
       <c r="H47" s="0">
-        <v>4823</v>
+        <v>366</v>
       </c>
       <c r="I47" s="0">
-        <v>233.22463006850967</v>
+        <v>17.479485466792831</v>
       </c>
       <c r="J47" s="0">
-        <v>42720.73412698412</v>
+        <v>239.96459538756574</v>
       </c>
       <c r="K47" s="0">
-        <v>112.81257441123842</v>
+        <v>8.1079777832848503</v>
       </c>
       <c r="L47" s="0">
-        <v>1181.9188243279252</v>
+        <v>73.223760084914616</v>
       </c>
       <c r="M47" s="0">
-        <v>0.38430255497135807</v>
+        <v>0.5624099317627792</v>
       </c>
       <c r="N47" s="0">
-        <v>0.2940384535503765</v>
+        <v>0.13223469333762858</v>
       </c>
       <c r="O47" s="0">
-        <v>501.99274310595064</v>
+        <v>500.22677595628414</v>
       </c>
       <c r="P47" s="0">
-        <v>160.17934895293385</v>
+        <v>384.10928961748635</v>
       </c>
       <c r="Q47" s="0">
-        <v>54.549081601927142</v>
+        <v>5.7366007905138359</v>
       </c>
       <c r="R47" s="0">
-        <v>54.549081601927142</v>
+        <v>5.7366007905138359</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="B48" s="0">
         <v>47</v>
       </c>
       <c r="C48" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D48" s="0">
-        <v>2.9761904761904758</v>
+        <v>1.7421602787456445</v>
       </c>
       <c r="E48" s="0">
-        <v>684.5238095238094</v>
+        <v>670.73170731707319</v>
       </c>
       <c r="F48" s="0">
-        <v>598.21428571428567</v>
+        <v>555.7491289198606</v>
       </c>
       <c r="G48" s="0">
-        <v>1.144278606965174</v>
+        <v>1.2068965517241381</v>
       </c>
       <c r="H48" s="0">
-        <v>17089</v>
+        <v>37556</v>
       </c>
       <c r="I48" s="0">
-        <v>439.00969055013411</v>
+        <v>380.9630298815905</v>
       </c>
       <c r="J48" s="0">
-        <v>151369.4019274376</v>
+        <v>113987.0582379293</v>
       </c>
       <c r="K48" s="0">
-        <v>198.45004257694367</v>
+        <v>224.97685681176046</v>
       </c>
       <c r="L48" s="0">
-        <v>2594.7804094117705</v>
+        <v>2644.5993031358885</v>
       </c>
       <c r="M48" s="0">
-        <v>0.28251840019482732</v>
+        <v>0.20480740329609595</v>
       </c>
       <c r="N48" s="0">
-        <v>0.34923220730026111</v>
+        <v>0.34493441511111622</v>
       </c>
       <c r="O48" s="0">
-        <v>596.41008836093397</v>
+        <v>463.26504420066033</v>
       </c>
       <c r="P48" s="0">
-        <v>291.65720639007549</v>
+        <v>615.06214719352431</v>
       </c>
       <c r="Q48" s="0">
-        <v>53.893411552346606</v>
+        <v>38.857706775982635</v>
       </c>
       <c r="R48" s="0">
-        <v>53.893411552346606</v>
+        <v>38.857706775982635</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="B49" s="0">
         <v>48</v>
       </c>
       <c r="C49" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D49" s="0">
-        <v>2.9761904761904758</v>
+        <v>1.7421602787456445</v>
       </c>
       <c r="E49" s="0">
-        <v>68.452380952380949</v>
+        <v>297.90940766550523</v>
       </c>
       <c r="F49" s="0">
-        <v>65.476190476190467</v>
+        <v>236.93379790940764</v>
       </c>
       <c r="G49" s="0">
-        <v>1.0454545454545456</v>
+        <v>1.2573529411764708</v>
       </c>
       <c r="H49" s="0">
-        <v>310</v>
+        <v>13413</v>
       </c>
       <c r="I49" s="0">
-        <v>59.128468290363145</v>
+        <v>227.67016862724705</v>
       </c>
       <c r="J49" s="0">
-        <v>2745.8900226757364</v>
+        <v>40710.097245322868</v>
       </c>
       <c r="K49" s="0">
-        <v>23.69240440529801</v>
+        <v>84.924607674566346</v>
       </c>
       <c r="L49" s="0">
-        <v>223.71829968530756</v>
+        <v>921.14078125992728</v>
       </c>
       <c r="M49" s="0">
-        <v>0.68942969166229773</v>
+        <v>0.60292040707308625</v>
       </c>
       <c r="N49" s="0">
-        <v>0.22096917280189901</v>
+        <v>0.43761732424953165</v>
       </c>
       <c r="O49" s="0">
-        <v>509.54838709677421</v>
+        <v>728.34466562290311</v>
       </c>
       <c r="P49" s="0">
-        <v>240.81612903225806</v>
+        <v>570.25930067844627</v>
       </c>
       <c r="Q49" s="0">
-        <v>18.32516129032259</v>
+        <v>48.258035186506277</v>
       </c>
       <c r="R49" s="0">
-        <v>18.32516129032259</v>
+        <v>48.258035186506277</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="B50" s="0">
         <v>49</v>
@@ -3233,51 +3313,51 @@
         <v>2.9761904761904758</v>
       </c>
       <c r="E50" s="0">
-        <v>675.59523809523796</v>
+        <v>392.85714285714283</v>
       </c>
       <c r="F50" s="0">
-        <v>547.61904761904759</v>
+        <v>193.45238095238093</v>
       </c>
       <c r="G50" s="0">
-        <v>1.2336956521739129</v>
+        <v>2.0307692307692307</v>
       </c>
       <c r="H50" s="0">
-        <v>12785</v>
+        <v>4812</v>
       </c>
       <c r="I50" s="0">
-        <v>379.72233965321198</v>
+        <v>232.95851609452035</v>
       </c>
       <c r="J50" s="0">
-        <v>113245.81916099771</v>
+        <v>42623.299319727885</v>
       </c>
       <c r="K50" s="0">
-        <v>223.68946868753591</v>
+        <v>112.87115250848693</v>
       </c>
       <c r="L50" s="0">
-        <v>2497.0238095238092</v>
+        <v>1179.689073594134</v>
       </c>
       <c r="M50" s="0">
-        <v>0.22823732820100839</v>
+        <v>0.38487687175592694</v>
       </c>
       <c r="N50" s="0">
-        <v>0.19563852339345231</v>
+        <v>0.29488655053634499</v>
       </c>
       <c r="O50" s="0">
-        <v>197.91615174032069</v>
+        <v>501.94243557772234</v>
       </c>
       <c r="P50" s="0">
-        <v>877.12139225655062</v>
+        <v>160.17373233582711</v>
       </c>
       <c r="Q50" s="0">
-        <v>48.470947562097535</v>
+        <v>52.969933333333344</v>
       </c>
       <c r="R50" s="0">
-        <v>48.470947562097535</v>
+        <v>52.969933333333344</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="B51" s="0">
         <v>50</v>
@@ -3289,219 +3369,219 @@
         <v>2.9761904761904758</v>
       </c>
       <c r="E51" s="0">
-        <v>297.61904761904759</v>
+        <v>684.5238095238094</v>
       </c>
       <c r="F51" s="0">
-        <v>232.14285714285711</v>
+        <v>598.21428571428567</v>
       </c>
       <c r="G51" s="0">
-        <v>1.2820512820512822</v>
+        <v>1.144278606965174</v>
       </c>
       <c r="H51" s="0">
-        <v>4635</v>
+        <v>17094</v>
       </c>
       <c r="I51" s="0">
-        <v>228.63391402089519</v>
+        <v>439.07390987005317</v>
       </c>
       <c r="J51" s="0">
-        <v>41055.484693877544</v>
+        <v>151413.69047619044</v>
       </c>
       <c r="K51" s="0">
-        <v>83.229709992887962</v>
+        <v>198.43180169410556</v>
       </c>
       <c r="L51" s="0">
-        <v>911.67841514443876</v>
+        <v>2587.1998846324955</v>
       </c>
       <c r="M51" s="0">
-        <v>0.62072280663394364</v>
+        <v>0.2842595357873115</v>
       </c>
       <c r="N51" s="0">
-        <v>0.26267497345821511</v>
+        <v>0.34895135965977536</v>
       </c>
       <c r="O51" s="0">
-        <v>355.0314994606257</v>
+        <v>596.38036738036737</v>
       </c>
       <c r="P51" s="0">
-        <v>847.85911542610575</v>
+        <v>291.67421317421315</v>
       </c>
       <c r="Q51" s="0">
-        <v>52.946815286624208</v>
+        <v>65.371947331947325</v>
       </c>
       <c r="R51" s="0">
-        <v>52.946815286624208</v>
+        <v>65.371947331947325</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="B52" s="0">
         <v>51</v>
       </c>
       <c r="C52" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D52" s="0">
-        <v>5.1413881748071972</v>
+        <v>2.9761904761904758</v>
       </c>
       <c r="E52" s="0">
-        <v>1871.4652956298198</v>
+        <v>68.452380952380949</v>
       </c>
       <c r="F52" s="0">
-        <v>1048.8431876606683</v>
+        <v>65.476190476190467</v>
       </c>
       <c r="G52" s="0">
-        <v>1.784313725490196</v>
+        <v>1.0454545454545456</v>
       </c>
       <c r="H52" s="0">
-        <v>26363</v>
+        <v>308</v>
       </c>
       <c r="I52" s="0">
-        <v>941.96088374734722</v>
+        <v>58.937422659156582</v>
       </c>
       <c r="J52" s="0">
-        <v>696876.17713337846</v>
+        <v>2728.1746031746029</v>
       </c>
       <c r="K52" s="0">
-        <v>505.22297357936441</v>
+        <v>23.738947079938956</v>
       </c>
       <c r="L52" s="0">
-        <v>7017.9948586118244</v>
+        <v>223.14036909585275</v>
       </c>
       <c r="M52" s="0">
-        <v>0.17780312549818236</v>
+        <v>0.68853454034121431</v>
       </c>
       <c r="N52" s="0">
-        <v>0.23317125491670873</v>
+        <v>0.22225501809605311</v>
       </c>
       <c r="O52" s="0">
-        <v>590.53347494594698</v>
+        <v>509.57142857142856</v>
       </c>
       <c r="P52" s="0">
-        <v>186.15756932063877</v>
+        <v>240.83766233766235</v>
       </c>
       <c r="Q52" s="0">
-        <v>45.02266666666678</v>
+        <v>19.268210526315798</v>
       </c>
       <c r="R52" s="0">
-        <v>45.02266666666678</v>
+        <v>19.268210526315798</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="B53" s="0">
         <v>52</v>
       </c>
       <c r="C53" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D53" s="0">
-        <v>5.1413881748071972</v>
+        <v>2.9761904761904758</v>
       </c>
       <c r="E53" s="0">
-        <v>503.85604113110531</v>
+        <v>675.59523809523796</v>
       </c>
       <c r="F53" s="0">
-        <v>395.88688946015418</v>
+        <v>547.61904761904759</v>
       </c>
       <c r="G53" s="0">
-        <v>1.2727272727272727</v>
+        <v>1.2336956521739129</v>
       </c>
       <c r="H53" s="0">
-        <v>4177</v>
+        <v>12799</v>
       </c>
       <c r="I53" s="0">
-        <v>374.94510770684064</v>
+        <v>379.9301870611655</v>
       </c>
       <c r="J53" s="0">
-        <v>110414.2848646255</v>
+        <v>113369.82709750565</v>
       </c>
       <c r="K53" s="0">
-        <v>147.40189220926868</v>
+        <v>223.65487763924347</v>
       </c>
       <c r="L53" s="0">
-        <v>1501.2853470437017</v>
+        <v>2499.9999999999995</v>
       </c>
       <c r="M53" s="0">
-        <v>0.61561421064198563</v>
+        <v>0.2279435622068921</v>
       </c>
       <c r="N53" s="0">
-        <v>0.2562505337488174</v>
+        <v>0.1951385661237636</v>
       </c>
       <c r="O53" s="0">
-        <v>491.09265022743597</v>
+        <v>197.85186342683022</v>
       </c>
       <c r="P53" s="0">
-        <v>270.70457265980366</v>
+        <v>877.16845066020778</v>
       </c>
       <c r="Q53" s="0">
-        <v>42.573202614379085</v>
+        <v>43.747886178861862</v>
       </c>
       <c r="R53" s="0">
-        <v>42.573202614379085</v>
+        <v>43.747886178861862</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="B54" s="0">
         <v>53</v>
       </c>
       <c r="C54" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D54" s="0">
-        <v>5.1413881748071972</v>
+        <v>2.9761904761904758</v>
       </c>
       <c r="E54" s="0">
-        <v>215.93830334190227</v>
+        <v>297.61904761904759</v>
       </c>
       <c r="F54" s="0">
-        <v>205.65552699228789</v>
+        <v>232.14285714285711</v>
       </c>
       <c r="G54" s="0">
-        <v>1.0499999999999998</v>
+        <v>1.2820512820512822</v>
       </c>
       <c r="H54" s="0">
-        <v>1264</v>
+        <v>4629</v>
       </c>
       <c r="I54" s="0">
-        <v>206.25713961117836</v>
+        <v>228.4858829830255</v>
       </c>
       <c r="J54" s="0">
-        <v>33412.414668155761</v>
+        <v>41002.338435374142</v>
       </c>
       <c r="K54" s="0">
-        <v>74.319259946128739</v>
+        <v>83.192653197054838</v>
       </c>
       <c r="L54" s="0">
-        <v>791.77377892030836</v>
+        <v>912.78822240543388</v>
       </c>
       <c r="M54" s="0">
-        <v>0.66975427797900122</v>
+        <v>0.6184127492142516</v>
       </c>
       <c r="N54" s="0">
-        <v>0.2861826415416957</v>
+        <v>0.26318543314891801</v>
       </c>
       <c r="O54" s="0">
-        <v>702.76265822784808</v>
+        <v>355.0358608770793</v>
       </c>
       <c r="P54" s="0">
-        <v>347.16218354430379</v>
+        <v>847.83776193562323</v>
       </c>
       <c r="Q54" s="0">
-        <v>31.585030674846632</v>
+        <v>52.955948553054682</v>
       </c>
       <c r="R54" s="0">
-        <v>31.585030674846632</v>
+        <v>52.955948553054682</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="B55" s="0">
         <v>54</v>
@@ -3513,51 +3593,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E55" s="0">
-        <v>169.6658097686375</v>
+        <v>1871.4652956298198</v>
       </c>
       <c r="F55" s="0">
-        <v>169.6658097686375</v>
+        <v>1048.8431876606683</v>
       </c>
       <c r="G55" s="0">
-        <v>1</v>
+        <v>1.784313725490196</v>
       </c>
       <c r="H55" s="0">
-        <v>793</v>
+        <v>26314</v>
       </c>
       <c r="I55" s="0">
-        <v>163.36990154312042</v>
+        <v>941.08508147827877</v>
       </c>
       <c r="J55" s="0">
-        <v>20962.060784689496</v>
+        <v>695580.91738754022</v>
       </c>
       <c r="K55" s="0">
-        <v>59.355532509816683</v>
+        <v>504.7964538577815</v>
       </c>
       <c r="L55" s="0">
-        <v>586.11825192802053</v>
+        <v>7033.4190231362454</v>
       </c>
       <c r="M55" s="0">
-        <v>0.76678454118088823</v>
+        <v>0.17669511363873036</v>
       </c>
       <c r="N55" s="0">
-        <v>0.27808454190577137</v>
+        <v>0.23375693196197667</v>
       </c>
       <c r="O55" s="0">
-        <v>740.79823455233293</v>
+        <v>590.40309341035186</v>
       </c>
       <c r="P55" s="0">
-        <v>410.58511979823453</v>
+        <v>186.10374705479973</v>
       </c>
       <c r="Q55" s="0">
-        <v>32.477377049180333</v>
+        <v>44.26050505050506</v>
       </c>
       <c r="R55" s="0">
-        <v>32.477377049180333</v>
+        <v>44.26050505050506</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="B56" s="0">
         <v>55</v>
@@ -3569,51 +3649,51 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E56" s="0">
-        <v>1280.2056555269921</v>
+        <v>503.85604113110531</v>
       </c>
       <c r="F56" s="0">
-        <v>791.77377892030836</v>
+        <v>395.88688946015418</v>
       </c>
       <c r="G56" s="0">
-        <v>1.616883116883117</v>
+        <v>1.2727272727272727</v>
       </c>
       <c r="H56" s="0">
-        <v>16357</v>
+        <v>4190</v>
       </c>
       <c r="I56" s="0">
-        <v>741.97159679904701</v>
+        <v>375.52812180219121</v>
       </c>
       <c r="J56" s="0">
-        <v>432378.85025872139</v>
+        <v>110757.92520535811</v>
       </c>
       <c r="K56" s="0">
-        <v>373.34943259033338</v>
+        <v>147.57475988412219</v>
       </c>
       <c r="L56" s="0">
-        <v>4812.339331619537</v>
+        <v>1496.1439588688943</v>
       </c>
       <c r="M56" s="0">
-        <v>0.23461826573694317</v>
+        <v>0.62178166146083469</v>
       </c>
       <c r="N56" s="0">
-        <v>0.32558002009820936</v>
+        <v>0.25511212641680031</v>
       </c>
       <c r="O56" s="0">
-        <v>782.87155346334907</v>
+        <v>491.09379474940334</v>
       </c>
       <c r="P56" s="0">
-        <v>512.71675735159261</v>
+        <v>270.67136038186158</v>
       </c>
       <c r="Q56" s="0">
-        <v>54.96145454527057</v>
+        <v>43.246302428256072</v>
       </c>
       <c r="R56" s="0">
-        <v>54.96145454527057</v>
+        <v>43.246302428256072</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="B57" s="0">
         <v>56</v>
@@ -3625,214 +3705,214 @@
         <v>5.1413881748071972</v>
       </c>
       <c r="E57" s="0">
-        <v>478.14910025706934</v>
+        <v>215.93830334190227</v>
       </c>
       <c r="F57" s="0">
-        <v>370.1799485861182</v>
+        <v>205.65552699228789</v>
       </c>
       <c r="G57" s="0">
-        <v>1.2916666666666667</v>
+        <v>1.0499999999999998</v>
       </c>
       <c r="H57" s="0">
-        <v>3462</v>
+        <v>1270</v>
       </c>
       <c r="I57" s="0">
-        <v>341.349275506786</v>
+        <v>206.74609440149393</v>
       </c>
       <c r="J57" s="0">
-        <v>91514.066124331686</v>
+        <v>33571.017902340049</v>
       </c>
       <c r="K57" s="0">
-        <v>139.03513006514936</v>
+        <v>74.416472404123198</v>
       </c>
       <c r="L57" s="0">
-        <v>2123.3933161953723</v>
+        <v>791.77377892030836</v>
       </c>
       <c r="M57" s="0">
-        <v>0.25505675161906005</v>
+        <v>0.67293349132383828</v>
       </c>
       <c r="N57" s="0">
-        <v>0.25011937640526977</v>
+        <v>0.28502432414709072</v>
       </c>
       <c r="O57" s="0">
-        <v>418.72848064702487</v>
+        <v>702.82755905511806</v>
       </c>
       <c r="P57" s="0">
-        <v>778.8021374927788</v>
+        <v>347.26220472440946</v>
       </c>
       <c r="Q57" s="0">
-        <v>21.963066954643633</v>
+        <v>31.502307692307699</v>
       </c>
       <c r="R57" s="0">
-        <v>21.963066954643633</v>
+        <v>31.502307692307699</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="B58" s="0">
         <v>57</v>
       </c>
       <c r="C58" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D58" s="0">
-        <v>1.7421602787456445</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E58" s="0">
-        <v>670.73170731707319</v>
+        <v>169.6658097686375</v>
       </c>
       <c r="F58" s="0">
-        <v>555.7491289198606</v>
+        <v>169.6658097686375</v>
       </c>
       <c r="G58" s="0">
-        <v>1.2068965517241381</v>
+        <v>1</v>
       </c>
       <c r="H58" s="0">
-        <v>37560</v>
+        <v>783</v>
       </c>
       <c r="I58" s="0">
-        <v>380.98331707333375</v>
+        <v>162.33655846439825</v>
       </c>
       <c r="J58" s="0">
-        <v>113999.19872767666</v>
+        <v>20697.722061049022</v>
       </c>
       <c r="K58" s="0">
-        <v>224.97703580832004</v>
+        <v>58.974013449188909</v>
       </c>
       <c r="L58" s="0">
-        <v>2641.1149825783968</v>
+        <v>591.25964010282769</v>
       </c>
       <c r="M58" s="0">
-        <v>0.2053700198216955</v>
+        <v>0.74400515622255059</v>
       </c>
       <c r="N58" s="0">
-        <v>0.34485288536994063</v>
+        <v>0.28125025344010418</v>
       </c>
       <c r="O58" s="0">
-        <v>463.21246006389777</v>
+        <v>740.86079182630908</v>
       </c>
       <c r="P58" s="0">
-        <v>615.07859424920127</v>
+        <v>410.56577266922096</v>
       </c>
       <c r="Q58" s="0">
-        <v>46.904745503252968</v>
+        <v>31.405894736842107</v>
       </c>
       <c r="R58" s="0">
-        <v>46.904745503252968</v>
+        <v>31.405894736842107</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="B59" s="0">
         <v>58</v>
       </c>
       <c r="C59" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D59" s="0">
-        <v>1.7421602787456445</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E59" s="0">
-        <v>297.90940766550523</v>
+        <v>1280.2056555269921</v>
       </c>
       <c r="F59" s="0">
-        <v>236.93379790940764</v>
+        <v>791.77377892030836</v>
       </c>
       <c r="G59" s="0">
-        <v>1.2573529411764708</v>
+        <v>1.616883116883117</v>
       </c>
       <c r="H59" s="0">
-        <v>13402</v>
+        <v>16366</v>
       </c>
       <c r="I59" s="0">
-        <v>227.57679333744125</v>
+        <v>742.17569370133435</v>
       </c>
       <c r="J59" s="0">
-        <v>40676.710898517638</v>
+        <v>432616.75510999782</v>
       </c>
       <c r="K59" s="0">
-        <v>84.892057185312552</v>
+        <v>373.50706275618631</v>
       </c>
       <c r="L59" s="0">
-        <v>917.57197570047936</v>
+        <v>4812.339331619537</v>
       </c>
       <c r="M59" s="0">
-        <v>0.60712121773239502</v>
+        <v>0.23474735813723857</v>
       </c>
       <c r="N59" s="0">
-        <v>0.43789877024499041</v>
+        <v>0.32540486481895792</v>
       </c>
       <c r="O59" s="0">
-        <v>728.34785852857783</v>
+        <v>782.92618843944763</v>
       </c>
       <c r="P59" s="0">
-        <v>570.28741978809137</v>
+        <v>512.78461444458026</v>
       </c>
       <c r="Q59" s="0">
-        <v>51.702093863787766</v>
+        <v>47.21701923076931</v>
       </c>
       <c r="R59" s="0">
-        <v>51.702093863787766</v>
+        <v>47.21701923076931</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>83</v>
+        <v>136</v>
       </c>
       <c r="B60" s="0">
         <v>59</v>
       </c>
       <c r="C60" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D60" s="0">
-        <v>2.9761904761904758</v>
+        <v>5.1413881748071972</v>
       </c>
       <c r="E60" s="0">
-        <v>392.85714285714283</v>
+        <v>478.14910025706934</v>
       </c>
       <c r="F60" s="0">
-        <v>190.47619047619045</v>
+        <v>370.1799485861182</v>
       </c>
       <c r="G60" s="0">
-        <v>2.0625</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="H60" s="0">
-        <v>4829</v>
+        <v>3476</v>
       </c>
       <c r="I60" s="0">
-        <v>233.36965524372366</v>
+        <v>342.03877121111441</v>
       </c>
       <c r="J60" s="0">
-        <v>42773.880385487522</v>
+        <v>91884.140337428355</v>
       </c>
       <c r="K60" s="0">
-        <v>112.97736326654638</v>
+        <v>139.086765347198</v>
       </c>
       <c r="L60" s="0">
-        <v>1184.8842340733129</v>
+        <v>2082.262210796915</v>
       </c>
       <c r="M60" s="0">
-        <v>0.38285707139669334</v>
+        <v>0.26630516235642421</v>
       </c>
       <c r="N60" s="0">
-        <v>0.29364116309204702</v>
+        <v>0.24865882882948509</v>
       </c>
       <c r="O60" s="0">
-        <v>501.90639884033959</v>
+        <v>418.82105868814728</v>
       </c>
       <c r="P60" s="0">
-        <v>160.15137709670739</v>
+        <v>778.91024165707711</v>
       </c>
       <c r="Q60" s="0">
-        <v>52.061514587212947</v>
+        <v>21.405594713656384</v>
       </c>
       <c r="R60" s="0">
-        <v>52.061514587212947</v>
+        <v>21.405594713656384</v>
       </c>
     </row>
     <row r="61">

</xml_diff>